<commit_message>
All files updated for May 2023
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2023/2023.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3970F0B3-44B2-41E7-86E2-46AAD371D189}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F831DE-5FA2-470C-AFD7-93BF068C8070}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="719" activeTab="3" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="719" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="73">
   <si>
     <t>branchname</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>2023-04-01 - 2023-04-30</t>
+  </si>
+  <si>
+    <t>2023-05-01 - 2023-05-30</t>
+  </si>
+  <si>
+    <t>Prairie Hills Schools - Wetmore Academic Center (Permanently closed)</t>
   </si>
 </sst>
 </file>
@@ -627,7 +633,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -15129,7 +15135,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -19520,6 +19526,4320 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="33" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45047</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45048</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45049</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45050</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45051</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45052</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45053</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45054</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45055</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45056</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45057</v>
+      </c>
+      <c r="M2" s="1">
+        <v>45058</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45059</v>
+      </c>
+      <c r="O2" s="1">
+        <v>45060</v>
+      </c>
+      <c r="P2" s="1">
+        <v>45061</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>45062</v>
+      </c>
+      <c r="R2" s="1">
+        <v>45063</v>
+      </c>
+      <c r="S2" s="1">
+        <v>45064</v>
+      </c>
+      <c r="T2" s="1">
+        <v>45065</v>
+      </c>
+      <c r="U2" s="1">
+        <v>45066</v>
+      </c>
+      <c r="V2" s="1">
+        <v>45067</v>
+      </c>
+      <c r="W2" s="1">
+        <v>45068</v>
+      </c>
+      <c r="X2" s="1">
+        <v>45069</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>45070</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>45071</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>45072</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>45073</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>45074</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>45075</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>45076</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>45077</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" t="s">
+        <v>65</v>
+      </c>
+      <c r="V3" t="s">
+        <v>59</v>
+      </c>
+      <c r="W3" t="s">
+        <v>60</v>
+      </c>
+      <c r="X3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>72</v>
+      </c>
+      <c r="C4">
+        <v>81</v>
+      </c>
+      <c r="D4">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>59</v>
+      </c>
+      <c r="F4">
+        <v>52</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>67</v>
+      </c>
+      <c r="J4">
+        <v>60</v>
+      </c>
+      <c r="K4">
+        <v>54</v>
+      </c>
+      <c r="L4">
+        <v>54</v>
+      </c>
+      <c r="M4">
+        <v>43</v>
+      </c>
+      <c r="N4">
+        <v>23</v>
+      </c>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>57</v>
+      </c>
+      <c r="Q4">
+        <v>62</v>
+      </c>
+      <c r="R4">
+        <v>55</v>
+      </c>
+      <c r="S4">
+        <v>64</v>
+      </c>
+      <c r="T4">
+        <v>45</v>
+      </c>
+      <c r="U4">
+        <v>32</v>
+      </c>
+      <c r="V4">
+        <v>6</v>
+      </c>
+      <c r="W4">
+        <v>76</v>
+      </c>
+      <c r="X4">
+        <v>79</v>
+      </c>
+      <c r="Y4">
+        <v>54</v>
+      </c>
+      <c r="Z4">
+        <v>62</v>
+      </c>
+      <c r="AA4">
+        <v>47</v>
+      </c>
+      <c r="AB4">
+        <v>35</v>
+      </c>
+      <c r="AC4">
+        <v>2</v>
+      </c>
+      <c r="AD4">
+        <v>5</v>
+      </c>
+      <c r="AE4">
+        <v>103</v>
+      </c>
+      <c r="AF4">
+        <v>59</v>
+      </c>
+      <c r="AG4">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>34</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>37</v>
+      </c>
+      <c r="J5">
+        <v>29</v>
+      </c>
+      <c r="K5">
+        <v>30</v>
+      </c>
+      <c r="L5">
+        <v>38</v>
+      </c>
+      <c r="M5">
+        <v>35</v>
+      </c>
+      <c r="N5">
+        <v>15</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>53</v>
+      </c>
+      <c r="Q5">
+        <v>39</v>
+      </c>
+      <c r="R5">
+        <v>35</v>
+      </c>
+      <c r="S5">
+        <v>40</v>
+      </c>
+      <c r="T5">
+        <v>42</v>
+      </c>
+      <c r="U5">
+        <v>19</v>
+      </c>
+      <c r="V5">
+        <v>4</v>
+      </c>
+      <c r="W5">
+        <v>46</v>
+      </c>
+      <c r="X5">
+        <v>46</v>
+      </c>
+      <c r="Y5">
+        <v>42</v>
+      </c>
+      <c r="Z5">
+        <v>41</v>
+      </c>
+      <c r="AA5">
+        <v>32</v>
+      </c>
+      <c r="AB5">
+        <v>26</v>
+      </c>
+      <c r="AC5">
+        <v>2</v>
+      </c>
+      <c r="AD5">
+        <v>2</v>
+      </c>
+      <c r="AE5">
+        <v>47</v>
+      </c>
+      <c r="AF5">
+        <v>58</v>
+      </c>
+      <c r="AG5">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+      <c r="C6">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>78</v>
+      </c>
+      <c r="E6">
+        <v>69</v>
+      </c>
+      <c r="F6">
+        <v>55</v>
+      </c>
+      <c r="G6">
+        <v>55</v>
+      </c>
+      <c r="H6">
+        <v>39</v>
+      </c>
+      <c r="I6">
+        <v>64</v>
+      </c>
+      <c r="J6">
+        <v>80</v>
+      </c>
+      <c r="K6">
+        <v>99</v>
+      </c>
+      <c r="L6">
+        <v>80</v>
+      </c>
+      <c r="M6">
+        <v>56</v>
+      </c>
+      <c r="N6">
+        <v>42</v>
+      </c>
+      <c r="O6">
+        <v>28</v>
+      </c>
+      <c r="P6">
+        <v>78</v>
+      </c>
+      <c r="Q6">
+        <v>89</v>
+      </c>
+      <c r="R6">
+        <v>70</v>
+      </c>
+      <c r="S6">
+        <v>84</v>
+      </c>
+      <c r="T6">
+        <v>68</v>
+      </c>
+      <c r="U6">
+        <v>66</v>
+      </c>
+      <c r="V6">
+        <v>26</v>
+      </c>
+      <c r="W6">
+        <v>90</v>
+      </c>
+      <c r="X6">
+        <v>80</v>
+      </c>
+      <c r="Y6">
+        <v>88</v>
+      </c>
+      <c r="Z6">
+        <v>81</v>
+      </c>
+      <c r="AA6">
+        <v>97</v>
+      </c>
+      <c r="AB6">
+        <v>54</v>
+      </c>
+      <c r="AC6">
+        <v>12</v>
+      </c>
+      <c r="AD6">
+        <v>10</v>
+      </c>
+      <c r="AE6">
+        <v>162</v>
+      </c>
+      <c r="AF6">
+        <v>139</v>
+      </c>
+      <c r="AG6">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AA7">
+        <v>2</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+      <c r="AF7">
+        <v>6</v>
+      </c>
+      <c r="AG7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>67</v>
+      </c>
+      <c r="D8">
+        <v>48</v>
+      </c>
+      <c r="E8">
+        <v>51</v>
+      </c>
+      <c r="F8">
+        <v>53</v>
+      </c>
+      <c r="G8">
+        <v>43</v>
+      </c>
+      <c r="H8">
+        <v>23</v>
+      </c>
+      <c r="I8">
+        <v>62</v>
+      </c>
+      <c r="J8">
+        <v>60</v>
+      </c>
+      <c r="K8">
+        <v>57</v>
+      </c>
+      <c r="L8">
+        <v>52</v>
+      </c>
+      <c r="M8">
+        <v>52</v>
+      </c>
+      <c r="N8">
+        <v>28</v>
+      </c>
+      <c r="O8">
+        <v>19</v>
+      </c>
+      <c r="P8">
+        <v>67</v>
+      </c>
+      <c r="Q8">
+        <v>66</v>
+      </c>
+      <c r="R8">
+        <v>61</v>
+      </c>
+      <c r="S8">
+        <v>44</v>
+      </c>
+      <c r="T8">
+        <v>55</v>
+      </c>
+      <c r="U8">
+        <v>41</v>
+      </c>
+      <c r="V8">
+        <v>24</v>
+      </c>
+      <c r="W8">
+        <v>56</v>
+      </c>
+      <c r="X8">
+        <v>56</v>
+      </c>
+      <c r="Y8">
+        <v>52</v>
+      </c>
+      <c r="Z8">
+        <v>46</v>
+      </c>
+      <c r="AA8">
+        <v>44</v>
+      </c>
+      <c r="AB8">
+        <v>42</v>
+      </c>
+      <c r="AC8">
+        <v>5</v>
+      </c>
+      <c r="AD8">
+        <v>11</v>
+      </c>
+      <c r="AE8">
+        <v>123</v>
+      </c>
+      <c r="AF8">
+        <v>88</v>
+      </c>
+      <c r="AG8">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>8</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>4</v>
+      </c>
+      <c r="R9">
+        <v>10</v>
+      </c>
+      <c r="S9">
+        <v>12</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+      <c r="V9">
+        <v>2</v>
+      </c>
+      <c r="W9">
+        <v>9</v>
+      </c>
+      <c r="X9">
+        <v>4</v>
+      </c>
+      <c r="Y9">
+        <v>9</v>
+      </c>
+      <c r="Z9">
+        <v>6</v>
+      </c>
+      <c r="AA9">
+        <v>6</v>
+      </c>
+      <c r="AB9">
+        <v>5</v>
+      </c>
+      <c r="AC9">
+        <v>1</v>
+      </c>
+      <c r="AE9">
+        <v>6</v>
+      </c>
+      <c r="AF9">
+        <v>8</v>
+      </c>
+      <c r="AG9">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>12</v>
+      </c>
+      <c r="J10">
+        <v>13</v>
+      </c>
+      <c r="K10">
+        <v>19</v>
+      </c>
+      <c r="L10">
+        <v>6</v>
+      </c>
+      <c r="M10">
+        <v>6</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>7</v>
+      </c>
+      <c r="Q10">
+        <v>11</v>
+      </c>
+      <c r="R10">
+        <v>8</v>
+      </c>
+      <c r="S10">
+        <v>13</v>
+      </c>
+      <c r="T10">
+        <v>9</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="W10">
+        <v>4</v>
+      </c>
+      <c r="X10">
+        <v>10</v>
+      </c>
+      <c r="Y10">
+        <v>9</v>
+      </c>
+      <c r="Z10">
+        <v>11</v>
+      </c>
+      <c r="AA10">
+        <v>17</v>
+      </c>
+      <c r="AD10">
+        <v>2</v>
+      </c>
+      <c r="AE10">
+        <v>10</v>
+      </c>
+      <c r="AF10">
+        <v>7</v>
+      </c>
+      <c r="AG10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <v>15</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>5</v>
+      </c>
+      <c r="R11">
+        <v>5</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>6</v>
+      </c>
+      <c r="U11">
+        <v>5</v>
+      </c>
+      <c r="W11">
+        <v>13</v>
+      </c>
+      <c r="Y11">
+        <v>6</v>
+      </c>
+      <c r="Z11">
+        <v>6</v>
+      </c>
+      <c r="AA11">
+        <v>11</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>9</v>
+      </c>
+      <c r="AG11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="AA12">
+        <v>2</v>
+      </c>
+      <c r="AG12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="Z14">
+        <v>1</v>
+      </c>
+      <c r="AE14">
+        <v>6</v>
+      </c>
+      <c r="AF14">
+        <v>1</v>
+      </c>
+      <c r="AG14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>8</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>8</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>7</v>
+      </c>
+      <c r="Q15">
+        <v>3</v>
+      </c>
+      <c r="R15">
+        <v>7</v>
+      </c>
+      <c r="S15">
+        <v>6</v>
+      </c>
+      <c r="T15">
+        <v>6</v>
+      </c>
+      <c r="U15">
+        <v>6</v>
+      </c>
+      <c r="W15">
+        <v>10</v>
+      </c>
+      <c r="X15">
+        <v>7</v>
+      </c>
+      <c r="Y15">
+        <v>8</v>
+      </c>
+      <c r="Z15">
+        <v>7</v>
+      </c>
+      <c r="AA15">
+        <v>8</v>
+      </c>
+      <c r="AE15">
+        <v>8</v>
+      </c>
+      <c r="AF15">
+        <v>8</v>
+      </c>
+      <c r="AG15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+      <c r="L16">
+        <v>10</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="P16">
+        <v>13</v>
+      </c>
+      <c r="Q16">
+        <v>15</v>
+      </c>
+      <c r="R16">
+        <v>4</v>
+      </c>
+      <c r="S16">
+        <v>6</v>
+      </c>
+      <c r="T16">
+        <v>8</v>
+      </c>
+      <c r="U16">
+        <v>4</v>
+      </c>
+      <c r="W16">
+        <v>7</v>
+      </c>
+      <c r="X16">
+        <v>10</v>
+      </c>
+      <c r="Y16">
+        <v>13</v>
+      </c>
+      <c r="Z16">
+        <v>9</v>
+      </c>
+      <c r="AA16">
+        <v>7</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AD16">
+        <v>2</v>
+      </c>
+      <c r="AE16">
+        <v>23</v>
+      </c>
+      <c r="AF16">
+        <v>12</v>
+      </c>
+      <c r="AG16">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>7</v>
+      </c>
+      <c r="Q17">
+        <v>7</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <v>4</v>
+      </c>
+      <c r="T17">
+        <v>4</v>
+      </c>
+      <c r="U17">
+        <v>2</v>
+      </c>
+      <c r="W17">
+        <v>11</v>
+      </c>
+      <c r="Y17">
+        <v>9</v>
+      </c>
+      <c r="Z17">
+        <v>5</v>
+      </c>
+      <c r="AA17">
+        <v>5</v>
+      </c>
+      <c r="AE17">
+        <v>4</v>
+      </c>
+      <c r="AF17">
+        <v>6</v>
+      </c>
+      <c r="AG17">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>4</v>
+      </c>
+      <c r="R18">
+        <v>6</v>
+      </c>
+      <c r="S18">
+        <v>10</v>
+      </c>
+      <c r="T18">
+        <v>13</v>
+      </c>
+      <c r="U18">
+        <v>7</v>
+      </c>
+      <c r="W18">
+        <v>10</v>
+      </c>
+      <c r="X18">
+        <v>6</v>
+      </c>
+      <c r="Y18">
+        <v>2</v>
+      </c>
+      <c r="Z18">
+        <v>3</v>
+      </c>
+      <c r="AA18">
+        <v>3</v>
+      </c>
+      <c r="AB18">
+        <v>5</v>
+      </c>
+      <c r="AE18">
+        <v>12</v>
+      </c>
+      <c r="AF18">
+        <v>18</v>
+      </c>
+      <c r="AG18">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>41</v>
+      </c>
+      <c r="C19">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>33</v>
+      </c>
+      <c r="E19">
+        <v>27</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>30</v>
+      </c>
+      <c r="J19">
+        <v>26</v>
+      </c>
+      <c r="K19">
+        <v>23</v>
+      </c>
+      <c r="L19">
+        <v>18</v>
+      </c>
+      <c r="M19">
+        <v>16</v>
+      </c>
+      <c r="N19">
+        <v>22</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>31</v>
+      </c>
+      <c r="Q19">
+        <v>21</v>
+      </c>
+      <c r="R19">
+        <v>25</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>9</v>
+      </c>
+      <c r="V19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>42</v>
+      </c>
+      <c r="X19">
+        <v>23</v>
+      </c>
+      <c r="Y19">
+        <v>40</v>
+      </c>
+      <c r="Z19">
+        <v>25</v>
+      </c>
+      <c r="AA19">
+        <v>34</v>
+      </c>
+      <c r="AB19">
+        <v>20</v>
+      </c>
+      <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
+        <v>3</v>
+      </c>
+      <c r="AE19">
+        <v>33</v>
+      </c>
+      <c r="AF19">
+        <v>37</v>
+      </c>
+      <c r="AG19">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="S20">
+        <v>3</v>
+      </c>
+      <c r="T20">
+        <v>3</v>
+      </c>
+      <c r="W20">
+        <v>3</v>
+      </c>
+      <c r="X20">
+        <v>2</v>
+      </c>
+      <c r="AA20">
+        <v>4</v>
+      </c>
+      <c r="AB20">
+        <v>2</v>
+      </c>
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20">
+        <v>3</v>
+      </c>
+      <c r="AG20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>25</v>
+      </c>
+      <c r="C21">
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>30</v>
+      </c>
+      <c r="E21">
+        <v>34</v>
+      </c>
+      <c r="F21">
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>31</v>
+      </c>
+      <c r="J21">
+        <v>26</v>
+      </c>
+      <c r="K21">
+        <v>30</v>
+      </c>
+      <c r="L21">
+        <v>30</v>
+      </c>
+      <c r="M21">
+        <v>23</v>
+      </c>
+      <c r="N21">
+        <v>12</v>
+      </c>
+      <c r="O21">
+        <v>7</v>
+      </c>
+      <c r="P21">
+        <v>26</v>
+      </c>
+      <c r="Q21">
+        <v>30</v>
+      </c>
+      <c r="R21">
+        <v>19</v>
+      </c>
+      <c r="S21">
+        <v>32</v>
+      </c>
+      <c r="T21">
+        <v>21</v>
+      </c>
+      <c r="U21">
+        <v>18</v>
+      </c>
+      <c r="V21">
+        <v>9</v>
+      </c>
+      <c r="W21">
+        <v>30</v>
+      </c>
+      <c r="X21">
+        <v>24</v>
+      </c>
+      <c r="Y21">
+        <v>41</v>
+      </c>
+      <c r="Z21">
+        <v>33</v>
+      </c>
+      <c r="AA21">
+        <v>33</v>
+      </c>
+      <c r="AB21">
+        <v>15</v>
+      </c>
+      <c r="AC21">
+        <v>6</v>
+      </c>
+      <c r="AD21">
+        <v>2</v>
+      </c>
+      <c r="AE21">
+        <v>38</v>
+      </c>
+      <c r="AF21">
+        <v>22</v>
+      </c>
+      <c r="AG21">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>34</v>
+      </c>
+      <c r="D23">
+        <v>30</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <v>27</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="I23">
+        <v>35</v>
+      </c>
+      <c r="J23">
+        <v>18</v>
+      </c>
+      <c r="K23">
+        <v>33</v>
+      </c>
+      <c r="L23">
+        <v>46</v>
+      </c>
+      <c r="M23">
+        <v>27</v>
+      </c>
+      <c r="N23">
+        <v>13</v>
+      </c>
+      <c r="P23">
+        <v>20</v>
+      </c>
+      <c r="Q23">
+        <v>29</v>
+      </c>
+      <c r="R23">
+        <v>38</v>
+      </c>
+      <c r="S23">
+        <v>45</v>
+      </c>
+      <c r="T23">
+        <v>36</v>
+      </c>
+      <c r="U23">
+        <v>8</v>
+      </c>
+      <c r="V23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>30</v>
+      </c>
+      <c r="X23">
+        <v>33</v>
+      </c>
+      <c r="Y23">
+        <v>38</v>
+      </c>
+      <c r="Z23">
+        <v>39</v>
+      </c>
+      <c r="AA23">
+        <v>31</v>
+      </c>
+      <c r="AE23">
+        <v>45</v>
+      </c>
+      <c r="AF23">
+        <v>45</v>
+      </c>
+      <c r="AG23">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>6</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>8</v>
+      </c>
+      <c r="R24">
+        <v>3</v>
+      </c>
+      <c r="S24">
+        <v>4</v>
+      </c>
+      <c r="X24">
+        <v>2</v>
+      </c>
+      <c r="Z24">
+        <v>2</v>
+      </c>
+      <c r="AA24">
+        <v>3</v>
+      </c>
+      <c r="AE24">
+        <v>2</v>
+      </c>
+      <c r="AF24">
+        <v>3</v>
+      </c>
+      <c r="AG24">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>29</v>
+      </c>
+      <c r="E25">
+        <v>33</v>
+      </c>
+      <c r="F25">
+        <v>33</v>
+      </c>
+      <c r="G25">
+        <v>13</v>
+      </c>
+      <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
+        <v>30</v>
+      </c>
+      <c r="J25">
+        <v>24</v>
+      </c>
+      <c r="K25">
+        <v>31</v>
+      </c>
+      <c r="L25">
+        <v>31</v>
+      </c>
+      <c r="M25">
+        <v>29</v>
+      </c>
+      <c r="N25">
+        <v>16</v>
+      </c>
+      <c r="O25">
+        <v>2</v>
+      </c>
+      <c r="P25">
+        <v>36</v>
+      </c>
+      <c r="Q25">
+        <v>34</v>
+      </c>
+      <c r="R25">
+        <v>29</v>
+      </c>
+      <c r="S25">
+        <v>25</v>
+      </c>
+      <c r="T25">
+        <v>24</v>
+      </c>
+      <c r="U25">
+        <v>17</v>
+      </c>
+      <c r="V25">
+        <v>2</v>
+      </c>
+      <c r="W25">
+        <v>24</v>
+      </c>
+      <c r="X25">
+        <v>22</v>
+      </c>
+      <c r="Y25">
+        <v>30</v>
+      </c>
+      <c r="Z25">
+        <v>45</v>
+      </c>
+      <c r="AA25">
+        <v>36</v>
+      </c>
+      <c r="AB25">
+        <v>27</v>
+      </c>
+      <c r="AC25">
+        <v>1</v>
+      </c>
+      <c r="AD25">
+        <v>3</v>
+      </c>
+      <c r="AE25">
+        <v>45</v>
+      </c>
+      <c r="AF25">
+        <v>39</v>
+      </c>
+      <c r="AG25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>97</v>
+      </c>
+      <c r="C26">
+        <v>108</v>
+      </c>
+      <c r="D26">
+        <v>85</v>
+      </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
+      <c r="F26">
+        <v>84</v>
+      </c>
+      <c r="G26">
+        <v>59</v>
+      </c>
+      <c r="H26">
+        <v>38</v>
+      </c>
+      <c r="I26">
+        <v>75</v>
+      </c>
+      <c r="J26">
+        <v>101</v>
+      </c>
+      <c r="K26">
+        <v>110</v>
+      </c>
+      <c r="L26">
+        <v>76</v>
+      </c>
+      <c r="M26">
+        <v>84</v>
+      </c>
+      <c r="N26">
+        <v>52</v>
+      </c>
+      <c r="O26">
+        <v>33</v>
+      </c>
+      <c r="P26">
+        <v>112</v>
+      </c>
+      <c r="Q26">
+        <v>89</v>
+      </c>
+      <c r="R26">
+        <v>99</v>
+      </c>
+      <c r="S26">
+        <v>88</v>
+      </c>
+      <c r="T26">
+        <v>105</v>
+      </c>
+      <c r="U26">
+        <v>75</v>
+      </c>
+      <c r="V26">
+        <v>35</v>
+      </c>
+      <c r="W26">
+        <v>91</v>
+      </c>
+      <c r="X26">
+        <v>110</v>
+      </c>
+      <c r="Y26">
+        <v>102</v>
+      </c>
+      <c r="Z26">
+        <v>108</v>
+      </c>
+      <c r="AA26">
+        <v>80</v>
+      </c>
+      <c r="AB26">
+        <v>69</v>
+      </c>
+      <c r="AC26">
+        <v>34</v>
+      </c>
+      <c r="AD26">
+        <v>16</v>
+      </c>
+      <c r="AE26">
+        <v>154</v>
+      </c>
+      <c r="AF26">
+        <v>120</v>
+      </c>
+      <c r="AG26">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
+      </c>
+      <c r="L27">
+        <v>7</v>
+      </c>
+      <c r="M27">
+        <v>10</v>
+      </c>
+      <c r="N27">
+        <v>7</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>3</v>
+      </c>
+      <c r="Q27">
+        <v>8</v>
+      </c>
+      <c r="R27">
+        <v>9</v>
+      </c>
+      <c r="S27">
+        <v>4</v>
+      </c>
+      <c r="T27">
+        <v>11</v>
+      </c>
+      <c r="U27">
+        <v>2</v>
+      </c>
+      <c r="W27">
+        <v>11</v>
+      </c>
+      <c r="X27">
+        <v>6</v>
+      </c>
+      <c r="Y27">
+        <v>7</v>
+      </c>
+      <c r="Z27">
+        <v>10</v>
+      </c>
+      <c r="AA27">
+        <v>12</v>
+      </c>
+      <c r="AB27">
+        <v>5</v>
+      </c>
+      <c r="AD27">
+        <v>1</v>
+      </c>
+      <c r="AE27">
+        <v>12</v>
+      </c>
+      <c r="AF27">
+        <v>16</v>
+      </c>
+      <c r="AG27">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="E29">
+        <v>6</v>
+      </c>
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="I29">
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <v>9</v>
+      </c>
+      <c r="K29">
+        <v>11</v>
+      </c>
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="N29">
+        <v>4</v>
+      </c>
+      <c r="P29">
+        <v>7</v>
+      </c>
+      <c r="Q29">
+        <v>9</v>
+      </c>
+      <c r="R29">
+        <v>5</v>
+      </c>
+      <c r="S29">
+        <v>15</v>
+      </c>
+      <c r="U29">
+        <v>6</v>
+      </c>
+      <c r="W29">
+        <v>10</v>
+      </c>
+      <c r="X29">
+        <v>14</v>
+      </c>
+      <c r="Y29">
+        <v>6</v>
+      </c>
+      <c r="Z29">
+        <v>8</v>
+      </c>
+      <c r="AB29">
+        <v>7</v>
+      </c>
+      <c r="AC29">
+        <v>2</v>
+      </c>
+      <c r="AD29">
+        <v>1</v>
+      </c>
+      <c r="AE29">
+        <v>13</v>
+      </c>
+      <c r="AF29">
+        <v>10</v>
+      </c>
+      <c r="AG29">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>7</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30">
+        <v>3</v>
+      </c>
+      <c r="R30">
+        <v>5</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <v>5</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="W30">
+        <v>5</v>
+      </c>
+      <c r="X30">
+        <v>1</v>
+      </c>
+      <c r="Y30">
+        <v>3</v>
+      </c>
+      <c r="Z30">
+        <v>2</v>
+      </c>
+      <c r="AA30">
+        <v>4</v>
+      </c>
+      <c r="AB30">
+        <v>4</v>
+      </c>
+      <c r="AE30">
+        <v>2</v>
+      </c>
+      <c r="AF30">
+        <v>8</v>
+      </c>
+      <c r="AG30">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>15</v>
+      </c>
+      <c r="E31">
+        <v>16</v>
+      </c>
+      <c r="F31">
+        <v>18</v>
+      </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>14</v>
+      </c>
+      <c r="J31">
+        <v>22</v>
+      </c>
+      <c r="K31">
+        <v>14</v>
+      </c>
+      <c r="L31">
+        <v>16</v>
+      </c>
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="N31">
+        <v>7</v>
+      </c>
+      <c r="P31">
+        <v>9</v>
+      </c>
+      <c r="Q31">
+        <v>15</v>
+      </c>
+      <c r="R31">
+        <v>21</v>
+      </c>
+      <c r="S31">
+        <v>18</v>
+      </c>
+      <c r="T31">
+        <v>11</v>
+      </c>
+      <c r="U31">
+        <v>9</v>
+      </c>
+      <c r="W31">
+        <v>18</v>
+      </c>
+      <c r="X31">
+        <v>54</v>
+      </c>
+      <c r="Y31">
+        <v>33</v>
+      </c>
+      <c r="Z31">
+        <v>26</v>
+      </c>
+      <c r="AA31">
+        <v>36</v>
+      </c>
+      <c r="AB31">
+        <v>8</v>
+      </c>
+      <c r="AE31">
+        <v>37</v>
+      </c>
+      <c r="AF31">
+        <v>46</v>
+      </c>
+      <c r="AG31">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>4</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="W32">
+        <v>2</v>
+      </c>
+      <c r="Z32">
+        <v>1</v>
+      </c>
+      <c r="AA32">
+        <v>3</v>
+      </c>
+      <c r="AE32">
+        <v>1</v>
+      </c>
+      <c r="AF32">
+        <v>2</v>
+      </c>
+      <c r="AG32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>6</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>6</v>
+      </c>
+      <c r="K33">
+        <v>6</v>
+      </c>
+      <c r="L33">
+        <v>4</v>
+      </c>
+      <c r="M33">
+        <v>5</v>
+      </c>
+      <c r="Q33">
+        <v>6</v>
+      </c>
+      <c r="R33">
+        <v>5</v>
+      </c>
+      <c r="S33">
+        <v>6</v>
+      </c>
+      <c r="T33">
+        <v>2</v>
+      </c>
+      <c r="U33">
+        <v>3</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33">
+        <v>10</v>
+      </c>
+      <c r="Y33">
+        <v>2</v>
+      </c>
+      <c r="Z33">
+        <v>5</v>
+      </c>
+      <c r="AA33">
+        <v>5</v>
+      </c>
+      <c r="AB33">
+        <v>4</v>
+      </c>
+      <c r="AD33">
+        <v>1</v>
+      </c>
+      <c r="AE33">
+        <v>5</v>
+      </c>
+      <c r="AF33">
+        <v>3</v>
+      </c>
+      <c r="AG33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <v>31</v>
+      </c>
+      <c r="D34">
+        <v>42</v>
+      </c>
+      <c r="E34">
+        <v>19</v>
+      </c>
+      <c r="F34">
+        <v>26</v>
+      </c>
+      <c r="G34">
+        <v>14</v>
+      </c>
+      <c r="I34">
+        <v>33</v>
+      </c>
+      <c r="J34">
+        <v>30</v>
+      </c>
+      <c r="K34">
+        <v>37</v>
+      </c>
+      <c r="L34">
+        <v>37</v>
+      </c>
+      <c r="M34">
+        <v>25</v>
+      </c>
+      <c r="N34">
+        <v>10</v>
+      </c>
+      <c r="P34">
+        <v>47</v>
+      </c>
+      <c r="Q34">
+        <v>49</v>
+      </c>
+      <c r="R34">
+        <v>48</v>
+      </c>
+      <c r="S34">
+        <v>41</v>
+      </c>
+      <c r="T34">
+        <v>58</v>
+      </c>
+      <c r="U34">
+        <v>17</v>
+      </c>
+      <c r="W34">
+        <v>51</v>
+      </c>
+      <c r="X34">
+        <v>62</v>
+      </c>
+      <c r="Y34">
+        <v>48</v>
+      </c>
+      <c r="Z34">
+        <v>30</v>
+      </c>
+      <c r="AA34">
+        <v>39</v>
+      </c>
+      <c r="AB34">
+        <v>14</v>
+      </c>
+      <c r="AE34">
+        <v>59</v>
+      </c>
+      <c r="AF34">
+        <v>46</v>
+      </c>
+      <c r="AG34">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <v>13</v>
+      </c>
+      <c r="F35">
+        <v>26</v>
+      </c>
+      <c r="G35">
+        <v>8</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>15</v>
+      </c>
+      <c r="J35">
+        <v>16</v>
+      </c>
+      <c r="K35">
+        <v>10</v>
+      </c>
+      <c r="L35">
+        <v>14</v>
+      </c>
+      <c r="M35">
+        <v>19</v>
+      </c>
+      <c r="N35">
+        <v>13</v>
+      </c>
+      <c r="P35">
+        <v>28</v>
+      </c>
+      <c r="Q35">
+        <v>23</v>
+      </c>
+      <c r="R35">
+        <v>19</v>
+      </c>
+      <c r="S35">
+        <v>16</v>
+      </c>
+      <c r="T35">
+        <v>18</v>
+      </c>
+      <c r="U35">
+        <v>7</v>
+      </c>
+      <c r="V35">
+        <v>2</v>
+      </c>
+      <c r="W35">
+        <v>32</v>
+      </c>
+      <c r="X35">
+        <v>21</v>
+      </c>
+      <c r="Y35">
+        <v>17</v>
+      </c>
+      <c r="Z35">
+        <v>23</v>
+      </c>
+      <c r="AA35">
+        <v>23</v>
+      </c>
+      <c r="AE35">
+        <v>38</v>
+      </c>
+      <c r="AF35">
+        <v>17</v>
+      </c>
+      <c r="AG35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>13</v>
+      </c>
+      <c r="E36">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>16</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="I36">
+        <v>21</v>
+      </c>
+      <c r="J36">
+        <v>12</v>
+      </c>
+      <c r="K36">
+        <v>13</v>
+      </c>
+      <c r="L36">
+        <v>19</v>
+      </c>
+      <c r="M36">
+        <v>9</v>
+      </c>
+      <c r="N36">
+        <v>5</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>20</v>
+      </c>
+      <c r="Q36">
+        <v>13</v>
+      </c>
+      <c r="R36">
+        <v>12</v>
+      </c>
+      <c r="S36">
+        <v>13</v>
+      </c>
+      <c r="T36">
+        <v>11</v>
+      </c>
+      <c r="U36">
+        <v>6</v>
+      </c>
+      <c r="W36">
+        <v>12</v>
+      </c>
+      <c r="X36">
+        <v>18</v>
+      </c>
+      <c r="Y36">
+        <v>23</v>
+      </c>
+      <c r="Z36">
+        <v>17</v>
+      </c>
+      <c r="AA36">
+        <v>13</v>
+      </c>
+      <c r="AB36">
+        <v>7</v>
+      </c>
+      <c r="AE36">
+        <v>12</v>
+      </c>
+      <c r="AF36">
+        <v>23</v>
+      </c>
+      <c r="AG36">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>74</v>
+      </c>
+      <c r="C37">
+        <v>71</v>
+      </c>
+      <c r="D37">
+        <v>68</v>
+      </c>
+      <c r="E37">
+        <v>73</v>
+      </c>
+      <c r="F37">
+        <v>61</v>
+      </c>
+      <c r="G37">
+        <v>26</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>63</v>
+      </c>
+      <c r="J37">
+        <v>55</v>
+      </c>
+      <c r="K37">
+        <v>74</v>
+      </c>
+      <c r="L37">
+        <v>59</v>
+      </c>
+      <c r="M37">
+        <v>82</v>
+      </c>
+      <c r="N37">
+        <v>35</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>75</v>
+      </c>
+      <c r="Q37">
+        <v>65</v>
+      </c>
+      <c r="R37">
+        <v>60</v>
+      </c>
+      <c r="S37">
+        <v>77</v>
+      </c>
+      <c r="T37">
+        <v>60</v>
+      </c>
+      <c r="U37">
+        <v>42</v>
+      </c>
+      <c r="V37">
+        <v>6</v>
+      </c>
+      <c r="W37">
+        <v>130</v>
+      </c>
+      <c r="X37">
+        <v>73</v>
+      </c>
+      <c r="Y37">
+        <v>91</v>
+      </c>
+      <c r="Z37">
+        <v>75</v>
+      </c>
+      <c r="AA37">
+        <v>64</v>
+      </c>
+      <c r="AB37">
+        <v>34</v>
+      </c>
+      <c r="AC37">
+        <v>2</v>
+      </c>
+      <c r="AD37">
+        <v>2</v>
+      </c>
+      <c r="AE37">
+        <v>123</v>
+      </c>
+      <c r="AF37">
+        <v>75</v>
+      </c>
+      <c r="AG37">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>20</v>
+      </c>
+      <c r="D38">
+        <v>15</v>
+      </c>
+      <c r="E38">
+        <v>20</v>
+      </c>
+      <c r="F38">
+        <v>17</v>
+      </c>
+      <c r="G38">
+        <v>7</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>12</v>
+      </c>
+      <c r="J38">
+        <v>9</v>
+      </c>
+      <c r="K38">
+        <v>7</v>
+      </c>
+      <c r="L38">
+        <v>18</v>
+      </c>
+      <c r="M38">
+        <v>16</v>
+      </c>
+      <c r="N38">
+        <v>2</v>
+      </c>
+      <c r="P38">
+        <v>24</v>
+      </c>
+      <c r="Q38">
+        <v>15</v>
+      </c>
+      <c r="R38">
+        <v>14</v>
+      </c>
+      <c r="S38">
+        <v>17</v>
+      </c>
+      <c r="T38">
+        <v>15</v>
+      </c>
+      <c r="U38">
+        <v>7</v>
+      </c>
+      <c r="V38">
+        <v>1</v>
+      </c>
+      <c r="W38">
+        <v>15</v>
+      </c>
+      <c r="X38">
+        <v>16</v>
+      </c>
+      <c r="Y38">
+        <v>17</v>
+      </c>
+      <c r="Z38">
+        <v>17</v>
+      </c>
+      <c r="AA38">
+        <v>21</v>
+      </c>
+      <c r="AD38">
+        <v>2</v>
+      </c>
+      <c r="AE38">
+        <v>15</v>
+      </c>
+      <c r="AF38">
+        <v>19</v>
+      </c>
+      <c r="AG38">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>51</v>
+      </c>
+      <c r="C39">
+        <v>66</v>
+      </c>
+      <c r="D39">
+        <v>55</v>
+      </c>
+      <c r="E39">
+        <v>38</v>
+      </c>
+      <c r="F39">
+        <v>35</v>
+      </c>
+      <c r="G39">
+        <v>33</v>
+      </c>
+      <c r="I39">
+        <v>56</v>
+      </c>
+      <c r="J39">
+        <v>44</v>
+      </c>
+      <c r="K39">
+        <v>43</v>
+      </c>
+      <c r="L39">
+        <v>52</v>
+      </c>
+      <c r="M39">
+        <v>37</v>
+      </c>
+      <c r="N39">
+        <v>39</v>
+      </c>
+      <c r="O39">
+        <v>6</v>
+      </c>
+      <c r="P39">
+        <v>62</v>
+      </c>
+      <c r="Q39">
+        <v>46</v>
+      </c>
+      <c r="R39">
+        <v>52</v>
+      </c>
+      <c r="S39">
+        <v>42</v>
+      </c>
+      <c r="T39">
+        <v>2</v>
+      </c>
+      <c r="U39">
+        <v>38</v>
+      </c>
+      <c r="V39">
+        <v>3</v>
+      </c>
+      <c r="W39">
+        <v>64</v>
+      </c>
+      <c r="X39">
+        <v>98</v>
+      </c>
+      <c r="Y39">
+        <v>44</v>
+      </c>
+      <c r="Z39">
+        <v>43</v>
+      </c>
+      <c r="AA39">
+        <v>54</v>
+      </c>
+      <c r="AB39">
+        <v>25</v>
+      </c>
+      <c r="AC39">
+        <v>1</v>
+      </c>
+      <c r="AD39">
+        <v>3</v>
+      </c>
+      <c r="AE39">
+        <v>97</v>
+      </c>
+      <c r="AF39">
+        <v>65</v>
+      </c>
+      <c r="AG39">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <v>2</v>
+      </c>
+      <c r="N40">
+        <v>2</v>
+      </c>
+      <c r="Q40">
+        <v>3</v>
+      </c>
+      <c r="S40">
+        <v>2</v>
+      </c>
+      <c r="U40">
+        <v>1</v>
+      </c>
+      <c r="X40">
+        <v>2</v>
+      </c>
+      <c r="Z40">
+        <v>3</v>
+      </c>
+      <c r="AG40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41">
+        <v>4</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>4</v>
+      </c>
+      <c r="P41">
+        <v>2</v>
+      </c>
+      <c r="Q41">
+        <v>6</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>2</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>1</v>
+      </c>
+      <c r="X41">
+        <v>3</v>
+      </c>
+      <c r="Y41">
+        <v>4</v>
+      </c>
+      <c r="Z41">
+        <v>1</v>
+      </c>
+      <c r="AA41">
+        <v>1</v>
+      </c>
+      <c r="AE41">
+        <v>1</v>
+      </c>
+      <c r="AF41">
+        <v>5</v>
+      </c>
+      <c r="AG41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>19</v>
+      </c>
+      <c r="E42">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>8</v>
+      </c>
+      <c r="I42">
+        <v>8</v>
+      </c>
+      <c r="J42">
+        <v>6</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="R42">
+        <v>2</v>
+      </c>
+      <c r="AG42">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>56</v>
+      </c>
+      <c r="C43">
+        <v>45</v>
+      </c>
+      <c r="D43">
+        <v>58</v>
+      </c>
+      <c r="E43">
+        <v>71</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="AG43">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="AG44">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="AG45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>9</v>
+      </c>
+      <c r="E47">
+        <v>11</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>4</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>9</v>
+      </c>
+      <c r="L47">
+        <v>10</v>
+      </c>
+      <c r="M47">
+        <v>9</v>
+      </c>
+      <c r="N47">
+        <v>5</v>
+      </c>
+      <c r="P47">
+        <v>12</v>
+      </c>
+      <c r="R47">
+        <v>14</v>
+      </c>
+      <c r="S47">
+        <v>11</v>
+      </c>
+      <c r="T47">
+        <v>8</v>
+      </c>
+      <c r="U47">
+        <v>2</v>
+      </c>
+      <c r="W47">
+        <v>12</v>
+      </c>
+      <c r="X47">
+        <v>1</v>
+      </c>
+      <c r="Y47">
+        <v>18</v>
+      </c>
+      <c r="Z47">
+        <v>13</v>
+      </c>
+      <c r="AA47">
+        <v>11</v>
+      </c>
+      <c r="AB47">
+        <v>3</v>
+      </c>
+      <c r="AF47">
+        <v>13</v>
+      </c>
+      <c r="AG47">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>19</v>
+      </c>
+      <c r="E48">
+        <v>21</v>
+      </c>
+      <c r="F48">
+        <v>13</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="I48">
+        <v>19</v>
+      </c>
+      <c r="J48">
+        <v>29</v>
+      </c>
+      <c r="K48">
+        <v>18</v>
+      </c>
+      <c r="L48">
+        <v>13</v>
+      </c>
+      <c r="M48">
+        <v>11</v>
+      </c>
+      <c r="N48">
+        <v>3</v>
+      </c>
+      <c r="P48">
+        <v>24</v>
+      </c>
+      <c r="Q48">
+        <v>21</v>
+      </c>
+      <c r="R48">
+        <v>52</v>
+      </c>
+      <c r="S48">
+        <v>18</v>
+      </c>
+      <c r="T48">
+        <v>20</v>
+      </c>
+      <c r="U48">
+        <v>6</v>
+      </c>
+      <c r="V48">
+        <v>1</v>
+      </c>
+      <c r="W48">
+        <v>26</v>
+      </c>
+      <c r="X48">
+        <v>14</v>
+      </c>
+      <c r="Y48">
+        <v>18</v>
+      </c>
+      <c r="Z48">
+        <v>21</v>
+      </c>
+      <c r="AA48">
+        <v>32</v>
+      </c>
+      <c r="AB48">
+        <v>2</v>
+      </c>
+      <c r="AC48">
+        <v>1</v>
+      </c>
+      <c r="AE48">
+        <v>39</v>
+      </c>
+      <c r="AF48">
+        <v>20</v>
+      </c>
+      <c r="AG48">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>25</v>
+      </c>
+      <c r="C49">
+        <v>33</v>
+      </c>
+      <c r="D49">
+        <v>25</v>
+      </c>
+      <c r="E49">
+        <v>27</v>
+      </c>
+      <c r="F49">
+        <v>19</v>
+      </c>
+      <c r="G49">
+        <v>19</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>31</v>
+      </c>
+      <c r="J49">
+        <v>31</v>
+      </c>
+      <c r="K49">
+        <v>24</v>
+      </c>
+      <c r="L49">
+        <v>22</v>
+      </c>
+      <c r="M49">
+        <v>24</v>
+      </c>
+      <c r="N49">
+        <v>15</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49">
+        <v>28</v>
+      </c>
+      <c r="Q49">
+        <v>37</v>
+      </c>
+      <c r="R49">
+        <v>26</v>
+      </c>
+      <c r="S49">
+        <v>31</v>
+      </c>
+      <c r="T49">
+        <v>34</v>
+      </c>
+      <c r="U49">
+        <v>19</v>
+      </c>
+      <c r="V49">
+        <v>1</v>
+      </c>
+      <c r="W49">
+        <v>40</v>
+      </c>
+      <c r="X49">
+        <v>53</v>
+      </c>
+      <c r="Y49">
+        <v>42</v>
+      </c>
+      <c r="Z49">
+        <v>40</v>
+      </c>
+      <c r="AA49">
+        <v>38</v>
+      </c>
+      <c r="AB49">
+        <v>18</v>
+      </c>
+      <c r="AD49">
+        <v>3</v>
+      </c>
+      <c r="AE49">
+        <v>47</v>
+      </c>
+      <c r="AF49">
+        <v>39</v>
+      </c>
+      <c r="AG49">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>21</v>
+      </c>
+      <c r="C50">
+        <v>24</v>
+      </c>
+      <c r="D50">
+        <v>22</v>
+      </c>
+      <c r="E50">
+        <v>18</v>
+      </c>
+      <c r="F50">
+        <v>24</v>
+      </c>
+      <c r="G50">
+        <v>12</v>
+      </c>
+      <c r="I50">
+        <v>31</v>
+      </c>
+      <c r="J50">
+        <v>24</v>
+      </c>
+      <c r="K50">
+        <v>22</v>
+      </c>
+      <c r="L50">
+        <v>20</v>
+      </c>
+      <c r="M50">
+        <v>28</v>
+      </c>
+      <c r="N50">
+        <v>5</v>
+      </c>
+      <c r="P50">
+        <v>23</v>
+      </c>
+      <c r="Q50">
+        <v>43</v>
+      </c>
+      <c r="R50">
+        <v>28</v>
+      </c>
+      <c r="S50">
+        <v>34</v>
+      </c>
+      <c r="T50">
+        <v>29</v>
+      </c>
+      <c r="U50">
+        <v>14</v>
+      </c>
+      <c r="W50">
+        <v>47</v>
+      </c>
+      <c r="X50">
+        <v>40</v>
+      </c>
+      <c r="Y50">
+        <v>38</v>
+      </c>
+      <c r="Z50">
+        <v>36</v>
+      </c>
+      <c r="AA50">
+        <v>31</v>
+      </c>
+      <c r="AB50">
+        <v>12</v>
+      </c>
+      <c r="AD50">
+        <v>1</v>
+      </c>
+      <c r="AE50">
+        <v>47</v>
+      </c>
+      <c r="AF50">
+        <v>42</v>
+      </c>
+      <c r="AG50">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>22</v>
+      </c>
+      <c r="C51">
+        <v>14</v>
+      </c>
+      <c r="D51">
+        <v>22</v>
+      </c>
+      <c r="E51">
+        <v>28</v>
+      </c>
+      <c r="F51">
+        <v>9</v>
+      </c>
+      <c r="G51">
+        <v>6</v>
+      </c>
+      <c r="I51">
+        <v>13</v>
+      </c>
+      <c r="J51">
+        <v>40</v>
+      </c>
+      <c r="K51">
+        <v>22</v>
+      </c>
+      <c r="L51">
+        <v>25</v>
+      </c>
+      <c r="M51">
+        <v>16</v>
+      </c>
+      <c r="N51">
+        <v>4</v>
+      </c>
+      <c r="O51">
+        <v>2</v>
+      </c>
+      <c r="P51">
+        <v>20</v>
+      </c>
+      <c r="Q51">
+        <v>30</v>
+      </c>
+      <c r="R51">
+        <v>23</v>
+      </c>
+      <c r="S51">
+        <v>21</v>
+      </c>
+      <c r="T51">
+        <v>14</v>
+      </c>
+      <c r="U51">
+        <v>1</v>
+      </c>
+      <c r="W51">
+        <v>25</v>
+      </c>
+      <c r="X51">
+        <v>18</v>
+      </c>
+      <c r="Y51">
+        <v>15</v>
+      </c>
+      <c r="Z51">
+        <v>28</v>
+      </c>
+      <c r="AA51">
+        <v>17</v>
+      </c>
+      <c r="AB51">
+        <v>6</v>
+      </c>
+      <c r="AD51">
+        <v>1</v>
+      </c>
+      <c r="AE51">
+        <v>27</v>
+      </c>
+      <c r="AF51">
+        <v>25</v>
+      </c>
+      <c r="AG51">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>60</v>
+      </c>
+      <c r="C52">
+        <v>55</v>
+      </c>
+      <c r="D52">
+        <v>45</v>
+      </c>
+      <c r="E52">
+        <v>51</v>
+      </c>
+      <c r="F52">
+        <v>34</v>
+      </c>
+      <c r="G52">
+        <v>27</v>
+      </c>
+      <c r="H52">
+        <v>17</v>
+      </c>
+      <c r="I52">
+        <v>39</v>
+      </c>
+      <c r="J52">
+        <v>39</v>
+      </c>
+      <c r="K52">
+        <v>52</v>
+      </c>
+      <c r="L52">
+        <v>51</v>
+      </c>
+      <c r="M52">
+        <v>39</v>
+      </c>
+      <c r="N52">
+        <v>19</v>
+      </c>
+      <c r="O52">
+        <v>10</v>
+      </c>
+      <c r="P52">
+        <v>57</v>
+      </c>
+      <c r="Q52">
+        <v>61</v>
+      </c>
+      <c r="R52">
+        <v>48</v>
+      </c>
+      <c r="S52">
+        <v>96</v>
+      </c>
+      <c r="T52">
+        <v>54</v>
+      </c>
+      <c r="U52">
+        <v>39</v>
+      </c>
+      <c r="V52">
+        <v>18</v>
+      </c>
+      <c r="W52">
+        <v>55</v>
+      </c>
+      <c r="X52">
+        <v>98</v>
+      </c>
+      <c r="Y52">
+        <v>74</v>
+      </c>
+      <c r="Z52">
+        <v>91</v>
+      </c>
+      <c r="AA52">
+        <v>51</v>
+      </c>
+      <c r="AB52">
+        <v>30</v>
+      </c>
+      <c r="AC52">
+        <v>13</v>
+      </c>
+      <c r="AD52">
+        <v>7</v>
+      </c>
+      <c r="AE52">
+        <v>82</v>
+      </c>
+      <c r="AF52">
+        <v>98</v>
+      </c>
+      <c r="AG52">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>9</v>
+      </c>
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53">
+        <v>7</v>
+      </c>
+      <c r="F53">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="I53">
+        <v>7</v>
+      </c>
+      <c r="J53">
+        <v>4</v>
+      </c>
+      <c r="K53">
+        <v>9</v>
+      </c>
+      <c r="L53">
+        <v>4</v>
+      </c>
+      <c r="M53">
+        <v>10</v>
+      </c>
+      <c r="N53">
+        <v>3</v>
+      </c>
+      <c r="P53">
+        <v>5</v>
+      </c>
+      <c r="Q53">
+        <v>8</v>
+      </c>
+      <c r="R53">
+        <v>5</v>
+      </c>
+      <c r="S53">
+        <v>7</v>
+      </c>
+      <c r="T53">
+        <v>13</v>
+      </c>
+      <c r="U53">
+        <v>8</v>
+      </c>
+      <c r="W53">
+        <v>9</v>
+      </c>
+      <c r="X53">
+        <v>11</v>
+      </c>
+      <c r="Y53">
+        <v>9</v>
+      </c>
+      <c r="Z53">
+        <v>3</v>
+      </c>
+      <c r="AA53">
+        <v>11</v>
+      </c>
+      <c r="AB53">
+        <v>3</v>
+      </c>
+      <c r="AD53">
+        <v>1</v>
+      </c>
+      <c r="AE53">
+        <v>7</v>
+      </c>
+      <c r="AF53">
+        <v>8</v>
+      </c>
+      <c r="AG53">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>23</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
+      </c>
+      <c r="E54">
+        <v>13</v>
+      </c>
+      <c r="F54">
+        <v>20</v>
+      </c>
+      <c r="G54">
+        <v>10</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>12</v>
+      </c>
+      <c r="J54">
+        <v>7</v>
+      </c>
+      <c r="K54">
+        <v>89</v>
+      </c>
+      <c r="L54">
+        <v>15</v>
+      </c>
+      <c r="M54">
+        <v>15</v>
+      </c>
+      <c r="N54">
+        <v>3</v>
+      </c>
+      <c r="P54">
+        <v>12</v>
+      </c>
+      <c r="Q54">
+        <v>23</v>
+      </c>
+      <c r="R54">
+        <v>27</v>
+      </c>
+      <c r="S54">
+        <v>11</v>
+      </c>
+      <c r="T54">
+        <v>18</v>
+      </c>
+      <c r="U54">
+        <v>5</v>
+      </c>
+      <c r="V54">
+        <v>1</v>
+      </c>
+      <c r="W54">
+        <v>30</v>
+      </c>
+      <c r="X54">
+        <v>22</v>
+      </c>
+      <c r="Y54">
+        <v>24</v>
+      </c>
+      <c r="Z54">
+        <v>14</v>
+      </c>
+      <c r="AA54">
+        <v>16</v>
+      </c>
+      <c r="AB54">
+        <v>11</v>
+      </c>
+      <c r="AD54">
+        <v>2</v>
+      </c>
+      <c r="AE54">
+        <v>27</v>
+      </c>
+      <c r="AF54">
+        <v>36</v>
+      </c>
+      <c r="AG54">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+      <c r="D55">
+        <v>6</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55">
+        <v>8</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="K55">
+        <v>7</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>4</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>4</v>
+      </c>
+      <c r="Q55">
+        <v>14</v>
+      </c>
+      <c r="R55">
+        <v>4</v>
+      </c>
+      <c r="S55">
+        <v>3</v>
+      </c>
+      <c r="T55">
+        <v>5</v>
+      </c>
+      <c r="U55">
+        <v>7</v>
+      </c>
+      <c r="W55">
+        <v>3</v>
+      </c>
+      <c r="X55">
+        <v>2</v>
+      </c>
+      <c r="Y55">
+        <v>7</v>
+      </c>
+      <c r="Z55">
+        <v>4</v>
+      </c>
+      <c r="AA55">
+        <v>5</v>
+      </c>
+      <c r="AE55">
+        <v>3</v>
+      </c>
+      <c r="AF55">
+        <v>14</v>
+      </c>
+      <c r="AG55">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+      <c r="D56">
+        <v>8</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <v>4</v>
+      </c>
+      <c r="K56">
+        <v>10</v>
+      </c>
+      <c r="L56">
+        <v>2</v>
+      </c>
+      <c r="N56">
+        <v>3</v>
+      </c>
+      <c r="P56">
+        <v>6</v>
+      </c>
+      <c r="Q56">
+        <v>1</v>
+      </c>
+      <c r="R56">
+        <v>4</v>
+      </c>
+      <c r="S56">
+        <v>2</v>
+      </c>
+      <c r="T56">
+        <v>6</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+      <c r="W56">
+        <v>4</v>
+      </c>
+      <c r="X56">
+        <v>4</v>
+      </c>
+      <c r="Y56">
+        <v>7</v>
+      </c>
+      <c r="AB56">
+        <v>1</v>
+      </c>
+      <c r="AD56">
+        <v>2</v>
+      </c>
+      <c r="AE56">
+        <v>7</v>
+      </c>
+      <c r="AF56">
+        <v>9</v>
+      </c>
+      <c r="AG56">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>8</v>
+      </c>
+      <c r="D57">
+        <v>6</v>
+      </c>
+      <c r="E57">
+        <v>8</v>
+      </c>
+      <c r="F57">
+        <v>5</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="I57">
+        <v>12</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+      <c r="K57">
+        <v>5</v>
+      </c>
+      <c r="L57">
+        <v>8</v>
+      </c>
+      <c r="M57">
+        <v>4</v>
+      </c>
+      <c r="N57">
+        <v>3</v>
+      </c>
+      <c r="P57">
+        <v>7</v>
+      </c>
+      <c r="Q57">
+        <v>6</v>
+      </c>
+      <c r="S57">
+        <v>5</v>
+      </c>
+      <c r="T57">
+        <v>6</v>
+      </c>
+      <c r="U57">
+        <v>1</v>
+      </c>
+      <c r="V57">
+        <v>1</v>
+      </c>
+      <c r="W57">
+        <v>7</v>
+      </c>
+      <c r="X57">
+        <v>2</v>
+      </c>
+      <c r="Y57">
+        <v>8</v>
+      </c>
+      <c r="Z57">
+        <v>7</v>
+      </c>
+      <c r="AA57">
+        <v>3</v>
+      </c>
+      <c r="AB57">
+        <v>4</v>
+      </c>
+      <c r="AE57">
+        <v>13</v>
+      </c>
+      <c r="AF57">
+        <v>14</v>
+      </c>
+      <c r="AG57">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A3:AG57" xr:uid="{CF4BD388-15BB-4ED1-B3EC-71F3785ED5DD}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7559C5-98A6-49B7-ABC7-2F44371F9A3D}">
+  <sheetPr codeName="Sheet12"/>
+  <dimension ref="A1:AG57"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
@@ -19944,18 +24264,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AG57" xr:uid="{CF4BD388-15BB-4ED1-B3EC-71F3785ED5DD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC7559C5-98A6-49B7-ABC7-2F44371F9A3D}">
-  <sheetPr codeName="Sheet12"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA1B21F-6FFE-4052-B555-7EB4F04AC5E9}">
+  <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="Q4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
@@ -20384,9 +24703,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA1B21F-6FFE-4052-B555-7EB4F04AC5E9}">
-  <sheetPr codeName="Sheet14"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236D8D1A-9F6E-4A67-B4B4-577BAEA41071}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -20816,12 +25135,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236D8D1A-9F6E-4A67-B4B4-577BAEA41071}">
-  <sheetPr codeName="Sheet16"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F138D5-7324-41CA-BDE7-6178B269EFE3}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -21250,442 +25570,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F138D5-7324-41CA-BDE7-6178B269EFE3}">
-  <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:AG57"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="33" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-      <c r="Z1">
-        <v>25</v>
-      </c>
-      <c r="AA1">
-        <v>26</v>
-      </c>
-      <c r="AB1">
-        <v>27</v>
-      </c>
-      <c r="AC1">
-        <v>28</v>
-      </c>
-      <c r="AD1">
-        <v>29</v>
-      </c>
-      <c r="AE1">
-        <v>30</v>
-      </c>
-      <c r="AF1">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
   <autoFilter ref="A3:AG57" xr:uid="{AFC2BCF1-614C-4B72-8DE9-95317B022DA5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add June 2023 files and update all annual files
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2023/2023.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F831DE-5FA2-470C-AFD7-93BF068C8070}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C34E34B-4756-4819-907F-9D007D0EED1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="719" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="74">
   <si>
     <t>branchname</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>Prairie Hills Schools - Wetmore Academic Center (Permanently closed)</t>
+  </si>
+  <si>
+    <t>2023-06-01 - 2023-06-30</t>
   </si>
 </sst>
 </file>
@@ -23956,6 +23959,4307 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="1">
+        <v>45078</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45079</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45080</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45081</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45082</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45083</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45084</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45085</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45086</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45087</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45088</v>
+      </c>
+      <c r="M2" s="1">
+        <v>45089</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45090</v>
+      </c>
+      <c r="O2" s="1">
+        <v>45091</v>
+      </c>
+      <c r="P2" s="1">
+        <v>45092</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>45093</v>
+      </c>
+      <c r="R2" s="1">
+        <v>45094</v>
+      </c>
+      <c r="S2" s="1">
+        <v>45095</v>
+      </c>
+      <c r="T2" s="1">
+        <v>45096</v>
+      </c>
+      <c r="U2" s="1">
+        <v>45097</v>
+      </c>
+      <c r="V2" s="1">
+        <v>45098</v>
+      </c>
+      <c r="W2" s="1">
+        <v>45099</v>
+      </c>
+      <c r="X2" s="1">
+        <v>45100</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>45101</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>45102</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>45103</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>45104</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>45105</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>45106</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>45107</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>70</v>
+      </c>
+      <c r="C4">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>94</v>
+      </c>
+      <c r="G4">
+        <v>80</v>
+      </c>
+      <c r="H4">
+        <v>70</v>
+      </c>
+      <c r="I4">
+        <v>70</v>
+      </c>
+      <c r="J4">
+        <v>43</v>
+      </c>
+      <c r="K4">
+        <v>40</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <v>84</v>
+      </c>
+      <c r="N4">
+        <v>65</v>
+      </c>
+      <c r="O4">
+        <v>72</v>
+      </c>
+      <c r="P4">
+        <v>88</v>
+      </c>
+      <c r="Q4">
+        <v>61</v>
+      </c>
+      <c r="R4">
+        <v>46</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>73</v>
+      </c>
+      <c r="U4">
+        <v>67</v>
+      </c>
+      <c r="V4">
+        <v>73</v>
+      </c>
+      <c r="W4">
+        <v>87</v>
+      </c>
+      <c r="X4">
+        <v>64</v>
+      </c>
+      <c r="Y4">
+        <v>50</v>
+      </c>
+      <c r="Z4">
+        <v>8</v>
+      </c>
+      <c r="AA4">
+        <v>75</v>
+      </c>
+      <c r="AB4">
+        <v>68</v>
+      </c>
+      <c r="AC4">
+        <v>89</v>
+      </c>
+      <c r="AD4">
+        <v>67</v>
+      </c>
+      <c r="AE4">
+        <v>63</v>
+      </c>
+      <c r="AG4">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>65</v>
+      </c>
+      <c r="H5">
+        <v>55</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>26</v>
+      </c>
+      <c r="K5">
+        <v>29</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>55</v>
+      </c>
+      <c r="N5">
+        <v>44</v>
+      </c>
+      <c r="O5">
+        <v>51</v>
+      </c>
+      <c r="P5">
+        <v>45</v>
+      </c>
+      <c r="Q5">
+        <v>26</v>
+      </c>
+      <c r="R5">
+        <v>23</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>6</v>
+      </c>
+      <c r="U5">
+        <v>69</v>
+      </c>
+      <c r="V5">
+        <v>58</v>
+      </c>
+      <c r="W5">
+        <v>31</v>
+      </c>
+      <c r="X5">
+        <v>36</v>
+      </c>
+      <c r="Y5">
+        <v>25</v>
+      </c>
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <v>46</v>
+      </c>
+      <c r="AB5">
+        <v>45</v>
+      </c>
+      <c r="AC5">
+        <v>50</v>
+      </c>
+      <c r="AD5">
+        <v>44</v>
+      </c>
+      <c r="AE5">
+        <v>45</v>
+      </c>
+      <c r="AG5">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>99</v>
+      </c>
+      <c r="C6">
+        <v>101</v>
+      </c>
+      <c r="D6">
+        <v>62</v>
+      </c>
+      <c r="E6">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <v>125</v>
+      </c>
+      <c r="G6">
+        <v>109</v>
+      </c>
+      <c r="H6">
+        <v>111</v>
+      </c>
+      <c r="I6">
+        <v>103</v>
+      </c>
+      <c r="J6">
+        <v>67</v>
+      </c>
+      <c r="K6">
+        <v>65</v>
+      </c>
+      <c r="L6">
+        <v>37</v>
+      </c>
+      <c r="M6">
+        <v>104</v>
+      </c>
+      <c r="N6">
+        <v>115</v>
+      </c>
+      <c r="O6">
+        <v>117</v>
+      </c>
+      <c r="P6">
+        <v>116</v>
+      </c>
+      <c r="Q6">
+        <v>89</v>
+      </c>
+      <c r="R6">
+        <v>62</v>
+      </c>
+      <c r="S6">
+        <v>44</v>
+      </c>
+      <c r="T6">
+        <v>18</v>
+      </c>
+      <c r="U6">
+        <v>137</v>
+      </c>
+      <c r="V6">
+        <v>127</v>
+      </c>
+      <c r="W6">
+        <v>118</v>
+      </c>
+      <c r="X6">
+        <v>81</v>
+      </c>
+      <c r="Y6">
+        <v>78</v>
+      </c>
+      <c r="Z6">
+        <v>46</v>
+      </c>
+      <c r="AA6">
+        <v>101</v>
+      </c>
+      <c r="AB6">
+        <v>116</v>
+      </c>
+      <c r="AC6">
+        <v>133</v>
+      </c>
+      <c r="AD6">
+        <v>100</v>
+      </c>
+      <c r="AE6">
+        <v>62</v>
+      </c>
+      <c r="AG6">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <v>5</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>4</v>
+      </c>
+      <c r="Y7">
+        <v>5</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>8</v>
+      </c>
+      <c r="AC7">
+        <v>4</v>
+      </c>
+      <c r="AD7">
+        <v>3</v>
+      </c>
+      <c r="AG7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>66</v>
+      </c>
+      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="D8">
+        <v>83</v>
+      </c>
+      <c r="E8">
+        <v>23</v>
+      </c>
+      <c r="F8">
+        <v>70</v>
+      </c>
+      <c r="G8">
+        <v>71</v>
+      </c>
+      <c r="H8">
+        <v>77</v>
+      </c>
+      <c r="I8">
+        <v>70</v>
+      </c>
+      <c r="J8">
+        <v>44</v>
+      </c>
+      <c r="K8">
+        <v>41</v>
+      </c>
+      <c r="L8">
+        <v>22</v>
+      </c>
+      <c r="M8">
+        <v>70</v>
+      </c>
+      <c r="N8">
+        <v>82</v>
+      </c>
+      <c r="O8">
+        <v>85</v>
+      </c>
+      <c r="P8">
+        <v>50</v>
+      </c>
+      <c r="Q8">
+        <v>62</v>
+      </c>
+      <c r="R8">
+        <v>43</v>
+      </c>
+      <c r="S8">
+        <v>20</v>
+      </c>
+      <c r="T8">
+        <v>3</v>
+      </c>
+      <c r="U8">
+        <v>98</v>
+      </c>
+      <c r="V8">
+        <v>81</v>
+      </c>
+      <c r="W8">
+        <v>66</v>
+      </c>
+      <c r="X8">
+        <v>66</v>
+      </c>
+      <c r="Y8">
+        <v>60</v>
+      </c>
+      <c r="Z8">
+        <v>38</v>
+      </c>
+      <c r="AA8">
+        <v>63</v>
+      </c>
+      <c r="AB8">
+        <v>97</v>
+      </c>
+      <c r="AC8">
+        <v>71</v>
+      </c>
+      <c r="AD8">
+        <v>71</v>
+      </c>
+      <c r="AE8">
+        <v>71</v>
+      </c>
+      <c r="AG8">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>9</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>21</v>
+      </c>
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <v>6</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>7</v>
+      </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>17</v>
+      </c>
+      <c r="W9">
+        <v>7</v>
+      </c>
+      <c r="X9">
+        <v>4</v>
+      </c>
+      <c r="Y9">
+        <v>5</v>
+      </c>
+      <c r="Z9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>10</v>
+      </c>
+      <c r="AB9">
+        <v>5</v>
+      </c>
+      <c r="AC9">
+        <v>12</v>
+      </c>
+      <c r="AD9">
+        <v>10</v>
+      </c>
+      <c r="AE9">
+        <v>8</v>
+      </c>
+      <c r="AG9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>32</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>18</v>
+      </c>
+      <c r="N10">
+        <v>12</v>
+      </c>
+      <c r="O10">
+        <v>24</v>
+      </c>
+      <c r="P10">
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <v>5</v>
+      </c>
+      <c r="R10">
+        <v>6</v>
+      </c>
+      <c r="T10">
+        <v>8</v>
+      </c>
+      <c r="U10">
+        <v>7</v>
+      </c>
+      <c r="V10">
+        <v>26</v>
+      </c>
+      <c r="W10">
+        <v>5</v>
+      </c>
+      <c r="X10">
+        <v>9</v>
+      </c>
+      <c r="Y10">
+        <v>9</v>
+      </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
+      <c r="AB10">
+        <v>9</v>
+      </c>
+      <c r="AC10">
+        <v>22</v>
+      </c>
+      <c r="AD10">
+        <v>10</v>
+      </c>
+      <c r="AE10">
+        <v>17</v>
+      </c>
+      <c r="AG10">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>23</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <v>7</v>
+      </c>
+      <c r="O11">
+        <v>18</v>
+      </c>
+      <c r="P11">
+        <v>3</v>
+      </c>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="T11">
+        <v>9</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>22</v>
+      </c>
+      <c r="W11">
+        <v>6</v>
+      </c>
+      <c r="X11">
+        <v>13</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>11</v>
+      </c>
+      <c r="AC11">
+        <v>24</v>
+      </c>
+      <c r="AD11">
+        <v>3</v>
+      </c>
+      <c r="AE11">
+        <v>7</v>
+      </c>
+      <c r="AG11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>9</v>
+      </c>
+      <c r="R12">
+        <v>11</v>
+      </c>
+      <c r="X12">
+        <v>11</v>
+      </c>
+      <c r="AC12">
+        <v>1</v>
+      </c>
+      <c r="AD12">
+        <v>10</v>
+      </c>
+      <c r="AG12">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>2</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>1</v>
+      </c>
+      <c r="AC14">
+        <v>5</v>
+      </c>
+      <c r="AD14">
+        <v>5</v>
+      </c>
+      <c r="AE14">
+        <v>6</v>
+      </c>
+      <c r="AG14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <v>7</v>
+      </c>
+      <c r="O15">
+        <v>11</v>
+      </c>
+      <c r="P15">
+        <v>5</v>
+      </c>
+      <c r="Q15">
+        <v>9</v>
+      </c>
+      <c r="R15">
+        <v>4</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>7</v>
+      </c>
+      <c r="U15">
+        <v>8</v>
+      </c>
+      <c r="V15">
+        <v>13</v>
+      </c>
+      <c r="W15">
+        <v>5</v>
+      </c>
+      <c r="X15">
+        <v>2</v>
+      </c>
+      <c r="Y15">
+        <v>6</v>
+      </c>
+      <c r="AA15">
+        <v>8</v>
+      </c>
+      <c r="AB15">
+        <v>2</v>
+      </c>
+      <c r="AC15">
+        <v>9</v>
+      </c>
+      <c r="AD15">
+        <v>4</v>
+      </c>
+      <c r="AE15">
+        <v>5</v>
+      </c>
+      <c r="AG15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>18</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <v>11</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="N16">
+        <v>16</v>
+      </c>
+      <c r="O16">
+        <v>19</v>
+      </c>
+      <c r="P16">
+        <v>12</v>
+      </c>
+      <c r="Q16">
+        <v>6</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
+      <c r="T16">
+        <v>12</v>
+      </c>
+      <c r="U16">
+        <v>14</v>
+      </c>
+      <c r="V16">
+        <v>13</v>
+      </c>
+      <c r="W16">
+        <v>21</v>
+      </c>
+      <c r="X16">
+        <v>6</v>
+      </c>
+      <c r="Y16">
+        <v>6</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>16</v>
+      </c>
+      <c r="AB16">
+        <v>21</v>
+      </c>
+      <c r="AC16">
+        <v>13</v>
+      </c>
+      <c r="AD16">
+        <v>16</v>
+      </c>
+      <c r="AE16">
+        <v>14</v>
+      </c>
+      <c r="AG16">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>9</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>3</v>
+      </c>
+      <c r="P17">
+        <v>7</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>2</v>
+      </c>
+      <c r="T17">
+        <v>9</v>
+      </c>
+      <c r="U17">
+        <v>6</v>
+      </c>
+      <c r="V17">
+        <v>2</v>
+      </c>
+      <c r="W17">
+        <v>4</v>
+      </c>
+      <c r="X17">
+        <v>3</v>
+      </c>
+      <c r="Y17">
+        <v>2</v>
+      </c>
+      <c r="AA17">
+        <v>8</v>
+      </c>
+      <c r="AB17">
+        <v>7</v>
+      </c>
+      <c r="AC17">
+        <v>7</v>
+      </c>
+      <c r="AD17">
+        <v>4</v>
+      </c>
+      <c r="AE17">
+        <v>6</v>
+      </c>
+      <c r="AG17">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>7</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>14</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>1</v>
+      </c>
+      <c r="V18">
+        <v>12</v>
+      </c>
+      <c r="W18">
+        <v>3</v>
+      </c>
+      <c r="X18">
+        <v>4</v>
+      </c>
+      <c r="Y18">
+        <v>2</v>
+      </c>
+      <c r="AA18">
+        <v>4</v>
+      </c>
+      <c r="AB18">
+        <v>6</v>
+      </c>
+      <c r="AC18">
+        <v>9</v>
+      </c>
+      <c r="AD18">
+        <v>3</v>
+      </c>
+      <c r="AE18">
+        <v>4</v>
+      </c>
+      <c r="AG18">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>44</v>
+      </c>
+      <c r="G19">
+        <v>41</v>
+      </c>
+      <c r="H19">
+        <v>48</v>
+      </c>
+      <c r="I19">
+        <v>32</v>
+      </c>
+      <c r="J19">
+        <v>35</v>
+      </c>
+      <c r="K19">
+        <v>25</v>
+      </c>
+      <c r="L19">
+        <v>4</v>
+      </c>
+      <c r="M19">
+        <v>28</v>
+      </c>
+      <c r="N19">
+        <v>23</v>
+      </c>
+      <c r="O19">
+        <v>35</v>
+      </c>
+      <c r="P19">
+        <v>21</v>
+      </c>
+      <c r="Q19">
+        <v>25</v>
+      </c>
+      <c r="R19">
+        <v>15</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+      <c r="U19">
+        <v>43</v>
+      </c>
+      <c r="V19">
+        <v>46</v>
+      </c>
+      <c r="W19">
+        <v>32</v>
+      </c>
+      <c r="X19">
+        <v>26</v>
+      </c>
+      <c r="Y19">
+        <v>27</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>33</v>
+      </c>
+      <c r="AB19">
+        <v>30</v>
+      </c>
+      <c r="AC19">
+        <v>33</v>
+      </c>
+      <c r="AD19">
+        <v>26</v>
+      </c>
+      <c r="AE19">
+        <v>30</v>
+      </c>
+      <c r="AG19">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>2</v>
+      </c>
+      <c r="X20">
+        <v>4</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="AA20">
+        <v>2</v>
+      </c>
+      <c r="AB20">
+        <v>5</v>
+      </c>
+      <c r="AE20">
+        <v>1</v>
+      </c>
+      <c r="AG20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>47</v>
+      </c>
+      <c r="C21">
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>46</v>
+      </c>
+      <c r="G21">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>38</v>
+      </c>
+      <c r="I21">
+        <v>49</v>
+      </c>
+      <c r="J21">
+        <v>26</v>
+      </c>
+      <c r="K21">
+        <v>11</v>
+      </c>
+      <c r="L21">
+        <v>7</v>
+      </c>
+      <c r="M21">
+        <v>42</v>
+      </c>
+      <c r="N21">
+        <v>34</v>
+      </c>
+      <c r="O21">
+        <v>32</v>
+      </c>
+      <c r="P21">
+        <v>42</v>
+      </c>
+      <c r="Q21">
+        <v>26</v>
+      </c>
+      <c r="R21">
+        <v>10</v>
+      </c>
+      <c r="S21">
+        <v>3</v>
+      </c>
+      <c r="T21">
+        <v>2</v>
+      </c>
+      <c r="U21">
+        <v>36</v>
+      </c>
+      <c r="V21">
+        <v>8</v>
+      </c>
+      <c r="W21">
+        <v>55</v>
+      </c>
+      <c r="X21">
+        <v>29</v>
+      </c>
+      <c r="Y21">
+        <v>12</v>
+      </c>
+      <c r="Z21">
+        <v>6</v>
+      </c>
+      <c r="AA21">
+        <v>39</v>
+      </c>
+      <c r="AB21">
+        <v>37</v>
+      </c>
+      <c r="AC21">
+        <v>37</v>
+      </c>
+      <c r="AD21">
+        <v>31</v>
+      </c>
+      <c r="AE21">
+        <v>26</v>
+      </c>
+      <c r="AG21">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="AB22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>42</v>
+      </c>
+      <c r="C23">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>43</v>
+      </c>
+      <c r="G23">
+        <v>55</v>
+      </c>
+      <c r="H23">
+        <v>34</v>
+      </c>
+      <c r="I23">
+        <v>38</v>
+      </c>
+      <c r="J23">
+        <v>25</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="M23">
+        <v>45</v>
+      </c>
+      <c r="N23">
+        <v>43</v>
+      </c>
+      <c r="O23">
+        <v>36</v>
+      </c>
+      <c r="P23">
+        <v>54</v>
+      </c>
+      <c r="Q23">
+        <v>31</v>
+      </c>
+      <c r="R23">
+        <v>12</v>
+      </c>
+      <c r="T23">
+        <v>36</v>
+      </c>
+      <c r="U23">
+        <v>47</v>
+      </c>
+      <c r="V23">
+        <v>21</v>
+      </c>
+      <c r="W23">
+        <v>47</v>
+      </c>
+      <c r="X23">
+        <v>39</v>
+      </c>
+      <c r="Y23">
+        <v>8</v>
+      </c>
+      <c r="AA23">
+        <v>39</v>
+      </c>
+      <c r="AB23">
+        <v>44</v>
+      </c>
+      <c r="AC23">
+        <v>31</v>
+      </c>
+      <c r="AD23">
+        <v>49</v>
+      </c>
+      <c r="AE23">
+        <v>35</v>
+      </c>
+      <c r="AG23">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>3</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>2</v>
+      </c>
+      <c r="U24">
+        <v>2</v>
+      </c>
+      <c r="V24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>2</v>
+      </c>
+      <c r="X24">
+        <v>1</v>
+      </c>
+      <c r="Y24">
+        <v>2</v>
+      </c>
+      <c r="AA24">
+        <v>3</v>
+      </c>
+      <c r="AB24">
+        <v>1</v>
+      </c>
+      <c r="AC24">
+        <v>4</v>
+      </c>
+      <c r="AD24">
+        <v>1</v>
+      </c>
+      <c r="AE24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>41</v>
+      </c>
+      <c r="D25">
+        <v>40</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>43</v>
+      </c>
+      <c r="G25">
+        <v>55</v>
+      </c>
+      <c r="H25">
+        <v>47</v>
+      </c>
+      <c r="I25">
+        <v>54</v>
+      </c>
+      <c r="J25">
+        <v>26</v>
+      </c>
+      <c r="K25">
+        <v>39</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="M25">
+        <v>50</v>
+      </c>
+      <c r="N25">
+        <v>32</v>
+      </c>
+      <c r="O25">
+        <v>43</v>
+      </c>
+      <c r="P25">
+        <v>29</v>
+      </c>
+      <c r="Q25">
+        <v>37</v>
+      </c>
+      <c r="R25">
+        <v>19</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>36</v>
+      </c>
+      <c r="U25">
+        <v>51</v>
+      </c>
+      <c r="V25">
+        <v>33</v>
+      </c>
+      <c r="W25">
+        <v>48</v>
+      </c>
+      <c r="X25">
+        <v>40</v>
+      </c>
+      <c r="Y25">
+        <v>38</v>
+      </c>
+      <c r="Z25">
+        <v>4</v>
+      </c>
+      <c r="AA25">
+        <v>57</v>
+      </c>
+      <c r="AB25">
+        <v>31</v>
+      </c>
+      <c r="AC25">
+        <v>36</v>
+      </c>
+      <c r="AD25">
+        <v>35</v>
+      </c>
+      <c r="AE25">
+        <v>30</v>
+      </c>
+      <c r="AG25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>127</v>
+      </c>
+      <c r="C26">
+        <v>87</v>
+      </c>
+      <c r="D26">
+        <v>83</v>
+      </c>
+      <c r="E26">
+        <v>33</v>
+      </c>
+      <c r="F26">
+        <v>104</v>
+      </c>
+      <c r="G26">
+        <v>112</v>
+      </c>
+      <c r="H26">
+        <v>131</v>
+      </c>
+      <c r="I26">
+        <v>88</v>
+      </c>
+      <c r="J26">
+        <v>77</v>
+      </c>
+      <c r="K26">
+        <v>77</v>
+      </c>
+      <c r="L26">
+        <v>36</v>
+      </c>
+      <c r="M26">
+        <v>121</v>
+      </c>
+      <c r="N26">
+        <v>115</v>
+      </c>
+      <c r="O26">
+        <v>109</v>
+      </c>
+      <c r="P26">
+        <v>107</v>
+      </c>
+      <c r="Q26">
+        <v>76</v>
+      </c>
+      <c r="R26">
+        <v>74</v>
+      </c>
+      <c r="S26">
+        <v>37</v>
+      </c>
+      <c r="T26">
+        <v>6</v>
+      </c>
+      <c r="U26">
+        <v>159</v>
+      </c>
+      <c r="V26">
+        <v>112</v>
+      </c>
+      <c r="W26">
+        <v>91</v>
+      </c>
+      <c r="X26">
+        <v>84</v>
+      </c>
+      <c r="Y26">
+        <v>59</v>
+      </c>
+      <c r="Z26">
+        <v>41</v>
+      </c>
+      <c r="AA26">
+        <v>97</v>
+      </c>
+      <c r="AB26">
+        <v>107</v>
+      </c>
+      <c r="AC26">
+        <v>112</v>
+      </c>
+      <c r="AD26">
+        <v>106</v>
+      </c>
+      <c r="AE26">
+        <v>87</v>
+      </c>
+      <c r="AG26">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+      <c r="G27">
+        <v>11</v>
+      </c>
+      <c r="H27">
+        <v>12</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+      <c r="J27">
+        <v>13</v>
+      </c>
+      <c r="K27">
+        <v>7</v>
+      </c>
+      <c r="M27">
+        <v>11</v>
+      </c>
+      <c r="N27">
+        <v>13</v>
+      </c>
+      <c r="O27">
+        <v>9</v>
+      </c>
+      <c r="P27">
+        <v>8</v>
+      </c>
+      <c r="Q27">
+        <v>16</v>
+      </c>
+      <c r="R27">
+        <v>5</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>5</v>
+      </c>
+      <c r="U27">
+        <v>17</v>
+      </c>
+      <c r="V27">
+        <v>9</v>
+      </c>
+      <c r="W27">
+        <v>9</v>
+      </c>
+      <c r="X27">
+        <v>12</v>
+      </c>
+      <c r="Y27">
+        <v>6</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>11</v>
+      </c>
+      <c r="AB27">
+        <v>19</v>
+      </c>
+      <c r="AC27">
+        <v>15</v>
+      </c>
+      <c r="AD27">
+        <v>4</v>
+      </c>
+      <c r="AE27">
+        <v>13</v>
+      </c>
+      <c r="AG27">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="F29">
+        <v>21</v>
+      </c>
+      <c r="G29">
+        <v>15</v>
+      </c>
+      <c r="H29">
+        <v>13</v>
+      </c>
+      <c r="I29">
+        <v>11</v>
+      </c>
+      <c r="K29">
+        <v>7</v>
+      </c>
+      <c r="M29">
+        <v>22</v>
+      </c>
+      <c r="N29">
+        <v>9</v>
+      </c>
+      <c r="O29">
+        <v>15</v>
+      </c>
+      <c r="P29">
+        <v>12</v>
+      </c>
+      <c r="R29">
+        <v>2</v>
+      </c>
+      <c r="T29">
+        <v>22</v>
+      </c>
+      <c r="U29">
+        <v>12</v>
+      </c>
+      <c r="V29">
+        <v>16</v>
+      </c>
+      <c r="W29">
+        <v>12</v>
+      </c>
+      <c r="X29">
+        <v>1</v>
+      </c>
+      <c r="Y29">
+        <v>5</v>
+      </c>
+      <c r="AA29">
+        <v>19</v>
+      </c>
+      <c r="AB29">
+        <v>16</v>
+      </c>
+      <c r="AC29">
+        <v>14</v>
+      </c>
+      <c r="AD29">
+        <v>13</v>
+      </c>
+      <c r="AG29">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>6</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="M30">
+        <v>5</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>7</v>
+      </c>
+      <c r="P30">
+        <v>4</v>
+      </c>
+      <c r="Q30">
+        <v>5</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <v>3</v>
+      </c>
+      <c r="V30">
+        <v>6</v>
+      </c>
+      <c r="X30">
+        <v>4</v>
+      </c>
+      <c r="Z30">
+        <v>1</v>
+      </c>
+      <c r="AA30">
+        <v>7</v>
+      </c>
+      <c r="AB30">
+        <v>3</v>
+      </c>
+      <c r="AC30">
+        <v>3</v>
+      </c>
+      <c r="AD30">
+        <v>3</v>
+      </c>
+      <c r="AE30">
+        <v>5</v>
+      </c>
+      <c r="AG30">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>23</v>
+      </c>
+      <c r="G31">
+        <v>35</v>
+      </c>
+      <c r="H31">
+        <v>20</v>
+      </c>
+      <c r="I31">
+        <v>27</v>
+      </c>
+      <c r="J31">
+        <v>26</v>
+      </c>
+      <c r="K31">
+        <v>11</v>
+      </c>
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31">
+        <v>26</v>
+      </c>
+      <c r="N31">
+        <v>37</v>
+      </c>
+      <c r="O31">
+        <v>23</v>
+      </c>
+      <c r="P31">
+        <v>30</v>
+      </c>
+      <c r="Q31">
+        <v>15</v>
+      </c>
+      <c r="R31">
+        <v>4</v>
+      </c>
+      <c r="T31">
+        <v>25</v>
+      </c>
+      <c r="U31">
+        <v>36</v>
+      </c>
+      <c r="V31">
+        <v>25</v>
+      </c>
+      <c r="W31">
+        <v>24</v>
+      </c>
+      <c r="X31">
+        <v>36</v>
+      </c>
+      <c r="Y31">
+        <v>7</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+      <c r="AA31">
+        <v>25</v>
+      </c>
+      <c r="AB31">
+        <v>32</v>
+      </c>
+      <c r="AC31">
+        <v>16</v>
+      </c>
+      <c r="AD31">
+        <v>28</v>
+      </c>
+      <c r="AE31">
+        <v>25</v>
+      </c>
+      <c r="AG31">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>3</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="U32">
+        <v>2</v>
+      </c>
+      <c r="V32">
+        <v>2</v>
+      </c>
+      <c r="W32">
+        <v>4</v>
+      </c>
+      <c r="X32">
+        <v>2</v>
+      </c>
+      <c r="AA32">
+        <v>1</v>
+      </c>
+      <c r="AB32">
+        <v>1</v>
+      </c>
+      <c r="AC32">
+        <v>1</v>
+      </c>
+      <c r="AE32">
+        <v>2</v>
+      </c>
+      <c r="AG32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>9</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+      <c r="J33">
+        <v>7</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>8</v>
+      </c>
+      <c r="O33">
+        <v>3</v>
+      </c>
+      <c r="P33">
+        <v>12</v>
+      </c>
+      <c r="Q33">
+        <v>8</v>
+      </c>
+      <c r="R33">
+        <v>2</v>
+      </c>
+      <c r="U33">
+        <v>7</v>
+      </c>
+      <c r="V33">
+        <v>8</v>
+      </c>
+      <c r="W33">
+        <v>5</v>
+      </c>
+      <c r="X33">
+        <v>9</v>
+      </c>
+      <c r="Y33">
+        <v>2</v>
+      </c>
+      <c r="AA33">
+        <v>1</v>
+      </c>
+      <c r="AB33">
+        <v>8</v>
+      </c>
+      <c r="AD33">
+        <v>10</v>
+      </c>
+      <c r="AE33">
+        <v>4</v>
+      </c>
+      <c r="AG33">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>26</v>
+      </c>
+      <c r="C34">
+        <v>28</v>
+      </c>
+      <c r="D34">
+        <v>19</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>60</v>
+      </c>
+      <c r="G34">
+        <v>55</v>
+      </c>
+      <c r="H34">
+        <v>47</v>
+      </c>
+      <c r="I34">
+        <v>35</v>
+      </c>
+      <c r="J34">
+        <v>40</v>
+      </c>
+      <c r="K34">
+        <v>17</v>
+      </c>
+      <c r="M34">
+        <v>48</v>
+      </c>
+      <c r="N34">
+        <v>61</v>
+      </c>
+      <c r="O34">
+        <v>46</v>
+      </c>
+      <c r="P34">
+        <v>37</v>
+      </c>
+      <c r="Q34">
+        <v>37</v>
+      </c>
+      <c r="R34">
+        <v>13</v>
+      </c>
+      <c r="T34">
+        <v>42</v>
+      </c>
+      <c r="U34">
+        <v>50</v>
+      </c>
+      <c r="V34">
+        <v>58</v>
+      </c>
+      <c r="W34">
+        <v>29</v>
+      </c>
+      <c r="X34">
+        <v>26</v>
+      </c>
+      <c r="Y34">
+        <v>17</v>
+      </c>
+      <c r="AA34">
+        <v>36</v>
+      </c>
+      <c r="AB34">
+        <v>29</v>
+      </c>
+      <c r="AC34">
+        <v>40</v>
+      </c>
+      <c r="AD34">
+        <v>32</v>
+      </c>
+      <c r="AE34">
+        <v>50</v>
+      </c>
+      <c r="AG34">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>26</v>
+      </c>
+      <c r="C35">
+        <v>33</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
+      </c>
+      <c r="F35">
+        <v>23</v>
+      </c>
+      <c r="G35">
+        <v>44</v>
+      </c>
+      <c r="H35">
+        <v>35</v>
+      </c>
+      <c r="I35">
+        <v>37</v>
+      </c>
+      <c r="J35">
+        <v>34</v>
+      </c>
+      <c r="K35">
+        <v>15</v>
+      </c>
+      <c r="M35">
+        <v>52</v>
+      </c>
+      <c r="N35">
+        <v>35</v>
+      </c>
+      <c r="O35">
+        <v>37</v>
+      </c>
+      <c r="P35">
+        <v>32</v>
+      </c>
+      <c r="Q35">
+        <v>16</v>
+      </c>
+      <c r="R35">
+        <v>13</v>
+      </c>
+      <c r="S35">
+        <v>2</v>
+      </c>
+      <c r="T35">
+        <v>2</v>
+      </c>
+      <c r="U35">
+        <v>43</v>
+      </c>
+      <c r="V35">
+        <v>32</v>
+      </c>
+      <c r="W35">
+        <v>43</v>
+      </c>
+      <c r="X35">
+        <v>35</v>
+      </c>
+      <c r="Y35">
+        <v>12</v>
+      </c>
+      <c r="AA35">
+        <v>39</v>
+      </c>
+      <c r="AB35">
+        <v>28</v>
+      </c>
+      <c r="AC35">
+        <v>28</v>
+      </c>
+      <c r="AD35">
+        <v>31</v>
+      </c>
+      <c r="AE35">
+        <v>40</v>
+      </c>
+      <c r="AG35">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>16</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>24</v>
+      </c>
+      <c r="G36">
+        <v>18</v>
+      </c>
+      <c r="H36">
+        <v>17</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+      <c r="J36">
+        <v>23</v>
+      </c>
+      <c r="K36">
+        <v>16</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36">
+        <v>10</v>
+      </c>
+      <c r="N36">
+        <v>15</v>
+      </c>
+      <c r="O36">
+        <v>12</v>
+      </c>
+      <c r="P36">
+        <v>20</v>
+      </c>
+      <c r="Q36">
+        <v>19</v>
+      </c>
+      <c r="R36">
+        <v>7</v>
+      </c>
+      <c r="T36">
+        <v>22</v>
+      </c>
+      <c r="U36">
+        <v>16</v>
+      </c>
+      <c r="V36">
+        <v>9</v>
+      </c>
+      <c r="W36">
+        <v>14</v>
+      </c>
+      <c r="X36">
+        <v>15</v>
+      </c>
+      <c r="Y36">
+        <v>6</v>
+      </c>
+      <c r="AA36">
+        <v>20</v>
+      </c>
+      <c r="AB36">
+        <v>14</v>
+      </c>
+      <c r="AC36">
+        <v>12</v>
+      </c>
+      <c r="AD36">
+        <v>9</v>
+      </c>
+      <c r="AE36">
+        <v>28</v>
+      </c>
+      <c r="AG36">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>106</v>
+      </c>
+      <c r="C37">
+        <v>97</v>
+      </c>
+      <c r="D37">
+        <v>43</v>
+      </c>
+      <c r="F37">
+        <v>103</v>
+      </c>
+      <c r="G37">
+        <v>110</v>
+      </c>
+      <c r="H37">
+        <v>102</v>
+      </c>
+      <c r="I37">
+        <v>94</v>
+      </c>
+      <c r="J37">
+        <v>72</v>
+      </c>
+      <c r="K37">
+        <v>43</v>
+      </c>
+      <c r="L37">
+        <v>5</v>
+      </c>
+      <c r="M37">
+        <v>154</v>
+      </c>
+      <c r="N37">
+        <v>95</v>
+      </c>
+      <c r="O37">
+        <v>83</v>
+      </c>
+      <c r="P37">
+        <v>94</v>
+      </c>
+      <c r="Q37">
+        <v>83</v>
+      </c>
+      <c r="R37">
+        <v>26</v>
+      </c>
+      <c r="S37">
+        <v>2</v>
+      </c>
+      <c r="T37">
+        <v>120</v>
+      </c>
+      <c r="U37">
+        <v>90</v>
+      </c>
+      <c r="V37">
+        <v>84</v>
+      </c>
+      <c r="W37">
+        <v>89</v>
+      </c>
+      <c r="X37">
+        <v>74</v>
+      </c>
+      <c r="Y37">
+        <v>34</v>
+      </c>
+      <c r="Z37">
+        <v>5</v>
+      </c>
+      <c r="AA37">
+        <v>114</v>
+      </c>
+      <c r="AB37">
+        <v>113</v>
+      </c>
+      <c r="AC37">
+        <v>97</v>
+      </c>
+      <c r="AD37">
+        <v>100</v>
+      </c>
+      <c r="AE37">
+        <v>81</v>
+      </c>
+      <c r="AG37">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>20</v>
+      </c>
+      <c r="C38">
+        <v>12</v>
+      </c>
+      <c r="D38">
+        <v>7</v>
+      </c>
+      <c r="F38">
+        <v>14</v>
+      </c>
+      <c r="G38">
+        <v>15</v>
+      </c>
+      <c r="H38">
+        <v>18</v>
+      </c>
+      <c r="I38">
+        <v>14</v>
+      </c>
+      <c r="J38">
+        <v>20</v>
+      </c>
+      <c r="K38">
+        <v>12</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>21</v>
+      </c>
+      <c r="N38">
+        <v>28</v>
+      </c>
+      <c r="O38">
+        <v>17</v>
+      </c>
+      <c r="P38">
+        <v>29</v>
+      </c>
+      <c r="Q38">
+        <v>8</v>
+      </c>
+      <c r="R38">
+        <v>5</v>
+      </c>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>12</v>
+      </c>
+      <c r="U38">
+        <v>21</v>
+      </c>
+      <c r="V38">
+        <v>25</v>
+      </c>
+      <c r="W38">
+        <v>21</v>
+      </c>
+      <c r="X38">
+        <v>17</v>
+      </c>
+      <c r="Y38">
+        <v>8</v>
+      </c>
+      <c r="AA38">
+        <v>11</v>
+      </c>
+      <c r="AB38">
+        <v>17</v>
+      </c>
+      <c r="AC38">
+        <v>18</v>
+      </c>
+      <c r="AD38">
+        <v>28</v>
+      </c>
+      <c r="AE38">
+        <v>18</v>
+      </c>
+      <c r="AG38">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>76</v>
+      </c>
+      <c r="C39">
+        <v>55</v>
+      </c>
+      <c r="D39">
+        <v>33</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>71</v>
+      </c>
+      <c r="G39">
+        <v>71</v>
+      </c>
+      <c r="H39">
+        <v>71</v>
+      </c>
+      <c r="I39">
+        <v>88</v>
+      </c>
+      <c r="J39">
+        <v>48</v>
+      </c>
+      <c r="K39">
+        <v>26</v>
+      </c>
+      <c r="L39">
+        <v>3</v>
+      </c>
+      <c r="M39">
+        <v>70</v>
+      </c>
+      <c r="N39">
+        <v>63</v>
+      </c>
+      <c r="O39">
+        <v>58</v>
+      </c>
+      <c r="P39">
+        <v>54</v>
+      </c>
+      <c r="Q39">
+        <v>11</v>
+      </c>
+      <c r="R39">
+        <v>32</v>
+      </c>
+      <c r="S39">
+        <v>2</v>
+      </c>
+      <c r="T39">
+        <v>7</v>
+      </c>
+      <c r="U39">
+        <v>112</v>
+      </c>
+      <c r="V39">
+        <v>60</v>
+      </c>
+      <c r="W39">
+        <v>54</v>
+      </c>
+      <c r="X39">
+        <v>48</v>
+      </c>
+      <c r="Y39">
+        <v>32</v>
+      </c>
+      <c r="Z39">
+        <v>2</v>
+      </c>
+      <c r="AA39">
+        <v>60</v>
+      </c>
+      <c r="AB39">
+        <v>82</v>
+      </c>
+      <c r="AC39">
+        <v>68</v>
+      </c>
+      <c r="AD39">
+        <v>69</v>
+      </c>
+      <c r="AE39">
+        <v>52</v>
+      </c>
+      <c r="AG39">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="I40">
+        <v>22</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="N40">
+        <v>4</v>
+      </c>
+      <c r="P40">
+        <v>18</v>
+      </c>
+      <c r="U40">
+        <v>5</v>
+      </c>
+      <c r="W40">
+        <v>14</v>
+      </c>
+      <c r="Y40">
+        <v>6</v>
+      </c>
+      <c r="Z40">
+        <v>1</v>
+      </c>
+      <c r="AB40">
+        <v>12</v>
+      </c>
+      <c r="AD40">
+        <v>14</v>
+      </c>
+      <c r="AG40">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>7</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>5</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+      <c r="N41">
+        <v>6</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>3</v>
+      </c>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>3</v>
+      </c>
+      <c r="V41">
+        <v>4</v>
+      </c>
+      <c r="W41">
+        <v>5</v>
+      </c>
+      <c r="X41">
+        <v>1</v>
+      </c>
+      <c r="Y41">
+        <v>2</v>
+      </c>
+      <c r="AB41">
+        <v>7</v>
+      </c>
+      <c r="AD41">
+        <v>2</v>
+      </c>
+      <c r="AE41">
+        <v>4</v>
+      </c>
+      <c r="AG41">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>18</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <v>11</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>15</v>
+      </c>
+      <c r="I47">
+        <v>15</v>
+      </c>
+      <c r="J47">
+        <v>13</v>
+      </c>
+      <c r="K47">
+        <v>10</v>
+      </c>
+      <c r="M47">
+        <v>13</v>
+      </c>
+      <c r="O47">
+        <v>9</v>
+      </c>
+      <c r="P47">
+        <v>13</v>
+      </c>
+      <c r="Q47">
+        <v>10</v>
+      </c>
+      <c r="R47">
+        <v>3</v>
+      </c>
+      <c r="T47">
+        <v>1</v>
+      </c>
+      <c r="U47">
+        <v>1</v>
+      </c>
+      <c r="V47">
+        <v>21</v>
+      </c>
+      <c r="W47">
+        <v>13</v>
+      </c>
+      <c r="X47">
+        <v>17</v>
+      </c>
+      <c r="Y47">
+        <v>10</v>
+      </c>
+      <c r="Z47">
+        <v>1</v>
+      </c>
+      <c r="AA47">
+        <v>12</v>
+      </c>
+      <c r="AC47">
+        <v>12</v>
+      </c>
+      <c r="AD47">
+        <v>8</v>
+      </c>
+      <c r="AE47">
+        <v>10</v>
+      </c>
+      <c r="AG47">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>28</v>
+      </c>
+      <c r="C48">
+        <v>28</v>
+      </c>
+      <c r="D48">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>19</v>
+      </c>
+      <c r="G48">
+        <v>40</v>
+      </c>
+      <c r="H48">
+        <v>16</v>
+      </c>
+      <c r="I48">
+        <v>26</v>
+      </c>
+      <c r="J48">
+        <v>27</v>
+      </c>
+      <c r="K48">
+        <v>5</v>
+      </c>
+      <c r="M48">
+        <v>20</v>
+      </c>
+      <c r="N48">
+        <v>33</v>
+      </c>
+      <c r="O48">
+        <v>17</v>
+      </c>
+      <c r="P48">
+        <v>18</v>
+      </c>
+      <c r="Q48">
+        <v>39</v>
+      </c>
+      <c r="R48">
+        <v>8</v>
+      </c>
+      <c r="T48">
+        <v>32</v>
+      </c>
+      <c r="U48">
+        <v>16</v>
+      </c>
+      <c r="V48">
+        <v>38</v>
+      </c>
+      <c r="W48">
+        <v>22</v>
+      </c>
+      <c r="X48">
+        <v>9</v>
+      </c>
+      <c r="Y48">
+        <v>7</v>
+      </c>
+      <c r="Z48">
+        <v>1</v>
+      </c>
+      <c r="AA48">
+        <v>28</v>
+      </c>
+      <c r="AB48">
+        <v>27</v>
+      </c>
+      <c r="AC48">
+        <v>19</v>
+      </c>
+      <c r="AD48">
+        <v>32</v>
+      </c>
+      <c r="AE48">
+        <v>23</v>
+      </c>
+      <c r="AG48">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>38</v>
+      </c>
+      <c r="C49">
+        <v>38</v>
+      </c>
+      <c r="D49">
+        <v>20</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>44</v>
+      </c>
+      <c r="G49">
+        <v>29</v>
+      </c>
+      <c r="H49">
+        <v>39</v>
+      </c>
+      <c r="I49">
+        <v>32</v>
+      </c>
+      <c r="J49">
+        <v>31</v>
+      </c>
+      <c r="K49">
+        <v>17</v>
+      </c>
+      <c r="M49">
+        <v>35</v>
+      </c>
+      <c r="N49">
+        <v>25</v>
+      </c>
+      <c r="O49">
+        <v>40</v>
+      </c>
+      <c r="P49">
+        <v>28</v>
+      </c>
+      <c r="Q49">
+        <v>28</v>
+      </c>
+      <c r="R49">
+        <v>10</v>
+      </c>
+      <c r="S49">
+        <v>2</v>
+      </c>
+      <c r="T49">
+        <v>45</v>
+      </c>
+      <c r="U49">
+        <v>36</v>
+      </c>
+      <c r="V49">
+        <v>43</v>
+      </c>
+      <c r="W49">
+        <v>21</v>
+      </c>
+      <c r="X49">
+        <v>26</v>
+      </c>
+      <c r="Y49">
+        <v>17</v>
+      </c>
+      <c r="Z49">
+        <v>5</v>
+      </c>
+      <c r="AA49">
+        <v>25</v>
+      </c>
+      <c r="AB49">
+        <v>42</v>
+      </c>
+      <c r="AC49">
+        <v>40</v>
+      </c>
+      <c r="AD49">
+        <v>34</v>
+      </c>
+      <c r="AE49">
+        <v>27</v>
+      </c>
+      <c r="AG49">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>21</v>
+      </c>
+      <c r="C50">
+        <v>29</v>
+      </c>
+      <c r="D50">
+        <v>18</v>
+      </c>
+      <c r="F50">
+        <v>53</v>
+      </c>
+      <c r="G50">
+        <v>36</v>
+      </c>
+      <c r="H50">
+        <v>49</v>
+      </c>
+      <c r="I50">
+        <v>31</v>
+      </c>
+      <c r="J50">
+        <v>20</v>
+      </c>
+      <c r="K50">
+        <v>9</v>
+      </c>
+      <c r="L50">
+        <v>2</v>
+      </c>
+      <c r="M50">
+        <v>41</v>
+      </c>
+      <c r="N50">
+        <v>39</v>
+      </c>
+      <c r="O50">
+        <v>41</v>
+      </c>
+      <c r="P50">
+        <v>25</v>
+      </c>
+      <c r="Q50">
+        <v>32</v>
+      </c>
+      <c r="R50">
+        <v>13</v>
+      </c>
+      <c r="S50">
+        <v>2</v>
+      </c>
+      <c r="T50">
+        <v>46</v>
+      </c>
+      <c r="U50">
+        <v>37</v>
+      </c>
+      <c r="V50">
+        <v>29</v>
+      </c>
+      <c r="W50">
+        <v>43</v>
+      </c>
+      <c r="X50">
+        <v>32</v>
+      </c>
+      <c r="Y50">
+        <v>12</v>
+      </c>
+      <c r="AA50">
+        <v>42</v>
+      </c>
+      <c r="AB50">
+        <v>43</v>
+      </c>
+      <c r="AC50">
+        <v>30</v>
+      </c>
+      <c r="AD50">
+        <v>34</v>
+      </c>
+      <c r="AE50">
+        <v>24</v>
+      </c>
+      <c r="AG50">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>39</v>
+      </c>
+      <c r="C51">
+        <v>19</v>
+      </c>
+      <c r="D51">
+        <v>10</v>
+      </c>
+      <c r="F51">
+        <v>15</v>
+      </c>
+      <c r="G51">
+        <v>35</v>
+      </c>
+      <c r="H51">
+        <v>18</v>
+      </c>
+      <c r="I51">
+        <v>27</v>
+      </c>
+      <c r="J51">
+        <v>11</v>
+      </c>
+      <c r="K51">
+        <v>7</v>
+      </c>
+      <c r="L51">
+        <v>3</v>
+      </c>
+      <c r="M51">
+        <v>25</v>
+      </c>
+      <c r="N51">
+        <v>31</v>
+      </c>
+      <c r="O51">
+        <v>18</v>
+      </c>
+      <c r="P51">
+        <v>35</v>
+      </c>
+      <c r="Q51">
+        <v>8</v>
+      </c>
+      <c r="R51">
+        <v>4</v>
+      </c>
+      <c r="T51">
+        <v>16</v>
+      </c>
+      <c r="U51">
+        <v>36</v>
+      </c>
+      <c r="V51">
+        <v>9</v>
+      </c>
+      <c r="W51">
+        <v>37</v>
+      </c>
+      <c r="X51">
+        <v>20</v>
+      </c>
+      <c r="Y51">
+        <v>7</v>
+      </c>
+      <c r="AA51">
+        <v>16</v>
+      </c>
+      <c r="AB51">
+        <v>39</v>
+      </c>
+      <c r="AC51">
+        <v>17</v>
+      </c>
+      <c r="AD51">
+        <v>18</v>
+      </c>
+      <c r="AE51">
+        <v>12</v>
+      </c>
+      <c r="AG51">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>78</v>
+      </c>
+      <c r="C52">
+        <v>65</v>
+      </c>
+      <c r="D52">
+        <v>34</v>
+      </c>
+      <c r="E52">
+        <v>15</v>
+      </c>
+      <c r="F52">
+        <v>72</v>
+      </c>
+      <c r="G52">
+        <v>84</v>
+      </c>
+      <c r="H52">
+        <v>75</v>
+      </c>
+      <c r="I52">
+        <v>72</v>
+      </c>
+      <c r="J52">
+        <v>54</v>
+      </c>
+      <c r="K52">
+        <v>27</v>
+      </c>
+      <c r="L52">
+        <v>20</v>
+      </c>
+      <c r="M52">
+        <v>74</v>
+      </c>
+      <c r="N52">
+        <v>61</v>
+      </c>
+      <c r="O52">
+        <v>68</v>
+      </c>
+      <c r="P52">
+        <v>77</v>
+      </c>
+      <c r="Q52">
+        <v>45</v>
+      </c>
+      <c r="R52">
+        <v>23</v>
+      </c>
+      <c r="S52">
+        <v>15</v>
+      </c>
+      <c r="T52">
+        <v>54</v>
+      </c>
+      <c r="U52">
+        <v>74</v>
+      </c>
+      <c r="V52">
+        <v>62</v>
+      </c>
+      <c r="W52">
+        <v>73</v>
+      </c>
+      <c r="X52">
+        <v>48</v>
+      </c>
+      <c r="Y52">
+        <v>36</v>
+      </c>
+      <c r="Z52">
+        <v>22</v>
+      </c>
+      <c r="AA52">
+        <v>80</v>
+      </c>
+      <c r="AB52">
+        <v>60</v>
+      </c>
+      <c r="AC52">
+        <v>68</v>
+      </c>
+      <c r="AD52">
+        <v>66</v>
+      </c>
+      <c r="AE52">
+        <v>52</v>
+      </c>
+      <c r="AG52">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>12</v>
+      </c>
+      <c r="D53">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>10</v>
+      </c>
+      <c r="G53">
+        <v>7</v>
+      </c>
+      <c r="H53">
+        <v>9</v>
+      </c>
+      <c r="I53">
+        <v>5</v>
+      </c>
+      <c r="J53">
+        <v>14</v>
+      </c>
+      <c r="K53">
+        <v>6</v>
+      </c>
+      <c r="M53">
+        <v>8</v>
+      </c>
+      <c r="N53">
+        <v>7</v>
+      </c>
+      <c r="O53">
+        <v>11</v>
+      </c>
+      <c r="P53">
+        <v>7</v>
+      </c>
+      <c r="Q53">
+        <v>15</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+      <c r="T53">
+        <v>6</v>
+      </c>
+      <c r="U53">
+        <v>5</v>
+      </c>
+      <c r="V53">
+        <v>11</v>
+      </c>
+      <c r="W53">
+        <v>6</v>
+      </c>
+      <c r="X53">
+        <v>11</v>
+      </c>
+      <c r="Y53">
+        <v>2</v>
+      </c>
+      <c r="AA53">
+        <v>4</v>
+      </c>
+      <c r="AB53">
+        <v>8</v>
+      </c>
+      <c r="AC53">
+        <v>8</v>
+      </c>
+      <c r="AD53">
+        <v>2</v>
+      </c>
+      <c r="AE53">
+        <v>11</v>
+      </c>
+      <c r="AG53">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>25</v>
+      </c>
+      <c r="C54">
+        <v>17</v>
+      </c>
+      <c r="D54">
+        <v>16</v>
+      </c>
+      <c r="F54">
+        <v>24</v>
+      </c>
+      <c r="G54">
+        <v>25</v>
+      </c>
+      <c r="H54">
+        <v>41</v>
+      </c>
+      <c r="I54">
+        <v>19</v>
+      </c>
+      <c r="J54">
+        <v>21</v>
+      </c>
+      <c r="K54">
+        <v>7</v>
+      </c>
+      <c r="M54">
+        <v>22</v>
+      </c>
+      <c r="N54">
+        <v>28</v>
+      </c>
+      <c r="O54">
+        <v>38</v>
+      </c>
+      <c r="P54">
+        <v>15</v>
+      </c>
+      <c r="Q54">
+        <v>18</v>
+      </c>
+      <c r="R54">
+        <v>7</v>
+      </c>
+      <c r="T54">
+        <v>21</v>
+      </c>
+      <c r="U54">
+        <v>20</v>
+      </c>
+      <c r="V54">
+        <v>33</v>
+      </c>
+      <c r="W54">
+        <v>13</v>
+      </c>
+      <c r="X54">
+        <v>17</v>
+      </c>
+      <c r="Y54">
+        <v>12</v>
+      </c>
+      <c r="Z54">
+        <v>1</v>
+      </c>
+      <c r="AA54">
+        <v>16</v>
+      </c>
+      <c r="AB54">
+        <v>35</v>
+      </c>
+      <c r="AC54">
+        <v>24</v>
+      </c>
+      <c r="AD54">
+        <v>16</v>
+      </c>
+      <c r="AE54">
+        <v>18</v>
+      </c>
+      <c r="AG54">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>5</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>13</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>4</v>
+      </c>
+      <c r="K55">
+        <v>7</v>
+      </c>
+      <c r="M55">
+        <v>4</v>
+      </c>
+      <c r="N55">
+        <v>2</v>
+      </c>
+      <c r="O55">
+        <v>3</v>
+      </c>
+      <c r="P55">
+        <v>6</v>
+      </c>
+      <c r="Q55">
+        <v>6</v>
+      </c>
+      <c r="R55">
+        <v>2</v>
+      </c>
+      <c r="T55">
+        <v>7</v>
+      </c>
+      <c r="U55">
+        <v>3</v>
+      </c>
+      <c r="V55">
+        <v>8</v>
+      </c>
+      <c r="W55">
+        <v>9</v>
+      </c>
+      <c r="X55">
+        <v>8</v>
+      </c>
+      <c r="Y55">
+        <v>1</v>
+      </c>
+      <c r="AA55">
+        <v>2</v>
+      </c>
+      <c r="AB55">
+        <v>4</v>
+      </c>
+      <c r="AC55">
+        <v>14</v>
+      </c>
+      <c r="AD55">
+        <v>3</v>
+      </c>
+      <c r="AE55">
+        <v>2</v>
+      </c>
+      <c r="AG55">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>14</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>8</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>3</v>
+      </c>
+      <c r="M56">
+        <v>8</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
+        <v>7</v>
+      </c>
+      <c r="P56">
+        <v>3</v>
+      </c>
+      <c r="R56">
+        <v>3</v>
+      </c>
+      <c r="T56">
+        <v>6</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+      <c r="V56">
+        <v>9</v>
+      </c>
+      <c r="W56">
+        <v>1</v>
+      </c>
+      <c r="Y56">
+        <v>3</v>
+      </c>
+      <c r="AA56">
+        <v>14</v>
+      </c>
+      <c r="AB56">
+        <v>1</v>
+      </c>
+      <c r="AC56">
+        <v>10</v>
+      </c>
+      <c r="AD56">
+        <v>2</v>
+      </c>
+      <c r="AG56">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>13</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <v>14</v>
+      </c>
+      <c r="G57">
+        <v>7</v>
+      </c>
+      <c r="H57">
+        <v>8</v>
+      </c>
+      <c r="I57">
+        <v>14</v>
+      </c>
+      <c r="J57">
+        <v>17</v>
+      </c>
+      <c r="M57">
+        <v>8</v>
+      </c>
+      <c r="N57">
+        <v>15</v>
+      </c>
+      <c r="O57">
+        <v>11</v>
+      </c>
+      <c r="P57">
+        <v>8</v>
+      </c>
+      <c r="Q57">
+        <v>6</v>
+      </c>
+      <c r="R57">
+        <v>2</v>
+      </c>
+      <c r="T57">
+        <v>6</v>
+      </c>
+      <c r="U57">
+        <v>15</v>
+      </c>
+      <c r="V57">
+        <v>5</v>
+      </c>
+      <c r="W57">
+        <v>11</v>
+      </c>
+      <c r="X57">
+        <v>8</v>
+      </c>
+      <c r="Y57">
+        <v>4</v>
+      </c>
+      <c r="AA57">
+        <v>10</v>
+      </c>
+      <c r="AB57">
+        <v>15</v>
+      </c>
+      <c r="AC57">
+        <v>12</v>
+      </c>
+      <c r="AD57">
+        <v>16</v>
+      </c>
+      <c r="AE57">
+        <v>4</v>
+      </c>
+      <c r="AG57">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA1B21F-6FFE-4052-B555-7EB4F04AC5E9}">
+  <sheetPr codeName="Sheet14"/>
+  <dimension ref="A1:AG57"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="33" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -24268,9 +28572,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA1B21F-6FFE-4052-B555-7EB4F04AC5E9}">
-  <sheetPr codeName="Sheet14"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236D8D1A-9F6E-4A67-B4B4-577BAEA41071}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -24700,12 +29004,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236D8D1A-9F6E-4A67-B4B4-577BAEA41071}">
-  <sheetPr codeName="Sheet16"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F138D5-7324-41CA-BDE7-6178B269EFE3}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -25134,442 +29439,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F138D5-7324-41CA-BDE7-6178B269EFE3}">
-  <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:AG57"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="33" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-      <c r="Z1">
-        <v>25</v>
-      </c>
-      <c r="AA1">
-        <v>26</v>
-      </c>
-      <c r="AB1">
-        <v>27</v>
-      </c>
-      <c r="AC1">
-        <v>28</v>
-      </c>
-      <c r="AD1">
-        <v>29</v>
-      </c>
-      <c r="AE1">
-        <v>30</v>
-      </c>
-      <c r="AF1">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
   <autoFilter ref="A3:AG57" xr:uid="{AFC2BCF1-614C-4B72-8DE9-95317B022DA5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update statistic files for July 2023
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2023/2023.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C34E34B-4756-4819-907F-9D007D0EED1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89192F80-B118-4F54-8AFA-FA9A8A16BA17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="719" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="75">
   <si>
     <t>branchname</t>
   </si>
@@ -268,6 +268,9 @@
   <si>
     <t>2023-06-01 - 2023-06-30</t>
   </si>
+  <si>
+    <t>2023-07-01 - 2023-07-31</t>
+  </si>
 </sst>
 </file>
 
@@ -302,9 +305,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,7 +643,7 @@
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
@@ -4093,8 +4099,8 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F46">
@@ -5432,9 +5438,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
+    <row r="46" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -5867,9 +5873,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
+    <row r="46" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -5939,8 +5945,9 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
+      <selection activeCell="A46" sqref="A46"/>
+      <selection pane="topRight" activeCell="A46" sqref="A46"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -6302,9 +6309,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
+    <row r="46" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -9649,8 +9656,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B46">
@@ -14128,8 +14135,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B46">
@@ -18541,8 +18548,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E46">
@@ -22849,8 +22856,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -27157,8 +27164,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -28140,6 +28147,4232 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA1B21F-6FFE-4052-B555-7EB4F04AC5E9}">
   <sheetPr codeName="Sheet14"/>
+  <dimension ref="A1:AG57"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
+    <col min="2" max="33" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45108</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45109</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45110</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45111</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45112</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45113</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45114</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45115</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45116</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45117</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45118</v>
+      </c>
+      <c r="M2" s="1">
+        <v>45119</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45120</v>
+      </c>
+      <c r="O2" s="1">
+        <v>45121</v>
+      </c>
+      <c r="P2" s="1">
+        <v>45122</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>45123</v>
+      </c>
+      <c r="R2" s="1">
+        <v>45124</v>
+      </c>
+      <c r="S2" s="1">
+        <v>45125</v>
+      </c>
+      <c r="T2" s="1">
+        <v>45126</v>
+      </c>
+      <c r="U2" s="1">
+        <v>45127</v>
+      </c>
+      <c r="V2" s="1">
+        <v>45128</v>
+      </c>
+      <c r="W2" s="1">
+        <v>45129</v>
+      </c>
+      <c r="X2" s="1">
+        <v>45130</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>45131</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>45132</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>45133</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>45134</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>45135</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>45136</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>45137</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>45138</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>59</v>
+      </c>
+      <c r="R3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T3" t="s">
+        <v>62</v>
+      </c>
+      <c r="U3" t="s">
+        <v>63</v>
+      </c>
+      <c r="V3" t="s">
+        <v>64</v>
+      </c>
+      <c r="W3" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>61</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>68</v>
+      </c>
+      <c r="G4">
+        <v>77</v>
+      </c>
+      <c r="H4">
+        <v>63</v>
+      </c>
+      <c r="I4">
+        <v>37</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>89</v>
+      </c>
+      <c r="L4">
+        <v>75</v>
+      </c>
+      <c r="M4">
+        <v>78</v>
+      </c>
+      <c r="N4">
+        <v>86</v>
+      </c>
+      <c r="O4">
+        <v>51</v>
+      </c>
+      <c r="P4">
+        <v>32</v>
+      </c>
+      <c r="Q4">
+        <v>3</v>
+      </c>
+      <c r="R4">
+        <v>67</v>
+      </c>
+      <c r="S4">
+        <v>60</v>
+      </c>
+      <c r="T4">
+        <v>70</v>
+      </c>
+      <c r="U4">
+        <v>68</v>
+      </c>
+      <c r="V4">
+        <v>53</v>
+      </c>
+      <c r="W4">
+        <v>21</v>
+      </c>
+      <c r="X4">
+        <v>3</v>
+      </c>
+      <c r="Y4">
+        <v>66</v>
+      </c>
+      <c r="Z4">
+        <v>51</v>
+      </c>
+      <c r="AA4">
+        <v>68</v>
+      </c>
+      <c r="AB4">
+        <v>73</v>
+      </c>
+      <c r="AC4">
+        <v>54</v>
+      </c>
+      <c r="AD4">
+        <v>24</v>
+      </c>
+      <c r="AE4">
+        <v>9</v>
+      </c>
+      <c r="AF4">
+        <v>71</v>
+      </c>
+      <c r="AG4">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>53</v>
+      </c>
+      <c r="G5">
+        <v>28</v>
+      </c>
+      <c r="H5">
+        <v>32</v>
+      </c>
+      <c r="I5">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>58</v>
+      </c>
+      <c r="L5">
+        <v>34</v>
+      </c>
+      <c r="M5">
+        <v>34</v>
+      </c>
+      <c r="N5">
+        <v>35</v>
+      </c>
+      <c r="O5">
+        <v>27</v>
+      </c>
+      <c r="P5">
+        <v>28</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>48</v>
+      </c>
+      <c r="S5">
+        <v>38</v>
+      </c>
+      <c r="T5">
+        <v>45</v>
+      </c>
+      <c r="U5">
+        <v>43</v>
+      </c>
+      <c r="V5">
+        <v>29</v>
+      </c>
+      <c r="W5">
+        <v>23</v>
+      </c>
+      <c r="X5">
+        <v>6</v>
+      </c>
+      <c r="Y5">
+        <v>48</v>
+      </c>
+      <c r="Z5">
+        <v>38</v>
+      </c>
+      <c r="AA5">
+        <v>36</v>
+      </c>
+      <c r="AB5">
+        <v>26</v>
+      </c>
+      <c r="AC5">
+        <v>29</v>
+      </c>
+      <c r="AD5">
+        <v>24</v>
+      </c>
+      <c r="AE5">
+        <v>3</v>
+      </c>
+      <c r="AF5">
+        <v>47</v>
+      </c>
+      <c r="AG5">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>66</v>
+      </c>
+      <c r="C6">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>75</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>121</v>
+      </c>
+      <c r="G6">
+        <v>119</v>
+      </c>
+      <c r="H6">
+        <v>96</v>
+      </c>
+      <c r="I6">
+        <v>77</v>
+      </c>
+      <c r="J6">
+        <v>45</v>
+      </c>
+      <c r="K6">
+        <v>99</v>
+      </c>
+      <c r="L6">
+        <v>103</v>
+      </c>
+      <c r="M6">
+        <v>113</v>
+      </c>
+      <c r="N6">
+        <v>91</v>
+      </c>
+      <c r="O6">
+        <v>76</v>
+      </c>
+      <c r="P6">
+        <v>68</v>
+      </c>
+      <c r="Q6">
+        <v>57</v>
+      </c>
+      <c r="R6">
+        <v>119</v>
+      </c>
+      <c r="S6">
+        <v>87</v>
+      </c>
+      <c r="T6">
+        <v>123</v>
+      </c>
+      <c r="U6">
+        <v>119</v>
+      </c>
+      <c r="V6">
+        <v>84</v>
+      </c>
+      <c r="W6">
+        <v>56</v>
+      </c>
+      <c r="X6">
+        <v>52</v>
+      </c>
+      <c r="Y6">
+        <v>93</v>
+      </c>
+      <c r="Z6">
+        <v>125</v>
+      </c>
+      <c r="AA6">
+        <v>109</v>
+      </c>
+      <c r="AB6">
+        <v>86</v>
+      </c>
+      <c r="AC6">
+        <v>77</v>
+      </c>
+      <c r="AD6">
+        <v>59</v>
+      </c>
+      <c r="AE6">
+        <v>51</v>
+      </c>
+      <c r="AF6">
+        <v>104</v>
+      </c>
+      <c r="AG6">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="V7">
+        <v>2</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>6</v>
+      </c>
+      <c r="AB7">
+        <v>4</v>
+      </c>
+      <c r="AC7">
+        <v>1</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AF7">
+        <v>2</v>
+      </c>
+      <c r="AG7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>88</v>
+      </c>
+      <c r="G8">
+        <v>81</v>
+      </c>
+      <c r="H8">
+        <v>64</v>
+      </c>
+      <c r="I8">
+        <v>56</v>
+      </c>
+      <c r="J8">
+        <v>31</v>
+      </c>
+      <c r="K8">
+        <v>78</v>
+      </c>
+      <c r="L8">
+        <v>74</v>
+      </c>
+      <c r="M8">
+        <v>76</v>
+      </c>
+      <c r="N8">
+        <v>67</v>
+      </c>
+      <c r="O8">
+        <v>50</v>
+      </c>
+      <c r="P8">
+        <v>53</v>
+      </c>
+      <c r="Q8">
+        <v>30</v>
+      </c>
+      <c r="R8">
+        <v>58</v>
+      </c>
+      <c r="S8">
+        <v>86</v>
+      </c>
+      <c r="T8">
+        <v>82</v>
+      </c>
+      <c r="U8">
+        <v>69</v>
+      </c>
+      <c r="V8">
+        <v>48</v>
+      </c>
+      <c r="W8">
+        <v>43</v>
+      </c>
+      <c r="X8">
+        <v>29</v>
+      </c>
+      <c r="Y8">
+        <v>72</v>
+      </c>
+      <c r="Z8">
+        <v>83</v>
+      </c>
+      <c r="AA8">
+        <v>73</v>
+      </c>
+      <c r="AB8">
+        <v>72</v>
+      </c>
+      <c r="AC8">
+        <v>72</v>
+      </c>
+      <c r="AD8">
+        <v>51</v>
+      </c>
+      <c r="AE8">
+        <v>25</v>
+      </c>
+      <c r="AF8">
+        <v>71</v>
+      </c>
+      <c r="AG8">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>13</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="O9">
+        <v>5</v>
+      </c>
+      <c r="P9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="S9">
+        <v>7</v>
+      </c>
+      <c r="T9">
+        <v>5</v>
+      </c>
+      <c r="U9">
+        <v>9</v>
+      </c>
+      <c r="V9">
+        <v>3</v>
+      </c>
+      <c r="W9">
+        <v>7</v>
+      </c>
+      <c r="Y9">
+        <v>9</v>
+      </c>
+      <c r="Z9">
+        <v>3</v>
+      </c>
+      <c r="AA9">
+        <v>14</v>
+      </c>
+      <c r="AB9">
+        <v>5</v>
+      </c>
+      <c r="AD9">
+        <v>6</v>
+      </c>
+      <c r="AF9">
+        <v>6</v>
+      </c>
+      <c r="AG9">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <v>15</v>
+      </c>
+      <c r="N10">
+        <v>14</v>
+      </c>
+      <c r="O10">
+        <v>12</v>
+      </c>
+      <c r="P10">
+        <v>10</v>
+      </c>
+      <c r="R10">
+        <v>9</v>
+      </c>
+      <c r="S10">
+        <v>6</v>
+      </c>
+      <c r="T10">
+        <v>7</v>
+      </c>
+      <c r="U10">
+        <v>11</v>
+      </c>
+      <c r="V10">
+        <v>12</v>
+      </c>
+      <c r="W10">
+        <v>11</v>
+      </c>
+      <c r="Y10">
+        <v>9</v>
+      </c>
+      <c r="Z10">
+        <v>10</v>
+      </c>
+      <c r="AA10">
+        <v>10</v>
+      </c>
+      <c r="AB10">
+        <v>12</v>
+      </c>
+      <c r="AC10">
+        <v>16</v>
+      </c>
+      <c r="AD10">
+        <v>5</v>
+      </c>
+      <c r="AF10">
+        <v>14</v>
+      </c>
+      <c r="AG10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>8</v>
+      </c>
+      <c r="T11">
+        <v>15</v>
+      </c>
+      <c r="U11">
+        <v>4</v>
+      </c>
+      <c r="V11">
+        <v>11</v>
+      </c>
+      <c r="W11">
+        <v>3</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>14</v>
+      </c>
+      <c r="AA11">
+        <v>11</v>
+      </c>
+      <c r="AB11">
+        <v>3</v>
+      </c>
+      <c r="AC11">
+        <v>6</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AF11">
+        <v>11</v>
+      </c>
+      <c r="AG11">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>2</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>4</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <v>8</v>
+      </c>
+      <c r="U14">
+        <v>5</v>
+      </c>
+      <c r="V14">
+        <v>5</v>
+      </c>
+      <c r="Y14">
+        <v>6</v>
+      </c>
+      <c r="AA14">
+        <v>6</v>
+      </c>
+      <c r="AB14">
+        <v>5</v>
+      </c>
+      <c r="AC14">
+        <v>5</v>
+      </c>
+      <c r="AF14">
+        <v>5</v>
+      </c>
+      <c r="AG14">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15">
+        <v>9</v>
+      </c>
+      <c r="N15">
+        <v>3</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>10</v>
+      </c>
+      <c r="S15">
+        <v>8</v>
+      </c>
+      <c r="T15">
+        <v>12</v>
+      </c>
+      <c r="U15">
+        <v>3</v>
+      </c>
+      <c r="V15">
+        <v>7</v>
+      </c>
+      <c r="W15">
+        <v>3</v>
+      </c>
+      <c r="X15">
+        <v>3</v>
+      </c>
+      <c r="Y15">
+        <v>8</v>
+      </c>
+      <c r="Z15">
+        <v>8</v>
+      </c>
+      <c r="AA15">
+        <v>8</v>
+      </c>
+      <c r="AB15">
+        <v>4</v>
+      </c>
+      <c r="AC15">
+        <v>7</v>
+      </c>
+      <c r="AD15">
+        <v>4</v>
+      </c>
+      <c r="AF15">
+        <v>11</v>
+      </c>
+      <c r="AG15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>13</v>
+      </c>
+      <c r="H16">
+        <v>13</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>12</v>
+      </c>
+      <c r="L16">
+        <v>15</v>
+      </c>
+      <c r="M16">
+        <v>21</v>
+      </c>
+      <c r="N16">
+        <v>12</v>
+      </c>
+      <c r="O16">
+        <v>7</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>14</v>
+      </c>
+      <c r="S16">
+        <v>16</v>
+      </c>
+      <c r="T16">
+        <v>15</v>
+      </c>
+      <c r="U16">
+        <v>9</v>
+      </c>
+      <c r="V16">
+        <v>13</v>
+      </c>
+      <c r="W16">
+        <v>5</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+      <c r="Y16">
+        <v>9</v>
+      </c>
+      <c r="Z16">
+        <v>13</v>
+      </c>
+      <c r="AA16">
+        <v>12</v>
+      </c>
+      <c r="AB16">
+        <v>15</v>
+      </c>
+      <c r="AC16">
+        <v>8</v>
+      </c>
+      <c r="AD16">
+        <v>3</v>
+      </c>
+      <c r="AF16">
+        <v>15</v>
+      </c>
+      <c r="AG16">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <v>6</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <v>5</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="R17">
+        <v>12</v>
+      </c>
+      <c r="S17">
+        <v>9</v>
+      </c>
+      <c r="T17">
+        <v>6</v>
+      </c>
+      <c r="U17">
+        <v>7</v>
+      </c>
+      <c r="V17">
+        <v>4</v>
+      </c>
+      <c r="W17">
+        <v>4</v>
+      </c>
+      <c r="Y17">
+        <v>12</v>
+      </c>
+      <c r="Z17">
+        <v>8</v>
+      </c>
+      <c r="AA17">
+        <v>6</v>
+      </c>
+      <c r="AB17">
+        <v>7</v>
+      </c>
+      <c r="AC17">
+        <v>4</v>
+      </c>
+      <c r="AD17">
+        <v>5</v>
+      </c>
+      <c r="AF17">
+        <v>3</v>
+      </c>
+      <c r="AG17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>11</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>6</v>
+      </c>
+      <c r="L18">
+        <v>6</v>
+      </c>
+      <c r="M18">
+        <v>6</v>
+      </c>
+      <c r="N18">
+        <v>4</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>3</v>
+      </c>
+      <c r="R18">
+        <v>5</v>
+      </c>
+      <c r="S18">
+        <v>4</v>
+      </c>
+      <c r="T18">
+        <v>9</v>
+      </c>
+      <c r="U18">
+        <v>2</v>
+      </c>
+      <c r="V18">
+        <v>3</v>
+      </c>
+      <c r="W18">
+        <v>4</v>
+      </c>
+      <c r="Y18">
+        <v>2</v>
+      </c>
+      <c r="Z18">
+        <v>4</v>
+      </c>
+      <c r="AA18">
+        <v>13</v>
+      </c>
+      <c r="AB18">
+        <v>5</v>
+      </c>
+      <c r="AC18">
+        <v>2</v>
+      </c>
+      <c r="AD18">
+        <v>6</v>
+      </c>
+      <c r="AF18">
+        <v>6</v>
+      </c>
+      <c r="AG18">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>46</v>
+      </c>
+      <c r="H19">
+        <v>42</v>
+      </c>
+      <c r="I19">
+        <v>24</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>41</v>
+      </c>
+      <c r="L19">
+        <v>28</v>
+      </c>
+      <c r="M19">
+        <v>33</v>
+      </c>
+      <c r="N19">
+        <v>34</v>
+      </c>
+      <c r="O19">
+        <v>17</v>
+      </c>
+      <c r="P19">
+        <v>19</v>
+      </c>
+      <c r="Q19">
+        <v>3</v>
+      </c>
+      <c r="R19">
+        <v>37</v>
+      </c>
+      <c r="S19">
+        <v>33</v>
+      </c>
+      <c r="T19">
+        <v>30</v>
+      </c>
+      <c r="U19">
+        <v>23</v>
+      </c>
+      <c r="V19">
+        <v>29</v>
+      </c>
+      <c r="W19">
+        <v>25</v>
+      </c>
+      <c r="X19">
+        <v>3</v>
+      </c>
+      <c r="Y19">
+        <v>30</v>
+      </c>
+      <c r="Z19">
+        <v>32</v>
+      </c>
+      <c r="AA19">
+        <v>27</v>
+      </c>
+      <c r="AB19">
+        <v>25</v>
+      </c>
+      <c r="AC19">
+        <v>23</v>
+      </c>
+      <c r="AD19">
+        <v>12</v>
+      </c>
+      <c r="AF19">
+        <v>33</v>
+      </c>
+      <c r="AG19">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="R20">
+        <v>3</v>
+      </c>
+      <c r="S20">
+        <v>4</v>
+      </c>
+      <c r="U20">
+        <v>4</v>
+      </c>
+      <c r="W20">
+        <v>3</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>2</v>
+      </c>
+      <c r="AB20">
+        <v>4</v>
+      </c>
+      <c r="AF20">
+        <v>3</v>
+      </c>
+      <c r="AG20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>27</v>
+      </c>
+      <c r="G21">
+        <v>38</v>
+      </c>
+      <c r="H21">
+        <v>33</v>
+      </c>
+      <c r="I21">
+        <v>14</v>
+      </c>
+      <c r="J21">
+        <v>11</v>
+      </c>
+      <c r="K21">
+        <v>43</v>
+      </c>
+      <c r="L21">
+        <v>31</v>
+      </c>
+      <c r="M21">
+        <v>38</v>
+      </c>
+      <c r="N21">
+        <v>40</v>
+      </c>
+      <c r="O21">
+        <v>22</v>
+      </c>
+      <c r="P21">
+        <v>13</v>
+      </c>
+      <c r="Q21">
+        <v>13</v>
+      </c>
+      <c r="R21">
+        <v>32</v>
+      </c>
+      <c r="S21">
+        <v>31</v>
+      </c>
+      <c r="T21">
+        <v>30</v>
+      </c>
+      <c r="U21">
+        <v>41</v>
+      </c>
+      <c r="V21">
+        <v>23</v>
+      </c>
+      <c r="W21">
+        <v>14</v>
+      </c>
+      <c r="X21">
+        <v>11</v>
+      </c>
+      <c r="Y21">
+        <v>38</v>
+      </c>
+      <c r="Z21">
+        <v>45</v>
+      </c>
+      <c r="AA21">
+        <v>36</v>
+      </c>
+      <c r="AB21">
+        <v>45</v>
+      </c>
+      <c r="AC21">
+        <v>23</v>
+      </c>
+      <c r="AD21">
+        <v>9</v>
+      </c>
+      <c r="AE21">
+        <v>13</v>
+      </c>
+      <c r="AF21">
+        <v>37</v>
+      </c>
+      <c r="AG21">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23">
+        <v>60</v>
+      </c>
+      <c r="G23">
+        <v>43</v>
+      </c>
+      <c r="H23">
+        <v>38</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>31</v>
+      </c>
+      <c r="L23">
+        <v>45</v>
+      </c>
+      <c r="M23">
+        <v>45</v>
+      </c>
+      <c r="N23">
+        <v>35</v>
+      </c>
+      <c r="O23">
+        <v>31</v>
+      </c>
+      <c r="P23">
+        <v>16</v>
+      </c>
+      <c r="R23">
+        <v>37</v>
+      </c>
+      <c r="S23">
+        <v>38</v>
+      </c>
+      <c r="T23">
+        <v>37</v>
+      </c>
+      <c r="U23">
+        <v>34</v>
+      </c>
+      <c r="V23">
+        <v>21</v>
+      </c>
+      <c r="W23">
+        <v>11</v>
+      </c>
+      <c r="Y23">
+        <v>35</v>
+      </c>
+      <c r="Z23">
+        <v>40</v>
+      </c>
+      <c r="AA23">
+        <v>38</v>
+      </c>
+      <c r="AB23">
+        <v>30</v>
+      </c>
+      <c r="AC23">
+        <v>41</v>
+      </c>
+      <c r="AD23">
+        <v>13</v>
+      </c>
+      <c r="AF23">
+        <v>40</v>
+      </c>
+      <c r="AG23">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>3</v>
+      </c>
+      <c r="O24">
+        <v>3</v>
+      </c>
+      <c r="R24">
+        <v>6</v>
+      </c>
+      <c r="S24">
+        <v>4</v>
+      </c>
+      <c r="T24">
+        <v>5</v>
+      </c>
+      <c r="U24">
+        <v>2</v>
+      </c>
+      <c r="V24">
+        <v>5</v>
+      </c>
+      <c r="Y24">
+        <v>6</v>
+      </c>
+      <c r="Z24">
+        <v>4</v>
+      </c>
+      <c r="AA24">
+        <v>3</v>
+      </c>
+      <c r="AB24">
+        <v>3</v>
+      </c>
+      <c r="AF24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>44</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>43</v>
+      </c>
+      <c r="G25">
+        <v>55</v>
+      </c>
+      <c r="H25">
+        <v>25</v>
+      </c>
+      <c r="I25">
+        <v>30</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>42</v>
+      </c>
+      <c r="L25">
+        <v>38</v>
+      </c>
+      <c r="M25">
+        <v>33</v>
+      </c>
+      <c r="N25">
+        <v>39</v>
+      </c>
+      <c r="O25">
+        <v>37</v>
+      </c>
+      <c r="P25">
+        <v>20</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25">
+        <v>34</v>
+      </c>
+      <c r="S25">
+        <v>52</v>
+      </c>
+      <c r="T25">
+        <v>35</v>
+      </c>
+      <c r="U25">
+        <v>49</v>
+      </c>
+      <c r="V25">
+        <v>49</v>
+      </c>
+      <c r="W25">
+        <v>18</v>
+      </c>
+      <c r="X25">
+        <v>2</v>
+      </c>
+      <c r="Y25">
+        <v>37</v>
+      </c>
+      <c r="Z25">
+        <v>41</v>
+      </c>
+      <c r="AA25">
+        <v>39</v>
+      </c>
+      <c r="AB25">
+        <v>38</v>
+      </c>
+      <c r="AC25">
+        <v>41</v>
+      </c>
+      <c r="AD25">
+        <v>22</v>
+      </c>
+      <c r="AE25">
+        <v>4</v>
+      </c>
+      <c r="AF25">
+        <v>48</v>
+      </c>
+      <c r="AG25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>64</v>
+      </c>
+      <c r="C26">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>99</v>
+      </c>
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26">
+        <v>155</v>
+      </c>
+      <c r="G26">
+        <v>102</v>
+      </c>
+      <c r="H26">
+        <v>92</v>
+      </c>
+      <c r="I26">
+        <v>64</v>
+      </c>
+      <c r="J26">
+        <v>34</v>
+      </c>
+      <c r="K26">
+        <v>120</v>
+      </c>
+      <c r="L26">
+        <v>110</v>
+      </c>
+      <c r="M26">
+        <v>105</v>
+      </c>
+      <c r="N26">
+        <v>110</v>
+      </c>
+      <c r="O26">
+        <v>77</v>
+      </c>
+      <c r="P26">
+        <v>70</v>
+      </c>
+      <c r="Q26">
+        <v>40</v>
+      </c>
+      <c r="R26">
+        <v>98</v>
+      </c>
+      <c r="S26">
+        <v>101</v>
+      </c>
+      <c r="T26">
+        <v>114</v>
+      </c>
+      <c r="U26">
+        <v>104</v>
+      </c>
+      <c r="V26">
+        <v>95</v>
+      </c>
+      <c r="W26">
+        <v>81</v>
+      </c>
+      <c r="X26">
+        <v>32</v>
+      </c>
+      <c r="Y26">
+        <v>125</v>
+      </c>
+      <c r="Z26">
+        <v>119</v>
+      </c>
+      <c r="AA26">
+        <v>144</v>
+      </c>
+      <c r="AB26">
+        <v>91</v>
+      </c>
+      <c r="AC26">
+        <v>90</v>
+      </c>
+      <c r="AD26">
+        <v>71</v>
+      </c>
+      <c r="AE26">
+        <v>41</v>
+      </c>
+      <c r="AF26">
+        <v>127</v>
+      </c>
+      <c r="AG26">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>16</v>
+      </c>
+      <c r="G27">
+        <v>14</v>
+      </c>
+      <c r="H27">
+        <v>9</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <v>11</v>
+      </c>
+      <c r="L27">
+        <v>11</v>
+      </c>
+      <c r="M27">
+        <v>17</v>
+      </c>
+      <c r="N27">
+        <v>9</v>
+      </c>
+      <c r="O27">
+        <v>10</v>
+      </c>
+      <c r="P27">
+        <v>7</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>12</v>
+      </c>
+      <c r="S27">
+        <v>17</v>
+      </c>
+      <c r="T27">
+        <v>7</v>
+      </c>
+      <c r="U27">
+        <v>17</v>
+      </c>
+      <c r="V27">
+        <v>10</v>
+      </c>
+      <c r="W27">
+        <v>6</v>
+      </c>
+      <c r="X27">
+        <v>1</v>
+      </c>
+      <c r="Y27">
+        <v>12</v>
+      </c>
+      <c r="Z27">
+        <v>9</v>
+      </c>
+      <c r="AA27">
+        <v>7</v>
+      </c>
+      <c r="AB27">
+        <v>11</v>
+      </c>
+      <c r="AC27">
+        <v>9</v>
+      </c>
+      <c r="AD27">
+        <v>7</v>
+      </c>
+      <c r="AE27">
+        <v>2</v>
+      </c>
+      <c r="AF27">
+        <v>12</v>
+      </c>
+      <c r="AG27">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>15</v>
+      </c>
+      <c r="I29">
+        <v>8</v>
+      </c>
+      <c r="K29">
+        <v>18</v>
+      </c>
+      <c r="L29">
+        <v>8</v>
+      </c>
+      <c r="M29">
+        <v>7</v>
+      </c>
+      <c r="N29">
+        <v>16</v>
+      </c>
+      <c r="P29">
+        <v>9</v>
+      </c>
+      <c r="Q29">
+        <v>1</v>
+      </c>
+      <c r="R29">
+        <v>17</v>
+      </c>
+      <c r="S29">
+        <v>4</v>
+      </c>
+      <c r="T29">
+        <v>13</v>
+      </c>
+      <c r="U29">
+        <v>11</v>
+      </c>
+      <c r="W29">
+        <v>5</v>
+      </c>
+      <c r="Y29">
+        <v>17</v>
+      </c>
+      <c r="Z29">
+        <v>9</v>
+      </c>
+      <c r="AA29">
+        <v>12</v>
+      </c>
+      <c r="AB29">
+        <v>10</v>
+      </c>
+      <c r="AD29">
+        <v>6</v>
+      </c>
+      <c r="AE29">
+        <v>1</v>
+      </c>
+      <c r="AF29">
+        <v>10</v>
+      </c>
+      <c r="AG29">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>5</v>
+      </c>
+      <c r="L30">
+        <v>5</v>
+      </c>
+      <c r="M30">
+        <v>6</v>
+      </c>
+      <c r="N30">
+        <v>3</v>
+      </c>
+      <c r="O30">
+        <v>2</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>5</v>
+      </c>
+      <c r="T30">
+        <v>8</v>
+      </c>
+      <c r="U30">
+        <v>3</v>
+      </c>
+      <c r="V30">
+        <v>7</v>
+      </c>
+      <c r="W30">
+        <v>6</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>2</v>
+      </c>
+      <c r="AA30">
+        <v>4</v>
+      </c>
+      <c r="AB30">
+        <v>2</v>
+      </c>
+      <c r="AC30">
+        <v>4</v>
+      </c>
+      <c r="AD30">
+        <v>1</v>
+      </c>
+      <c r="AF30">
+        <v>3</v>
+      </c>
+      <c r="AG30">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>31</v>
+      </c>
+      <c r="F31">
+        <v>28</v>
+      </c>
+      <c r="G31">
+        <v>31</v>
+      </c>
+      <c r="H31">
+        <v>24</v>
+      </c>
+      <c r="I31">
+        <v>7</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="K31">
+        <v>27</v>
+      </c>
+      <c r="L31">
+        <v>33</v>
+      </c>
+      <c r="M31">
+        <v>28</v>
+      </c>
+      <c r="N31">
+        <v>29</v>
+      </c>
+      <c r="O31">
+        <v>15</v>
+      </c>
+      <c r="P31">
+        <v>12</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+      <c r="R31">
+        <v>16</v>
+      </c>
+      <c r="S31">
+        <v>33</v>
+      </c>
+      <c r="T31">
+        <v>24</v>
+      </c>
+      <c r="U31">
+        <v>22</v>
+      </c>
+      <c r="V31">
+        <v>30</v>
+      </c>
+      <c r="W31">
+        <v>6</v>
+      </c>
+      <c r="X31">
+        <v>1</v>
+      </c>
+      <c r="Y31">
+        <v>20</v>
+      </c>
+      <c r="Z31">
+        <v>29</v>
+      </c>
+      <c r="AA31">
+        <v>22</v>
+      </c>
+      <c r="AB31">
+        <v>17</v>
+      </c>
+      <c r="AC31">
+        <v>19</v>
+      </c>
+      <c r="AD31">
+        <v>7</v>
+      </c>
+      <c r="AF31">
+        <v>23</v>
+      </c>
+      <c r="AG31">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>3</v>
+      </c>
+      <c r="S32">
+        <v>2</v>
+      </c>
+      <c r="V32">
+        <v>7</v>
+      </c>
+      <c r="Y32">
+        <v>2</v>
+      </c>
+      <c r="Z32">
+        <v>1</v>
+      </c>
+      <c r="AA32">
+        <v>2</v>
+      </c>
+      <c r="AC32">
+        <v>1</v>
+      </c>
+      <c r="AF32">
+        <v>3</v>
+      </c>
+      <c r="AG32">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>11</v>
+      </c>
+      <c r="H33">
+        <v>12</v>
+      </c>
+      <c r="L33">
+        <v>8</v>
+      </c>
+      <c r="M33">
+        <v>7</v>
+      </c>
+      <c r="N33">
+        <v>6</v>
+      </c>
+      <c r="O33">
+        <v>12</v>
+      </c>
+      <c r="P33">
+        <v>2</v>
+      </c>
+      <c r="S33">
+        <v>10</v>
+      </c>
+      <c r="T33">
+        <v>3</v>
+      </c>
+      <c r="U33">
+        <v>1</v>
+      </c>
+      <c r="V33">
+        <v>4</v>
+      </c>
+      <c r="W33">
+        <v>3</v>
+      </c>
+      <c r="Z33">
+        <v>7</v>
+      </c>
+      <c r="AA33">
+        <v>5</v>
+      </c>
+      <c r="AB33">
+        <v>9</v>
+      </c>
+      <c r="AC33">
+        <v>5</v>
+      </c>
+      <c r="AD33">
+        <v>1</v>
+      </c>
+      <c r="AF33">
+        <v>1</v>
+      </c>
+      <c r="AG33">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="D34">
+        <v>25</v>
+      </c>
+      <c r="F34">
+        <v>36</v>
+      </c>
+      <c r="G34">
+        <v>38</v>
+      </c>
+      <c r="H34">
+        <v>50</v>
+      </c>
+      <c r="I34">
+        <v>12</v>
+      </c>
+      <c r="K34">
+        <v>48</v>
+      </c>
+      <c r="L34">
+        <v>53</v>
+      </c>
+      <c r="M34">
+        <v>46</v>
+      </c>
+      <c r="N34">
+        <v>43</v>
+      </c>
+      <c r="O34">
+        <v>34</v>
+      </c>
+      <c r="P34">
+        <v>24</v>
+      </c>
+      <c r="R34">
+        <v>56</v>
+      </c>
+      <c r="S34">
+        <v>39</v>
+      </c>
+      <c r="T34">
+        <v>51</v>
+      </c>
+      <c r="U34">
+        <v>37</v>
+      </c>
+      <c r="V34">
+        <v>34</v>
+      </c>
+      <c r="W34">
+        <v>18</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <v>38</v>
+      </c>
+      <c r="Z34">
+        <v>35</v>
+      </c>
+      <c r="AA34">
+        <v>33</v>
+      </c>
+      <c r="AB34">
+        <v>16</v>
+      </c>
+      <c r="AC34">
+        <v>30</v>
+      </c>
+      <c r="AD34">
+        <v>17</v>
+      </c>
+      <c r="AF34">
+        <v>43</v>
+      </c>
+      <c r="AG34">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>31</v>
+      </c>
+      <c r="G35">
+        <v>22</v>
+      </c>
+      <c r="H35">
+        <v>40</v>
+      </c>
+      <c r="I35">
+        <v>15</v>
+      </c>
+      <c r="K35">
+        <v>5</v>
+      </c>
+      <c r="L35">
+        <v>46</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <v>28</v>
+      </c>
+      <c r="O35">
+        <v>17</v>
+      </c>
+      <c r="P35">
+        <v>14</v>
+      </c>
+      <c r="Q35">
+        <v>2</v>
+      </c>
+      <c r="R35">
+        <v>31</v>
+      </c>
+      <c r="S35">
+        <v>29</v>
+      </c>
+      <c r="T35">
+        <v>19</v>
+      </c>
+      <c r="U35">
+        <v>32</v>
+      </c>
+      <c r="V35">
+        <v>27</v>
+      </c>
+      <c r="W35">
+        <v>13</v>
+      </c>
+      <c r="Y35">
+        <v>47</v>
+      </c>
+      <c r="Z35">
+        <v>18</v>
+      </c>
+      <c r="AA35">
+        <v>23</v>
+      </c>
+      <c r="AB35">
+        <v>27</v>
+      </c>
+      <c r="AC35">
+        <v>23</v>
+      </c>
+      <c r="AD35">
+        <v>19</v>
+      </c>
+      <c r="AE35">
+        <v>2</v>
+      </c>
+      <c r="AF35">
+        <v>27</v>
+      </c>
+      <c r="AG35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>23</v>
+      </c>
+      <c r="G36">
+        <v>24</v>
+      </c>
+      <c r="H36">
+        <v>17</v>
+      </c>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>19</v>
+      </c>
+      <c r="L36">
+        <v>15</v>
+      </c>
+      <c r="M36">
+        <v>16</v>
+      </c>
+      <c r="N36">
+        <v>21</v>
+      </c>
+      <c r="O36">
+        <v>7</v>
+      </c>
+      <c r="P36">
+        <v>6</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>21</v>
+      </c>
+      <c r="T36">
+        <v>24</v>
+      </c>
+      <c r="U36">
+        <v>18</v>
+      </c>
+      <c r="V36">
+        <v>12</v>
+      </c>
+      <c r="W36">
+        <v>6</v>
+      </c>
+      <c r="X36">
+        <v>3</v>
+      </c>
+      <c r="Y36">
+        <v>1</v>
+      </c>
+      <c r="AA36">
+        <v>26</v>
+      </c>
+      <c r="AB36">
+        <v>22</v>
+      </c>
+      <c r="AC36">
+        <v>16</v>
+      </c>
+      <c r="AD36">
+        <v>10</v>
+      </c>
+      <c r="AF36">
+        <v>24</v>
+      </c>
+      <c r="AG36">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>43</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>109</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>114</v>
+      </c>
+      <c r="G37">
+        <v>98</v>
+      </c>
+      <c r="H37">
+        <v>87</v>
+      </c>
+      <c r="I37">
+        <v>40</v>
+      </c>
+      <c r="J37">
+        <v>5</v>
+      </c>
+      <c r="K37">
+        <v>107</v>
+      </c>
+      <c r="L37">
+        <v>91</v>
+      </c>
+      <c r="M37">
+        <v>103</v>
+      </c>
+      <c r="N37">
+        <v>80</v>
+      </c>
+      <c r="O37">
+        <v>77</v>
+      </c>
+      <c r="P37">
+        <v>46</v>
+      </c>
+      <c r="Q37">
+        <v>3</v>
+      </c>
+      <c r="R37">
+        <v>113</v>
+      </c>
+      <c r="S37">
+        <v>92</v>
+      </c>
+      <c r="T37">
+        <v>94</v>
+      </c>
+      <c r="U37">
+        <v>102</v>
+      </c>
+      <c r="V37">
+        <v>84</v>
+      </c>
+      <c r="W37">
+        <v>43</v>
+      </c>
+      <c r="X37">
+        <v>2</v>
+      </c>
+      <c r="Y37">
+        <v>108</v>
+      </c>
+      <c r="Z37">
+        <v>80</v>
+      </c>
+      <c r="AA37">
+        <v>82</v>
+      </c>
+      <c r="AB37">
+        <v>70</v>
+      </c>
+      <c r="AC37">
+        <v>71</v>
+      </c>
+      <c r="AD37">
+        <v>30</v>
+      </c>
+      <c r="AE37">
+        <v>2</v>
+      </c>
+      <c r="AF37">
+        <v>82</v>
+      </c>
+      <c r="AG37">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>15</v>
+      </c>
+      <c r="F38">
+        <v>15</v>
+      </c>
+      <c r="G38">
+        <v>23</v>
+      </c>
+      <c r="H38">
+        <v>21</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="K38">
+        <v>16</v>
+      </c>
+      <c r="L38">
+        <v>12</v>
+      </c>
+      <c r="M38">
+        <v>17</v>
+      </c>
+      <c r="N38">
+        <v>28</v>
+      </c>
+      <c r="O38">
+        <v>15</v>
+      </c>
+      <c r="P38">
+        <v>8</v>
+      </c>
+      <c r="R38">
+        <v>22</v>
+      </c>
+      <c r="S38">
+        <v>17</v>
+      </c>
+      <c r="T38">
+        <v>18</v>
+      </c>
+      <c r="U38">
+        <v>25</v>
+      </c>
+      <c r="V38">
+        <v>14</v>
+      </c>
+      <c r="W38">
+        <v>6</v>
+      </c>
+      <c r="Y38">
+        <v>16</v>
+      </c>
+      <c r="Z38">
+        <v>22</v>
+      </c>
+      <c r="AA38">
+        <v>14</v>
+      </c>
+      <c r="AB38">
+        <v>13</v>
+      </c>
+      <c r="AC38">
+        <v>17</v>
+      </c>
+      <c r="AD38">
+        <v>10</v>
+      </c>
+      <c r="AF38">
+        <v>18</v>
+      </c>
+      <c r="AG38">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39">
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>57</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>67</v>
+      </c>
+      <c r="G39">
+        <v>78</v>
+      </c>
+      <c r="H39">
+        <v>56</v>
+      </c>
+      <c r="I39">
+        <v>42</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>81</v>
+      </c>
+      <c r="L39">
+        <v>62</v>
+      </c>
+      <c r="M39">
+        <v>73</v>
+      </c>
+      <c r="N39">
+        <v>70</v>
+      </c>
+      <c r="O39">
+        <v>56</v>
+      </c>
+      <c r="P39">
+        <v>32</v>
+      </c>
+      <c r="Q39">
+        <v>3</v>
+      </c>
+      <c r="R39">
+        <v>68</v>
+      </c>
+      <c r="S39">
+        <v>64</v>
+      </c>
+      <c r="T39">
+        <v>67</v>
+      </c>
+      <c r="U39">
+        <v>60</v>
+      </c>
+      <c r="V39">
+        <v>54</v>
+      </c>
+      <c r="W39">
+        <v>23</v>
+      </c>
+      <c r="X39">
+        <v>3</v>
+      </c>
+      <c r="Y39">
+        <v>74</v>
+      </c>
+      <c r="Z39">
+        <v>73</v>
+      </c>
+      <c r="AA39">
+        <v>48</v>
+      </c>
+      <c r="AB39">
+        <v>50</v>
+      </c>
+      <c r="AC39">
+        <v>48</v>
+      </c>
+      <c r="AD39">
+        <v>29</v>
+      </c>
+      <c r="AE39">
+        <v>3</v>
+      </c>
+      <c r="AF39">
+        <v>83</v>
+      </c>
+      <c r="AG39">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>8</v>
+      </c>
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="L40">
+        <v>6</v>
+      </c>
+      <c r="N40">
+        <v>13</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+      <c r="S40">
+        <v>6</v>
+      </c>
+      <c r="U40">
+        <v>15</v>
+      </c>
+      <c r="W40">
+        <v>2</v>
+      </c>
+      <c r="Z40">
+        <v>2</v>
+      </c>
+      <c r="AB40">
+        <v>2</v>
+      </c>
+      <c r="AD40">
+        <v>2</v>
+      </c>
+      <c r="AE40">
+        <v>1</v>
+      </c>
+      <c r="AG40">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>9</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>3</v>
+      </c>
+      <c r="T41">
+        <v>2</v>
+      </c>
+      <c r="U41">
+        <v>6</v>
+      </c>
+      <c r="V41">
+        <v>3</v>
+      </c>
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="Z41">
+        <v>4</v>
+      </c>
+      <c r="AA41">
+        <v>3</v>
+      </c>
+      <c r="AC41">
+        <v>4</v>
+      </c>
+      <c r="AD41">
+        <v>3</v>
+      </c>
+      <c r="AF41">
+        <v>1</v>
+      </c>
+      <c r="AG41">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>13</v>
+      </c>
+      <c r="F47">
+        <v>15</v>
+      </c>
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47">
+        <v>10</v>
+      </c>
+      <c r="I47">
+        <v>4</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>10</v>
+      </c>
+      <c r="M47">
+        <v>14</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>2</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+      <c r="R47">
+        <v>9</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
+      </c>
+      <c r="T47">
+        <v>15</v>
+      </c>
+      <c r="U47">
+        <v>17</v>
+      </c>
+      <c r="V47">
+        <v>13</v>
+      </c>
+      <c r="W47">
+        <v>6</v>
+      </c>
+      <c r="Y47">
+        <v>9</v>
+      </c>
+      <c r="AA47">
+        <v>19</v>
+      </c>
+      <c r="AB47">
+        <v>12</v>
+      </c>
+      <c r="AC47">
+        <v>7</v>
+      </c>
+      <c r="AD47">
+        <v>4</v>
+      </c>
+      <c r="AF47">
+        <v>1</v>
+      </c>
+      <c r="AG47">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>12</v>
+      </c>
+      <c r="F48">
+        <v>20</v>
+      </c>
+      <c r="G48">
+        <v>21</v>
+      </c>
+      <c r="H48">
+        <v>16</v>
+      </c>
+      <c r="I48">
+        <v>7</v>
+      </c>
+      <c r="K48">
+        <v>44</v>
+      </c>
+      <c r="L48">
+        <v>31</v>
+      </c>
+      <c r="M48">
+        <v>26</v>
+      </c>
+      <c r="N48">
+        <v>12</v>
+      </c>
+      <c r="O48">
+        <v>18</v>
+      </c>
+      <c r="P48">
+        <v>4</v>
+      </c>
+      <c r="R48">
+        <v>28</v>
+      </c>
+      <c r="S48">
+        <v>32</v>
+      </c>
+      <c r="T48">
+        <v>39</v>
+      </c>
+      <c r="U48">
+        <v>31</v>
+      </c>
+      <c r="V48">
+        <v>27</v>
+      </c>
+      <c r="W48">
+        <v>1</v>
+      </c>
+      <c r="Y48">
+        <v>27</v>
+      </c>
+      <c r="Z48">
+        <v>53</v>
+      </c>
+      <c r="AA48">
+        <v>20</v>
+      </c>
+      <c r="AB48">
+        <v>27</v>
+      </c>
+      <c r="AC48">
+        <v>28</v>
+      </c>
+      <c r="AD48">
+        <v>5</v>
+      </c>
+      <c r="AE48">
+        <v>1</v>
+      </c>
+      <c r="AF48">
+        <v>36</v>
+      </c>
+      <c r="AG48">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>40</v>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>40</v>
+      </c>
+      <c r="G49">
+        <v>30</v>
+      </c>
+      <c r="H49">
+        <v>21</v>
+      </c>
+      <c r="I49">
+        <v>22</v>
+      </c>
+      <c r="J49">
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <v>45</v>
+      </c>
+      <c r="L49">
+        <v>33</v>
+      </c>
+      <c r="M49">
+        <v>41</v>
+      </c>
+      <c r="N49">
+        <v>40</v>
+      </c>
+      <c r="O49">
+        <v>21</v>
+      </c>
+      <c r="P49">
+        <v>16</v>
+      </c>
+      <c r="Q49">
+        <v>2</v>
+      </c>
+      <c r="R49">
+        <v>34</v>
+      </c>
+      <c r="S49">
+        <v>21</v>
+      </c>
+      <c r="T49">
+        <v>39</v>
+      </c>
+      <c r="U49">
+        <v>30</v>
+      </c>
+      <c r="V49">
+        <v>27</v>
+      </c>
+      <c r="W49">
+        <v>20</v>
+      </c>
+      <c r="X49">
+        <v>2</v>
+      </c>
+      <c r="Y49">
+        <v>35</v>
+      </c>
+      <c r="Z49">
+        <v>19</v>
+      </c>
+      <c r="AA49">
+        <v>26</v>
+      </c>
+      <c r="AB49">
+        <v>28</v>
+      </c>
+      <c r="AC49">
+        <v>23</v>
+      </c>
+      <c r="AD49">
+        <v>9</v>
+      </c>
+      <c r="AF49">
+        <v>40</v>
+      </c>
+      <c r="AG49">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>35</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>3</v>
+      </c>
+      <c r="G50">
+        <v>56</v>
+      </c>
+      <c r="H50">
+        <v>44</v>
+      </c>
+      <c r="I50">
+        <v>11</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>44</v>
+      </c>
+      <c r="L50">
+        <v>24</v>
+      </c>
+      <c r="M50">
+        <v>35</v>
+      </c>
+      <c r="N50">
+        <v>33</v>
+      </c>
+      <c r="O50">
+        <v>40</v>
+      </c>
+      <c r="P50">
+        <v>6</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>41</v>
+      </c>
+      <c r="S50">
+        <v>28</v>
+      </c>
+      <c r="T50">
+        <v>27</v>
+      </c>
+      <c r="U50">
+        <v>36</v>
+      </c>
+      <c r="V50">
+        <v>31</v>
+      </c>
+      <c r="W50">
+        <v>5</v>
+      </c>
+      <c r="X50">
+        <v>1</v>
+      </c>
+      <c r="Y50">
+        <v>35</v>
+      </c>
+      <c r="Z50">
+        <v>33</v>
+      </c>
+      <c r="AA50">
+        <v>31</v>
+      </c>
+      <c r="AB50">
+        <v>21</v>
+      </c>
+      <c r="AC50">
+        <v>30</v>
+      </c>
+      <c r="AD50">
+        <v>8</v>
+      </c>
+      <c r="AF50">
+        <v>30</v>
+      </c>
+      <c r="AG50">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <v>17</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>19</v>
+      </c>
+      <c r="G51">
+        <v>28</v>
+      </c>
+      <c r="H51">
+        <v>13</v>
+      </c>
+      <c r="I51">
+        <v>9</v>
+      </c>
+      <c r="K51">
+        <v>16</v>
+      </c>
+      <c r="L51">
+        <v>49</v>
+      </c>
+      <c r="M51">
+        <v>10</v>
+      </c>
+      <c r="N51">
+        <v>30</v>
+      </c>
+      <c r="O51">
+        <v>9</v>
+      </c>
+      <c r="P51">
+        <v>6</v>
+      </c>
+      <c r="Q51">
+        <v>3</v>
+      </c>
+      <c r="R51">
+        <v>32</v>
+      </c>
+      <c r="S51">
+        <v>22</v>
+      </c>
+      <c r="T51">
+        <v>11</v>
+      </c>
+      <c r="U51">
+        <v>6</v>
+      </c>
+      <c r="V51">
+        <v>15</v>
+      </c>
+      <c r="W51">
+        <v>7</v>
+      </c>
+      <c r="Y51">
+        <v>36</v>
+      </c>
+      <c r="Z51">
+        <v>26</v>
+      </c>
+      <c r="AA51">
+        <v>17</v>
+      </c>
+      <c r="AB51">
+        <v>13</v>
+      </c>
+      <c r="AC51">
+        <v>23</v>
+      </c>
+      <c r="AD51">
+        <v>8</v>
+      </c>
+      <c r="AF51">
+        <v>13</v>
+      </c>
+      <c r="AG51">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52">
+        <v>40</v>
+      </c>
+      <c r="C52">
+        <v>15</v>
+      </c>
+      <c r="D52">
+        <v>44</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52">
+        <v>62</v>
+      </c>
+      <c r="G52">
+        <v>76</v>
+      </c>
+      <c r="H52">
+        <v>65</v>
+      </c>
+      <c r="I52">
+        <v>31</v>
+      </c>
+      <c r="J52">
+        <v>13</v>
+      </c>
+      <c r="K52">
+        <v>45</v>
+      </c>
+      <c r="L52">
+        <v>63</v>
+      </c>
+      <c r="M52">
+        <v>56</v>
+      </c>
+      <c r="N52">
+        <v>38</v>
+      </c>
+      <c r="O52">
+        <v>53</v>
+      </c>
+      <c r="P52">
+        <v>38</v>
+      </c>
+      <c r="Q52">
+        <v>13</v>
+      </c>
+      <c r="R52">
+        <v>76</v>
+      </c>
+      <c r="S52">
+        <v>58</v>
+      </c>
+      <c r="T52">
+        <v>89</v>
+      </c>
+      <c r="U52">
+        <v>60</v>
+      </c>
+      <c r="V52">
+        <v>37</v>
+      </c>
+      <c r="W52">
+        <v>34</v>
+      </c>
+      <c r="X52">
+        <v>10</v>
+      </c>
+      <c r="Y52">
+        <v>43</v>
+      </c>
+      <c r="Z52">
+        <v>38</v>
+      </c>
+      <c r="AA52">
+        <v>48</v>
+      </c>
+      <c r="AB52">
+        <v>47</v>
+      </c>
+      <c r="AC52">
+        <v>47</v>
+      </c>
+      <c r="AD52">
+        <v>27</v>
+      </c>
+      <c r="AE52">
+        <v>21</v>
+      </c>
+      <c r="AF52">
+        <v>56</v>
+      </c>
+      <c r="AG52">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>5</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>8</v>
+      </c>
+      <c r="G53">
+        <v>8</v>
+      </c>
+      <c r="H53">
+        <v>13</v>
+      </c>
+      <c r="I53">
+        <v>5</v>
+      </c>
+      <c r="K53">
+        <v>5</v>
+      </c>
+      <c r="L53">
+        <v>7</v>
+      </c>
+      <c r="M53">
+        <v>14</v>
+      </c>
+      <c r="N53">
+        <v>7</v>
+      </c>
+      <c r="O53">
+        <v>10</v>
+      </c>
+      <c r="P53">
+        <v>10</v>
+      </c>
+      <c r="R53">
+        <v>9</v>
+      </c>
+      <c r="S53">
+        <v>7</v>
+      </c>
+      <c r="T53">
+        <v>10</v>
+      </c>
+      <c r="U53">
+        <v>5</v>
+      </c>
+      <c r="V53">
+        <v>6</v>
+      </c>
+      <c r="W53">
+        <v>4</v>
+      </c>
+      <c r="Y53">
+        <v>10</v>
+      </c>
+      <c r="Z53">
+        <v>5</v>
+      </c>
+      <c r="AA53">
+        <v>7</v>
+      </c>
+      <c r="AB53">
+        <v>3</v>
+      </c>
+      <c r="AC53">
+        <v>11</v>
+      </c>
+      <c r="AD53">
+        <v>4</v>
+      </c>
+      <c r="AF53">
+        <v>13</v>
+      </c>
+      <c r="AG53">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>9</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54">
+        <v>23</v>
+      </c>
+      <c r="G54">
+        <v>13</v>
+      </c>
+      <c r="H54">
+        <v>21</v>
+      </c>
+      <c r="I54">
+        <v>14</v>
+      </c>
+      <c r="K54">
+        <v>22</v>
+      </c>
+      <c r="L54">
+        <v>30</v>
+      </c>
+      <c r="M54">
+        <v>10</v>
+      </c>
+      <c r="N54">
+        <v>24</v>
+      </c>
+      <c r="O54">
+        <v>24</v>
+      </c>
+      <c r="P54">
+        <v>6</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+      <c r="R54">
+        <v>26</v>
+      </c>
+      <c r="S54">
+        <v>11</v>
+      </c>
+      <c r="T54">
+        <v>28</v>
+      </c>
+      <c r="U54">
+        <v>21</v>
+      </c>
+      <c r="V54">
+        <v>24</v>
+      </c>
+      <c r="W54">
+        <v>10</v>
+      </c>
+      <c r="Y54">
+        <v>61</v>
+      </c>
+      <c r="Z54">
+        <v>16</v>
+      </c>
+      <c r="AA54">
+        <v>24</v>
+      </c>
+      <c r="AB54">
+        <v>15</v>
+      </c>
+      <c r="AC54">
+        <v>12</v>
+      </c>
+      <c r="AD54">
+        <v>3</v>
+      </c>
+      <c r="AE54">
+        <v>1</v>
+      </c>
+      <c r="AF54">
+        <v>18</v>
+      </c>
+      <c r="AG54">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <v>13</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55">
+        <v>13</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>3</v>
+      </c>
+      <c r="M55">
+        <v>15</v>
+      </c>
+      <c r="N55">
+        <v>3</v>
+      </c>
+      <c r="O55">
+        <v>5</v>
+      </c>
+      <c r="P55">
+        <v>6</v>
+      </c>
+      <c r="R55">
+        <v>4</v>
+      </c>
+      <c r="S55">
+        <v>7</v>
+      </c>
+      <c r="T55">
+        <v>3</v>
+      </c>
+      <c r="U55">
+        <v>4</v>
+      </c>
+      <c r="V55">
+        <v>13</v>
+      </c>
+      <c r="Y55">
+        <v>3</v>
+      </c>
+      <c r="Z55">
+        <v>5</v>
+      </c>
+      <c r="AA55">
+        <v>4</v>
+      </c>
+      <c r="AB55">
+        <v>1</v>
+      </c>
+      <c r="AC55">
+        <v>4</v>
+      </c>
+      <c r="AD55">
+        <v>1</v>
+      </c>
+      <c r="AF55">
+        <v>2</v>
+      </c>
+      <c r="AG55">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>9</v>
+      </c>
+      <c r="F56">
+        <v>8</v>
+      </c>
+      <c r="K56">
+        <v>8</v>
+      </c>
+      <c r="L56">
+        <v>2</v>
+      </c>
+      <c r="M56">
+        <v>14</v>
+      </c>
+      <c r="N56">
+        <v>4</v>
+      </c>
+      <c r="P56">
+        <v>3</v>
+      </c>
+      <c r="R56">
+        <v>8</v>
+      </c>
+      <c r="S56">
+        <v>1</v>
+      </c>
+      <c r="T56">
+        <v>8</v>
+      </c>
+      <c r="U56">
+        <v>1</v>
+      </c>
+      <c r="W56">
+        <v>4</v>
+      </c>
+      <c r="Y56">
+        <v>2</v>
+      </c>
+      <c r="Z56">
+        <v>2</v>
+      </c>
+      <c r="AB56">
+        <v>1</v>
+      </c>
+      <c r="AD56">
+        <v>4</v>
+      </c>
+      <c r="AE56">
+        <v>1</v>
+      </c>
+      <c r="AF56">
+        <v>8</v>
+      </c>
+      <c r="AG56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>7</v>
+      </c>
+      <c r="F57">
+        <v>11</v>
+      </c>
+      <c r="G57">
+        <v>10</v>
+      </c>
+      <c r="H57">
+        <v>8</v>
+      </c>
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="K57">
+        <v>11</v>
+      </c>
+      <c r="L57">
+        <v>5</v>
+      </c>
+      <c r="M57">
+        <v>8</v>
+      </c>
+      <c r="N57">
+        <v>12</v>
+      </c>
+      <c r="O57">
+        <v>9</v>
+      </c>
+      <c r="P57">
+        <v>2</v>
+      </c>
+      <c r="Q57">
+        <v>1</v>
+      </c>
+      <c r="R57">
+        <v>5</v>
+      </c>
+      <c r="S57">
+        <v>4</v>
+      </c>
+      <c r="T57">
+        <v>7</v>
+      </c>
+      <c r="U57">
+        <v>7</v>
+      </c>
+      <c r="V57">
+        <v>5</v>
+      </c>
+      <c r="Y57">
+        <v>12</v>
+      </c>
+      <c r="Z57">
+        <v>8</v>
+      </c>
+      <c r="AA57">
+        <v>4</v>
+      </c>
+      <c r="AB57">
+        <v>9</v>
+      </c>
+      <c r="AC57">
+        <v>6</v>
+      </c>
+      <c r="AD57">
+        <v>2</v>
+      </c>
+      <c r="AF57">
+        <v>2</v>
+      </c>
+      <c r="AG57">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236D8D1A-9F6E-4A67-B4B4-577BAEA41071}">
+  <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -28507,9 +32740,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
+    <row r="46" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -28569,12 +32802,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236D8D1A-9F6E-4A67-B4B4-577BAEA41071}">
-  <sheetPr codeName="Sheet16"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F138D5-7324-41CA-BDE7-6178B269EFE3}">
+  <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -28942,445 +33176,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F138D5-7324-41CA-BDE7-6178B269EFE3}">
-  <sheetPr codeName="Sheet18"/>
-  <dimension ref="A1:AG57"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="33" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-      <c r="Z1">
-        <v>25</v>
-      </c>
-      <c r="AA1">
-        <v>26</v>
-      </c>
-      <c r="AB1">
-        <v>27</v>
-      </c>
-      <c r="AC1">
-        <v>28</v>
-      </c>
-      <c r="AD1">
-        <v>29</v>
-      </c>
-      <c r="AE1">
-        <v>30</v>
-      </c>
-      <c r="AF1">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
+    <row r="46" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update all statistic files
</commit_message>
<xml_diff>
--- a/statistics_files/2023/2023.d.monthly_circ_by_borrower.unique_borrowers.xlsx
+++ b/statistics_files/2023/2023.d.monthly_circ_by_borrower.unique_borrowers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D567FD1F-85B8-4A12-98A1-71FAF497E054}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86345722-0127-44B5-8130-D6DAD705A641}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="719" activeTab="10" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="719" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="80">
   <si>
     <t>branchname</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>2023-11-01 - 2023-11-30</t>
+  </si>
+  <si>
+    <t>2023-12-01 - 2023-12-31</t>
   </si>
 </sst>
 </file>
@@ -655,7 +658,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -9643,7 +9646,7 @@
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -14036,87 +14039,935 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
+      <c r="B2" s="1">
+        <v>45261</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45262</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45263</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45264</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45265</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45266</v>
+      </c>
+      <c r="H2" s="1">
+        <v>45267</v>
+      </c>
+      <c r="I2" s="1">
+        <v>45268</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45269</v>
+      </c>
+      <c r="K2" s="1">
+        <v>45270</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45271</v>
+      </c>
+      <c r="M2" s="1">
+        <v>45272</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45273</v>
+      </c>
+      <c r="O2" s="1">
+        <v>45274</v>
+      </c>
+      <c r="P2" s="1">
+        <v>45275</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>45276</v>
+      </c>
+      <c r="R2" s="1">
+        <v>45277</v>
+      </c>
+      <c r="S2" s="1">
+        <v>45278</v>
+      </c>
+      <c r="T2" s="1">
+        <v>45279</v>
+      </c>
+      <c r="U2" s="1">
+        <v>45280</v>
+      </c>
+      <c r="V2" s="1">
+        <v>45281</v>
+      </c>
+      <c r="W2" s="1">
+        <v>45282</v>
+      </c>
+      <c r="X2" s="1">
+        <v>45283</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>45284</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>45285</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>45286</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>45287</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>45288</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>45289</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>45290</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>45291</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T3" t="s">
+        <v>61</v>
+      </c>
+      <c r="U3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W3" t="s">
+        <v>64</v>
+      </c>
+      <c r="X3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>56</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>61</v>
+      </c>
+      <c r="F4">
+        <v>46</v>
+      </c>
+      <c r="G4">
+        <v>49</v>
+      </c>
+      <c r="H4">
+        <v>58</v>
+      </c>
+      <c r="I4">
+        <v>39</v>
+      </c>
+      <c r="J4">
+        <v>31</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>43</v>
+      </c>
+      <c r="M4">
+        <v>56</v>
+      </c>
+      <c r="N4">
+        <v>63</v>
+      </c>
+      <c r="O4">
+        <v>49</v>
+      </c>
+      <c r="P4">
+        <v>51</v>
+      </c>
+      <c r="Q4">
+        <v>24</v>
+      </c>
+      <c r="R4">
+        <v>6</v>
+      </c>
+      <c r="S4">
+        <v>73</v>
+      </c>
+      <c r="T4">
+        <v>48</v>
+      </c>
+      <c r="U4">
+        <v>58</v>
+      </c>
+      <c r="V4">
+        <v>61</v>
+      </c>
+      <c r="W4">
+        <v>51</v>
+      </c>
+      <c r="X4">
+        <v>35</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+      <c r="AA4">
+        <v>43</v>
+      </c>
+      <c r="AB4">
+        <v>48</v>
+      </c>
+      <c r="AC4">
+        <v>56</v>
+      </c>
+      <c r="AD4">
+        <v>55</v>
+      </c>
+      <c r="AE4">
+        <v>29</v>
+      </c>
+      <c r="AF4">
+        <v>4</v>
+      </c>
+      <c r="AG4">
+        <v>556</v>
+      </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>38</v>
+      </c>
+      <c r="I5">
+        <v>27</v>
+      </c>
+      <c r="J5">
+        <v>21</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>37</v>
+      </c>
+      <c r="M5">
+        <v>28</v>
+      </c>
+      <c r="N5">
+        <v>35</v>
+      </c>
+      <c r="O5">
+        <v>28</v>
+      </c>
+      <c r="P5">
+        <v>20</v>
+      </c>
+      <c r="Q5">
+        <v>11</v>
+      </c>
+      <c r="S5">
+        <v>35</v>
+      </c>
+      <c r="T5">
+        <v>38</v>
+      </c>
+      <c r="U5">
+        <v>28</v>
+      </c>
+      <c r="V5">
+        <v>40</v>
+      </c>
+      <c r="W5">
+        <v>31</v>
+      </c>
+      <c r="X5">
+        <v>15</v>
+      </c>
+      <c r="Y5">
+        <v>4</v>
+      </c>
+      <c r="Z5">
+        <v>3</v>
+      </c>
+      <c r="AA5">
+        <v>6</v>
+      </c>
+      <c r="AB5">
+        <v>49</v>
+      </c>
+      <c r="AC5">
+        <v>27</v>
+      </c>
+      <c r="AD5">
+        <v>35</v>
+      </c>
+      <c r="AE5">
+        <v>21</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>303</v>
+      </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
+      </c>
+      <c r="B6">
+        <v>62</v>
+      </c>
+      <c r="C6">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>43</v>
+      </c>
+      <c r="E6">
+        <v>93</v>
+      </c>
+      <c r="F6">
+        <v>74</v>
+      </c>
+      <c r="G6">
+        <v>77</v>
+      </c>
+      <c r="H6">
+        <v>63</v>
+      </c>
+      <c r="I6">
+        <v>48</v>
+      </c>
+      <c r="J6">
+        <v>54</v>
+      </c>
+      <c r="K6">
+        <v>44</v>
+      </c>
+      <c r="L6">
+        <v>81</v>
+      </c>
+      <c r="M6">
+        <v>68</v>
+      </c>
+      <c r="N6">
+        <v>79</v>
+      </c>
+      <c r="O6">
+        <v>75</v>
+      </c>
+      <c r="P6">
+        <v>60</v>
+      </c>
+      <c r="Q6">
+        <v>69</v>
+      </c>
+      <c r="R6">
+        <v>43</v>
+      </c>
+      <c r="S6">
+        <v>75</v>
+      </c>
+      <c r="T6">
+        <v>81</v>
+      </c>
+      <c r="U6">
+        <v>79</v>
+      </c>
+      <c r="V6">
+        <v>72</v>
+      </c>
+      <c r="W6">
+        <v>51</v>
+      </c>
+      <c r="X6">
+        <v>53</v>
+      </c>
+      <c r="Y6">
+        <v>4</v>
+      </c>
+      <c r="Z6">
+        <v>4</v>
+      </c>
+      <c r="AA6">
+        <v>61</v>
+      </c>
+      <c r="AB6">
+        <v>81</v>
+      </c>
+      <c r="AC6">
+        <v>80</v>
+      </c>
+      <c r="AD6">
+        <v>53</v>
+      </c>
+      <c r="AE6">
+        <v>57</v>
+      </c>
+      <c r="AF6">
+        <v>8</v>
+      </c>
+      <c r="AG6">
+        <v>832</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="AB7">
+        <v>2</v>
+      </c>
+      <c r="AC7">
+        <v>3</v>
+      </c>
+      <c r="AD7">
+        <v>1</v>
+      </c>
+      <c r="AE7">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>59</v>
+      </c>
+      <c r="G8">
+        <v>64</v>
+      </c>
+      <c r="H8">
+        <v>43</v>
+      </c>
+      <c r="I8">
+        <v>36</v>
+      </c>
+      <c r="J8">
+        <v>35</v>
+      </c>
+      <c r="K8">
+        <v>26</v>
+      </c>
+      <c r="L8">
+        <v>67</v>
+      </c>
+      <c r="M8">
+        <v>53</v>
+      </c>
+      <c r="N8">
+        <v>57</v>
+      </c>
+      <c r="O8">
+        <v>54</v>
+      </c>
+      <c r="P8">
+        <v>38</v>
+      </c>
+      <c r="Q8">
+        <v>31</v>
+      </c>
+      <c r="R8">
+        <v>25</v>
+      </c>
+      <c r="S8">
+        <v>65</v>
+      </c>
+      <c r="T8">
+        <v>59</v>
+      </c>
+      <c r="U8">
+        <v>68</v>
+      </c>
+      <c r="V8">
+        <v>58</v>
+      </c>
+      <c r="W8">
+        <v>58</v>
+      </c>
+      <c r="X8">
+        <v>38</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
+        <v>5</v>
+      </c>
+      <c r="AA8">
+        <v>8</v>
+      </c>
+      <c r="AB8">
+        <v>61</v>
+      </c>
+      <c r="AC8">
+        <v>62</v>
+      </c>
+      <c r="AD8">
+        <v>52</v>
+      </c>
+      <c r="AE8">
+        <v>46</v>
+      </c>
+      <c r="AF8">
+        <v>19</v>
+      </c>
+      <c r="AG8">
+        <v>624</v>
+      </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+      <c r="N9">
+        <v>12</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>5</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>11</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9">
+        <v>8</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>8</v>
+      </c>
+      <c r="AC9">
+        <v>7</v>
+      </c>
+      <c r="AD9">
+        <v>6</v>
+      </c>
+      <c r="AE9">
+        <v>3</v>
+      </c>
+      <c r="AG9">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>14</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>6</v>
+      </c>
+      <c r="O10">
+        <v>11</v>
+      </c>
+      <c r="P10">
+        <v>5</v>
+      </c>
+      <c r="Q10">
+        <v>9</v>
+      </c>
+      <c r="S10">
+        <v>7</v>
+      </c>
+      <c r="T10">
+        <v>13</v>
+      </c>
+      <c r="U10">
+        <v>10</v>
+      </c>
+      <c r="V10">
+        <v>12</v>
+      </c>
+      <c r="W10">
+        <v>11</v>
+      </c>
+      <c r="AA10">
+        <v>5</v>
+      </c>
+      <c r="AB10">
+        <v>6</v>
+      </c>
+      <c r="AC10">
+        <v>8</v>
+      </c>
+      <c r="AD10">
+        <v>15</v>
+      </c>
+      <c r="AE10">
+        <v>9</v>
+      </c>
+      <c r="AG10">
+        <v>93</v>
+      </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>8</v>
+      </c>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="S11">
+        <v>3</v>
+      </c>
+      <c r="U11">
+        <v>16</v>
+      </c>
+      <c r="V11">
+        <v>8</v>
+      </c>
+      <c r="W11">
+        <v>14</v>
+      </c>
+      <c r="AB11">
+        <v>5</v>
+      </c>
+      <c r="AC11">
+        <v>4</v>
+      </c>
+      <c r="AD11">
+        <v>15</v>
+      </c>
+      <c r="AE11">
+        <v>3</v>
+      </c>
+      <c r="AG11">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>4</v>
+      </c>
+      <c r="W12">
+        <v>2</v>
+      </c>
+      <c r="AB12">
+        <v>1</v>
+      </c>
+      <c r="AG12">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -14127,220 +14978,3265 @@
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>3</v>
+      </c>
+      <c r="T14">
+        <v>2</v>
+      </c>
+      <c r="U14">
+        <v>2</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="AB14">
+        <v>2</v>
+      </c>
+      <c r="AC14">
+        <v>3</v>
+      </c>
+      <c r="AD14">
+        <v>1</v>
+      </c>
+      <c r="AG14">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>9</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>5</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>7</v>
+      </c>
+      <c r="N15">
+        <v>10</v>
+      </c>
+      <c r="O15">
+        <v>6</v>
+      </c>
+      <c r="P15">
+        <v>3</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="T15">
+        <v>6</v>
+      </c>
+      <c r="U15">
+        <v>5</v>
+      </c>
+      <c r="V15">
+        <v>5</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>3</v>
+      </c>
+      <c r="AB15">
+        <v>6</v>
+      </c>
+      <c r="AC15">
+        <v>6</v>
+      </c>
+      <c r="AD15">
+        <v>10</v>
+      </c>
+      <c r="AG15">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>17</v>
+      </c>
+      <c r="I16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="N16">
+        <v>15</v>
+      </c>
+      <c r="O16">
+        <v>12</v>
+      </c>
+      <c r="P16">
+        <v>7</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>14</v>
+      </c>
+      <c r="T16">
+        <v>9</v>
+      </c>
+      <c r="U16">
+        <v>11</v>
+      </c>
+      <c r="V16">
+        <v>23</v>
+      </c>
+      <c r="AA16">
+        <v>11</v>
+      </c>
+      <c r="AB16">
+        <v>5</v>
+      </c>
+      <c r="AC16">
+        <v>8</v>
+      </c>
+      <c r="AD16">
+        <v>19</v>
+      </c>
+      <c r="AE16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+      <c r="N17">
+        <v>10</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+      <c r="P17">
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="S17">
+        <v>3</v>
+      </c>
+      <c r="U17">
+        <v>2</v>
+      </c>
+      <c r="V17">
+        <v>7</v>
+      </c>
+      <c r="AA17">
+        <v>6</v>
+      </c>
+      <c r="AB17">
+        <v>5</v>
+      </c>
+      <c r="AC17">
+        <v>6</v>
+      </c>
+      <c r="AD17">
+        <v>5</v>
+      </c>
+      <c r="AG17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>9</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
+      <c r="T18">
+        <v>4</v>
+      </c>
+      <c r="U18">
+        <v>12</v>
+      </c>
+      <c r="V18">
+        <v>5</v>
+      </c>
+      <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
+        <v>2</v>
+      </c>
+      <c r="AB18">
+        <v>5</v>
+      </c>
+      <c r="AC18">
+        <v>2</v>
+      </c>
+      <c r="AD18">
+        <v>1</v>
+      </c>
+      <c r="AE18">
+        <v>7</v>
+      </c>
+      <c r="AG18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>28</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <v>13</v>
+      </c>
+      <c r="I19">
+        <v>13</v>
+      </c>
+      <c r="J19">
+        <v>16</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>31</v>
+      </c>
+      <c r="M19">
+        <v>24</v>
+      </c>
+      <c r="N19">
+        <v>19</v>
+      </c>
+      <c r="O19">
+        <v>19</v>
+      </c>
+      <c r="P19">
+        <v>18</v>
+      </c>
+      <c r="Q19">
+        <v>13</v>
+      </c>
+      <c r="S19">
+        <v>30</v>
+      </c>
+      <c r="T19">
+        <v>23</v>
+      </c>
+      <c r="U19">
+        <v>31</v>
+      </c>
+      <c r="V19">
+        <v>21</v>
+      </c>
+      <c r="W19">
+        <v>23</v>
+      </c>
+      <c r="X19">
+        <v>10</v>
+      </c>
+      <c r="Y19">
+        <v>3</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>3</v>
+      </c>
+      <c r="AB19">
+        <v>37</v>
+      </c>
+      <c r="AC19">
+        <v>24</v>
+      </c>
+      <c r="AD19">
+        <v>19</v>
+      </c>
+      <c r="AE19">
+        <v>21</v>
+      </c>
+      <c r="AF19">
+        <v>2</v>
+      </c>
+      <c r="AG19">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="T20">
+        <v>3</v>
+      </c>
+      <c r="U20">
+        <v>4</v>
+      </c>
+      <c r="V20">
+        <v>3</v>
+      </c>
+      <c r="W20">
+        <v>3</v>
+      </c>
+      <c r="X20">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>1</v>
+      </c>
+      <c r="AC20">
+        <v>2</v>
+      </c>
+      <c r="AD20">
+        <v>2</v>
+      </c>
+      <c r="AE20">
+        <v>2</v>
+      </c>
+      <c r="AG20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <v>34</v>
+      </c>
+      <c r="F21">
+        <v>22</v>
+      </c>
+      <c r="G21">
+        <v>21</v>
+      </c>
+      <c r="H21">
+        <v>23</v>
+      </c>
+      <c r="I21">
+        <v>19</v>
+      </c>
+      <c r="J21">
+        <v>14</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>30</v>
+      </c>
+      <c r="M21">
+        <v>30</v>
+      </c>
+      <c r="N21">
+        <v>24</v>
+      </c>
+      <c r="O21">
+        <v>24</v>
+      </c>
+      <c r="P21">
+        <v>13</v>
+      </c>
+      <c r="Q21">
+        <v>14</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>31</v>
+      </c>
+      <c r="T21">
+        <v>37</v>
+      </c>
+      <c r="U21">
+        <v>4</v>
+      </c>
+      <c r="V21">
+        <v>40</v>
+      </c>
+      <c r="W21">
+        <v>26</v>
+      </c>
+      <c r="X21">
+        <v>10</v>
+      </c>
+      <c r="AA21">
+        <v>17</v>
+      </c>
+      <c r="AB21">
+        <v>23</v>
+      </c>
+      <c r="AC21">
+        <v>31</v>
+      </c>
+      <c r="AD21">
+        <v>23</v>
+      </c>
+      <c r="AE21">
+        <v>14</v>
+      </c>
+      <c r="AF21">
+        <v>3</v>
+      </c>
+      <c r="AG21">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="AG22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>30</v>
+      </c>
+      <c r="F23">
+        <v>37</v>
+      </c>
+      <c r="G23">
+        <v>32</v>
+      </c>
+      <c r="H23">
+        <v>26</v>
+      </c>
+      <c r="I23">
+        <v>16</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="L23">
+        <v>34</v>
+      </c>
+      <c r="M23">
+        <v>24</v>
+      </c>
+      <c r="N23">
+        <v>27</v>
+      </c>
+      <c r="O23">
+        <v>26</v>
+      </c>
+      <c r="P23">
+        <v>24</v>
+      </c>
+      <c r="Q23">
+        <v>10</v>
+      </c>
+      <c r="S23">
+        <v>30</v>
+      </c>
+      <c r="T23">
+        <v>36</v>
+      </c>
+      <c r="U23">
+        <v>28</v>
+      </c>
+      <c r="V23">
+        <v>26</v>
+      </c>
+      <c r="W23">
+        <v>46</v>
+      </c>
+      <c r="AA23">
+        <v>18</v>
+      </c>
+      <c r="AB23">
+        <v>15</v>
+      </c>
+      <c r="AC23">
+        <v>24</v>
+      </c>
+      <c r="AD23">
+        <v>31</v>
+      </c>
+      <c r="AE23">
+        <v>1</v>
+      </c>
+      <c r="AG23">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>7</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>4</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+      <c r="S24">
+        <v>2</v>
+      </c>
+      <c r="T24">
+        <v>4</v>
+      </c>
+      <c r="U24">
+        <v>12</v>
+      </c>
+      <c r="W24">
+        <v>5</v>
+      </c>
+      <c r="AA24">
+        <v>2</v>
+      </c>
+      <c r="AB24">
+        <v>7</v>
+      </c>
+      <c r="AC24">
+        <v>8</v>
+      </c>
+      <c r="AD24">
+        <v>3</v>
+      </c>
+      <c r="AE24">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>33</v>
+      </c>
+      <c r="C25">
+        <v>17</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>28</v>
+      </c>
+      <c r="F25">
+        <v>35</v>
+      </c>
+      <c r="G25">
+        <v>25</v>
+      </c>
+      <c r="H25">
+        <v>24</v>
+      </c>
+      <c r="I25">
+        <v>26</v>
+      </c>
+      <c r="J25">
+        <v>25</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>28</v>
+      </c>
+      <c r="M25">
+        <v>26</v>
+      </c>
+      <c r="N25">
+        <v>29</v>
+      </c>
+      <c r="O25">
+        <v>39</v>
+      </c>
+      <c r="P25">
+        <v>25</v>
+      </c>
+      <c r="Q25">
+        <v>25</v>
+      </c>
+      <c r="R25">
+        <v>5</v>
+      </c>
+      <c r="S25">
+        <v>48</v>
+      </c>
+      <c r="T25">
+        <v>35</v>
+      </c>
+      <c r="U25">
+        <v>31</v>
+      </c>
+      <c r="V25">
+        <v>36</v>
+      </c>
+      <c r="W25">
+        <v>37</v>
+      </c>
+      <c r="X25">
+        <v>5</v>
+      </c>
+      <c r="Y25">
+        <v>3</v>
+      </c>
+      <c r="Z25">
+        <v>2</v>
+      </c>
+      <c r="AA25">
+        <v>21</v>
+      </c>
+      <c r="AB25">
+        <v>30</v>
+      </c>
+      <c r="AC25">
+        <v>36</v>
+      </c>
+      <c r="AD25">
+        <v>29</v>
+      </c>
+      <c r="AE25">
+        <v>16</v>
+      </c>
+      <c r="AF25">
+        <v>6</v>
+      </c>
+      <c r="AG25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>82</v>
+      </c>
+      <c r="C26">
+        <v>73</v>
+      </c>
+      <c r="D26">
+        <v>53</v>
+      </c>
+      <c r="E26">
+        <v>79</v>
+      </c>
+      <c r="F26">
+        <v>103</v>
+      </c>
+      <c r="G26">
+        <v>104</v>
+      </c>
+      <c r="H26">
+        <v>93</v>
+      </c>
+      <c r="I26">
+        <v>84</v>
+      </c>
+      <c r="J26">
+        <v>94</v>
+      </c>
+      <c r="K26">
+        <v>33</v>
+      </c>
+      <c r="L26">
+        <v>90</v>
+      </c>
+      <c r="M26">
+        <v>96</v>
+      </c>
+      <c r="N26">
+        <v>97</v>
+      </c>
+      <c r="O26">
+        <v>86</v>
+      </c>
+      <c r="P26">
+        <v>83</v>
+      </c>
+      <c r="Q26">
+        <v>73</v>
+      </c>
+      <c r="R26">
+        <v>30</v>
+      </c>
+      <c r="S26">
+        <v>87</v>
+      </c>
+      <c r="T26">
+        <v>87</v>
+      </c>
+      <c r="U26">
+        <v>73</v>
+      </c>
+      <c r="V26">
+        <v>97</v>
+      </c>
+      <c r="W26">
+        <v>90</v>
+      </c>
+      <c r="X26">
+        <v>12</v>
+      </c>
+      <c r="Y26">
+        <v>9</v>
+      </c>
+      <c r="Z26">
+        <v>6</v>
+      </c>
+      <c r="AA26">
+        <v>98</v>
+      </c>
+      <c r="AB26">
+        <v>94</v>
+      </c>
+      <c r="AC26">
+        <v>116</v>
+      </c>
+      <c r="AD26">
+        <v>82</v>
+      </c>
+      <c r="AE26">
+        <v>68</v>
+      </c>
+      <c r="AF26">
+        <v>18</v>
+      </c>
+      <c r="AG26">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>8</v>
+      </c>
+      <c r="J27">
+        <v>6</v>
+      </c>
+      <c r="L27">
+        <v>9</v>
+      </c>
+      <c r="M27">
+        <v>14</v>
+      </c>
+      <c r="N27">
+        <v>9</v>
+      </c>
+      <c r="O27">
+        <v>7</v>
+      </c>
+      <c r="P27">
+        <v>11</v>
+      </c>
+      <c r="Q27">
+        <v>12</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+      <c r="T27">
+        <v>12</v>
+      </c>
+      <c r="U27">
+        <v>6</v>
+      </c>
+      <c r="V27">
+        <v>8</v>
+      </c>
+      <c r="W27">
+        <v>15</v>
+      </c>
+      <c r="X27">
+        <v>2</v>
+      </c>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>9</v>
+      </c>
+      <c r="AB27">
+        <v>13</v>
+      </c>
+      <c r="AC27">
+        <v>5</v>
+      </c>
+      <c r="AD27">
+        <v>13</v>
+      </c>
+      <c r="AE27">
+        <v>6</v>
+      </c>
+      <c r="AG27">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>5</v>
+      </c>
+      <c r="J29">
+        <v>8</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <v>12</v>
+      </c>
+      <c r="M29">
+        <v>7</v>
+      </c>
+      <c r="N29">
+        <v>8</v>
+      </c>
+      <c r="O29">
+        <v>6</v>
+      </c>
+      <c r="Q29">
+        <v>5</v>
+      </c>
+      <c r="S29">
+        <v>15</v>
+      </c>
+      <c r="T29">
+        <v>8</v>
+      </c>
+      <c r="U29">
+        <v>15</v>
+      </c>
+      <c r="V29">
+        <v>5</v>
+      </c>
+      <c r="W29">
+        <v>1</v>
+      </c>
+      <c r="Z29">
+        <v>1</v>
+      </c>
+      <c r="AA29">
+        <v>9</v>
+      </c>
+      <c r="AB29">
+        <v>10</v>
+      </c>
+      <c r="AC29">
+        <v>9</v>
+      </c>
+      <c r="AD29">
+        <v>2</v>
+      </c>
+      <c r="AE29">
+        <v>11</v>
+      </c>
+      <c r="AF29">
+        <v>1</v>
+      </c>
+      <c r="AG29">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>3</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>7</v>
+      </c>
+      <c r="P30">
+        <v>2</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>8</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <v>2</v>
+      </c>
+      <c r="W30">
+        <v>2</v>
+      </c>
+      <c r="AA30">
+        <v>2</v>
+      </c>
+      <c r="AB30">
+        <v>3</v>
+      </c>
+      <c r="AC30">
+        <v>1</v>
+      </c>
+      <c r="AD30">
+        <v>4</v>
+      </c>
+      <c r="AG30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31">
+        <v>22</v>
+      </c>
+      <c r="G31">
+        <v>26</v>
+      </c>
+      <c r="H31">
+        <v>11</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>19</v>
+      </c>
+      <c r="M31">
+        <v>21</v>
+      </c>
+      <c r="N31">
+        <v>17</v>
+      </c>
+      <c r="O31">
+        <v>9</v>
+      </c>
+      <c r="P31">
+        <v>17</v>
+      </c>
+      <c r="Q31">
+        <v>5</v>
+      </c>
+      <c r="S31">
+        <v>17</v>
+      </c>
+      <c r="T31">
+        <v>13</v>
+      </c>
+      <c r="U31">
+        <v>14</v>
+      </c>
+      <c r="V31">
+        <v>15</v>
+      </c>
+      <c r="W31">
+        <v>8</v>
+      </c>
+      <c r="X31">
+        <v>2</v>
+      </c>
+      <c r="Y31">
+        <v>1</v>
+      </c>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+      <c r="AA31">
+        <v>2</v>
+      </c>
+      <c r="AB31">
+        <v>20</v>
+      </c>
+      <c r="AC31">
+        <v>17</v>
+      </c>
+      <c r="AD31">
+        <v>21</v>
+      </c>
+      <c r="AE31">
+        <v>5</v>
+      </c>
+      <c r="AG31">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>2</v>
+      </c>
+      <c r="M32">
+        <v>2</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>2</v>
+      </c>
+      <c r="P32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>2</v>
+      </c>
+      <c r="T32">
+        <v>2</v>
+      </c>
+      <c r="U32">
+        <v>1</v>
+      </c>
+      <c r="AA32">
+        <v>2</v>
+      </c>
+      <c r="AB32">
+        <v>2</v>
+      </c>
+      <c r="AD32">
+        <v>1</v>
+      </c>
+      <c r="AG32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>9</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>6</v>
+      </c>
+      <c r="H33">
+        <v>6</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>5</v>
+      </c>
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33">
+        <v>3</v>
+      </c>
+      <c r="P33">
+        <v>5</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>5</v>
+      </c>
+      <c r="U33">
+        <v>6</v>
+      </c>
+      <c r="V33">
+        <v>7</v>
+      </c>
+      <c r="W33">
+        <v>5</v>
+      </c>
+      <c r="X33">
+        <v>1</v>
+      </c>
+      <c r="AA33">
+        <v>3</v>
+      </c>
+      <c r="AB33">
+        <v>4</v>
+      </c>
+      <c r="AC33">
+        <v>4</v>
+      </c>
+      <c r="AD33">
+        <v>4</v>
+      </c>
+      <c r="AE33">
+        <v>2</v>
+      </c>
+      <c r="AF33">
+        <v>1</v>
+      </c>
+      <c r="AG33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>31</v>
+      </c>
+      <c r="C34">
+        <v>13</v>
+      </c>
+      <c r="E34">
+        <v>34</v>
+      </c>
+      <c r="F34">
+        <v>35</v>
+      </c>
+      <c r="G34">
+        <v>22</v>
+      </c>
+      <c r="H34">
+        <v>24</v>
+      </c>
+      <c r="I34">
+        <v>21</v>
+      </c>
+      <c r="J34">
+        <v>22</v>
+      </c>
+      <c r="L34">
+        <v>25</v>
+      </c>
+      <c r="M34">
+        <v>37</v>
+      </c>
+      <c r="N34">
+        <v>24</v>
+      </c>
+      <c r="O34">
+        <v>32</v>
+      </c>
+      <c r="P34">
+        <v>22</v>
+      </c>
+      <c r="Q34">
+        <v>12</v>
+      </c>
+      <c r="S34">
+        <v>23</v>
+      </c>
+      <c r="T34">
+        <v>30</v>
+      </c>
+      <c r="U34">
+        <v>40</v>
+      </c>
+      <c r="V34">
+        <v>29</v>
+      </c>
+      <c r="W34">
+        <v>20</v>
+      </c>
+      <c r="X34">
+        <v>14</v>
+      </c>
+      <c r="AB34">
+        <v>39</v>
+      </c>
+      <c r="AC34">
+        <v>36</v>
+      </c>
+      <c r="AD34">
+        <v>27</v>
+      </c>
+      <c r="AE34">
+        <v>11</v>
+      </c>
+      <c r="AG34">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>17</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>23</v>
+      </c>
+      <c r="F35">
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>15</v>
+      </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
+      <c r="J35">
+        <v>14</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>21</v>
+      </c>
+      <c r="M35">
+        <v>17</v>
+      </c>
+      <c r="N35">
+        <v>17</v>
+      </c>
+      <c r="O35">
+        <v>12</v>
+      </c>
+      <c r="P35">
+        <v>14</v>
+      </c>
+      <c r="Q35">
+        <v>16</v>
+      </c>
+      <c r="S35">
+        <v>33</v>
+      </c>
+      <c r="T35">
+        <v>14</v>
+      </c>
+      <c r="U35">
+        <v>19</v>
+      </c>
+      <c r="V35">
+        <v>15</v>
+      </c>
+      <c r="W35">
+        <v>29</v>
+      </c>
+      <c r="Y35">
+        <v>1</v>
+      </c>
+      <c r="Z35">
+        <v>1</v>
+      </c>
+      <c r="AA35">
+        <v>18</v>
+      </c>
+      <c r="AB35">
+        <v>11</v>
+      </c>
+      <c r="AC35">
+        <v>24</v>
+      </c>
+      <c r="AD35">
+        <v>13</v>
+      </c>
+      <c r="AE35">
+        <v>17</v>
+      </c>
+      <c r="AG35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>15</v>
+      </c>
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="F36">
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <v>12</v>
+      </c>
+      <c r="H36">
+        <v>10</v>
+      </c>
+      <c r="I36">
+        <v>10</v>
+      </c>
+      <c r="J36">
+        <v>11</v>
+      </c>
+      <c r="L36">
+        <v>12</v>
+      </c>
+      <c r="M36">
+        <v>9</v>
+      </c>
+      <c r="N36">
+        <v>13</v>
+      </c>
+      <c r="O36">
+        <v>7</v>
+      </c>
+      <c r="P36">
+        <v>9</v>
+      </c>
+      <c r="Q36">
+        <v>15</v>
+      </c>
+      <c r="S36">
+        <v>12</v>
+      </c>
+      <c r="T36">
+        <v>15</v>
+      </c>
+      <c r="U36">
+        <v>16</v>
+      </c>
+      <c r="V36">
+        <v>15</v>
+      </c>
+      <c r="W36">
+        <v>18</v>
+      </c>
+      <c r="X36">
+        <v>8</v>
+      </c>
+      <c r="AA36">
+        <v>12</v>
+      </c>
+      <c r="AB36">
+        <v>11</v>
+      </c>
+      <c r="AC36">
+        <v>12</v>
+      </c>
+      <c r="AD36">
+        <v>15</v>
+      </c>
+      <c r="AE36">
+        <v>4</v>
+      </c>
+      <c r="AF36">
+        <v>1</v>
+      </c>
+      <c r="AG36">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>67</v>
+      </c>
+      <c r="C37">
+        <v>32</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>79</v>
+      </c>
+      <c r="F37">
+        <v>56</v>
+      </c>
+      <c r="G37">
+        <v>58</v>
+      </c>
+      <c r="H37">
+        <v>58</v>
+      </c>
+      <c r="I37">
+        <v>55</v>
+      </c>
+      <c r="J37">
+        <v>31</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>97</v>
+      </c>
+      <c r="M37">
+        <v>79</v>
+      </c>
+      <c r="N37">
+        <v>36</v>
+      </c>
+      <c r="O37">
+        <v>52</v>
+      </c>
+      <c r="P37">
+        <v>64</v>
+      </c>
+      <c r="Q37">
+        <v>28</v>
+      </c>
+      <c r="R37">
+        <v>3</v>
+      </c>
+      <c r="S37">
+        <v>69</v>
+      </c>
+      <c r="T37">
+        <v>76</v>
+      </c>
+      <c r="U37">
+        <v>74</v>
+      </c>
+      <c r="V37">
+        <v>79</v>
+      </c>
+      <c r="W37">
+        <v>58</v>
+      </c>
+      <c r="X37">
+        <v>23</v>
+      </c>
+      <c r="Y37">
+        <v>4</v>
+      </c>
+      <c r="Z37">
+        <v>2</v>
+      </c>
+      <c r="AA37">
+        <v>8</v>
+      </c>
+      <c r="AB37">
+        <v>68</v>
+      </c>
+      <c r="AC37">
+        <v>74</v>
+      </c>
+      <c r="AD37">
+        <v>72</v>
+      </c>
+      <c r="AE37">
+        <v>27</v>
+      </c>
+      <c r="AF37">
+        <v>2</v>
+      </c>
+      <c r="AG37">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="E38">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>16</v>
+      </c>
+      <c r="G38">
+        <v>11</v>
+      </c>
+      <c r="H38">
+        <v>10</v>
+      </c>
+      <c r="I38">
+        <v>8</v>
+      </c>
+      <c r="J38">
+        <v>11</v>
+      </c>
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>14</v>
+      </c>
+      <c r="M38">
+        <v>6</v>
+      </c>
+      <c r="N38">
+        <v>5</v>
+      </c>
+      <c r="O38">
+        <v>12</v>
+      </c>
+      <c r="P38">
+        <v>9</v>
+      </c>
+      <c r="Q38">
+        <v>8</v>
+      </c>
+      <c r="S38">
+        <v>20</v>
+      </c>
+      <c r="T38">
+        <v>15</v>
+      </c>
+      <c r="U38">
+        <v>12</v>
+      </c>
+      <c r="V38">
+        <v>16</v>
+      </c>
+      <c r="W38">
+        <v>21</v>
+      </c>
+      <c r="AA38">
+        <v>13</v>
+      </c>
+      <c r="AB38">
+        <v>13</v>
+      </c>
+      <c r="AC38">
+        <v>9</v>
+      </c>
+      <c r="AD38">
+        <v>20</v>
+      </c>
+      <c r="AE38">
+        <v>3</v>
+      </c>
+      <c r="AG38">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>31</v>
+      </c>
+      <c r="C39">
+        <v>26</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>69</v>
+      </c>
+      <c r="F39">
+        <v>50</v>
+      </c>
+      <c r="G39">
+        <v>52</v>
+      </c>
+      <c r="H39">
+        <v>52</v>
+      </c>
+      <c r="I39">
+        <v>38</v>
+      </c>
+      <c r="J39">
+        <v>45</v>
+      </c>
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <v>61</v>
+      </c>
+      <c r="M39">
+        <v>45</v>
+      </c>
+      <c r="N39">
+        <v>44</v>
+      </c>
+      <c r="O39">
+        <v>43</v>
+      </c>
+      <c r="P39">
+        <v>38</v>
+      </c>
+      <c r="Q39">
+        <v>30</v>
+      </c>
+      <c r="R39">
+        <v>4</v>
+      </c>
+      <c r="S39">
+        <v>71</v>
+      </c>
+      <c r="T39">
+        <v>57</v>
+      </c>
+      <c r="U39">
+        <v>60</v>
+      </c>
+      <c r="V39">
+        <v>58</v>
+      </c>
+      <c r="W39">
+        <v>46</v>
+      </c>
+      <c r="X39">
+        <v>1</v>
+      </c>
+      <c r="Y39">
+        <v>2</v>
+      </c>
+      <c r="Z39">
+        <v>3</v>
+      </c>
+      <c r="AA39">
+        <v>53</v>
+      </c>
+      <c r="AB39">
+        <v>64</v>
+      </c>
+      <c r="AC39">
+        <v>50</v>
+      </c>
+      <c r="AD39">
+        <v>50</v>
+      </c>
+      <c r="AE39">
+        <v>37</v>
+      </c>
+      <c r="AF39">
+        <v>3</v>
+      </c>
+      <c r="AG39">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>2</v>
+      </c>
+      <c r="Q40">
+        <v>2</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+      <c r="V40">
+        <v>2</v>
+      </c>
+      <c r="X40">
+        <v>2</v>
+      </c>
+      <c r="Z40">
+        <v>2</v>
+      </c>
+      <c r="AC40">
+        <v>3</v>
+      </c>
+      <c r="AG40">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <v>9</v>
+      </c>
+      <c r="N41">
+        <v>3</v>
+      </c>
+      <c r="O41">
+        <v>2</v>
+      </c>
+      <c r="P41">
+        <v>2</v>
+      </c>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41">
+        <v>5</v>
+      </c>
+      <c r="V41">
+        <v>5</v>
+      </c>
+      <c r="W41">
+        <v>1</v>
+      </c>
+      <c r="AG41">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>11</v>
+      </c>
+      <c r="E42">
+        <v>6</v>
+      </c>
+      <c r="F42">
+        <v>23</v>
+      </c>
+      <c r="G42">
+        <v>19</v>
+      </c>
+      <c r="H42">
+        <v>14</v>
+      </c>
+      <c r="I42">
+        <v>12</v>
+      </c>
+      <c r="L42">
+        <v>14</v>
+      </c>
+      <c r="M42">
+        <v>7</v>
+      </c>
+      <c r="N42">
+        <v>5</v>
+      </c>
+      <c r="O42">
+        <v>12</v>
+      </c>
+      <c r="P42">
+        <v>7</v>
+      </c>
+      <c r="S42">
+        <v>9</v>
+      </c>
+      <c r="T42">
+        <v>12</v>
+      </c>
+      <c r="U42">
+        <v>16</v>
+      </c>
+      <c r="AG42">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>64</v>
+      </c>
+      <c r="F43">
+        <v>71</v>
+      </c>
+      <c r="G43">
+        <v>50</v>
+      </c>
+      <c r="H43">
+        <v>49</v>
+      </c>
+      <c r="I43">
+        <v>41</v>
+      </c>
+      <c r="L43">
+        <v>65</v>
+      </c>
+      <c r="M43">
+        <v>69</v>
+      </c>
+      <c r="N43">
+        <v>47</v>
+      </c>
+      <c r="O43">
+        <v>41</v>
+      </c>
+      <c r="P43">
+        <v>44</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+      <c r="S43">
+        <v>74</v>
+      </c>
+      <c r="T43">
+        <v>18</v>
+      </c>
+      <c r="U43">
+        <v>19</v>
+      </c>
+      <c r="V43">
+        <v>1</v>
+      </c>
+      <c r="AG43">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>2</v>
+      </c>
+      <c r="N44">
+        <v>2</v>
+      </c>
+      <c r="P44">
+        <v>8</v>
+      </c>
+      <c r="S44">
+        <v>2</v>
+      </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
+      <c r="U44">
+        <v>1</v>
+      </c>
+      <c r="AG44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>16</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>12</v>
+      </c>
+      <c r="M45">
+        <v>3</v>
+      </c>
+      <c r="N45">
+        <v>2</v>
+      </c>
+      <c r="O45">
+        <v>7</v>
+      </c>
+      <c r="P45">
+        <v>3</v>
+      </c>
+      <c r="S45">
+        <v>12</v>
+      </c>
+      <c r="T45">
+        <v>4</v>
+      </c>
+      <c r="AG45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>13</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>12</v>
+      </c>
+      <c r="G47">
+        <v>14</v>
+      </c>
+      <c r="H47">
+        <v>9</v>
+      </c>
+      <c r="I47">
+        <v>12</v>
+      </c>
+      <c r="L47">
+        <v>8</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>18</v>
+      </c>
+      <c r="O47">
+        <v>11</v>
+      </c>
+      <c r="P47">
+        <v>1</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+      <c r="S47">
+        <v>8</v>
+      </c>
+      <c r="U47">
+        <v>14</v>
+      </c>
+      <c r="V47">
+        <v>9</v>
+      </c>
+      <c r="W47">
+        <v>7</v>
+      </c>
+      <c r="X47">
+        <v>3</v>
+      </c>
+      <c r="AA47">
+        <v>3</v>
+      </c>
+      <c r="AB47">
+        <v>8</v>
+      </c>
+      <c r="AC47">
+        <v>9</v>
+      </c>
+      <c r="AD47">
+        <v>11</v>
+      </c>
+      <c r="AG47">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>21</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>22</v>
+      </c>
+      <c r="F48">
+        <v>23</v>
+      </c>
+      <c r="G48">
+        <v>18</v>
+      </c>
+      <c r="H48">
+        <v>28</v>
+      </c>
+      <c r="I48">
+        <v>14</v>
+      </c>
+      <c r="J48">
+        <v>8</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>46</v>
+      </c>
+      <c r="M48">
+        <v>24</v>
+      </c>
+      <c r="N48">
+        <v>24</v>
+      </c>
+      <c r="O48">
+        <v>16</v>
+      </c>
+      <c r="P48">
+        <v>29</v>
+      </c>
+      <c r="Q48">
+        <v>2</v>
+      </c>
+      <c r="S48">
+        <v>27</v>
+      </c>
+      <c r="T48">
+        <v>28</v>
+      </c>
+      <c r="U48">
+        <v>19</v>
+      </c>
+      <c r="V48">
+        <v>23</v>
+      </c>
+      <c r="W48">
+        <v>17</v>
+      </c>
+      <c r="AA48">
+        <v>4</v>
+      </c>
+      <c r="AB48">
+        <v>45</v>
+      </c>
+      <c r="AC48">
+        <v>17</v>
+      </c>
+      <c r="AD48">
+        <v>19</v>
+      </c>
+      <c r="AE48">
+        <v>5</v>
+      </c>
+      <c r="AG48">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>36</v>
+      </c>
+      <c r="C49">
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>31</v>
+      </c>
+      <c r="F49">
+        <v>33</v>
+      </c>
+      <c r="G49">
+        <v>26</v>
+      </c>
+      <c r="H49">
+        <v>20</v>
+      </c>
+      <c r="I49">
+        <v>22</v>
+      </c>
+      <c r="J49">
+        <v>21</v>
+      </c>
+      <c r="K49">
+        <v>3</v>
+      </c>
+      <c r="L49">
+        <v>30</v>
+      </c>
+      <c r="M49">
+        <v>28</v>
+      </c>
+      <c r="N49">
+        <v>33</v>
+      </c>
+      <c r="O49">
+        <v>25</v>
+      </c>
+      <c r="P49">
+        <v>21</v>
+      </c>
+      <c r="Q49">
+        <v>13</v>
+      </c>
+      <c r="R49">
+        <v>2</v>
+      </c>
+      <c r="S49">
+        <v>31</v>
+      </c>
+      <c r="T49">
+        <v>35</v>
+      </c>
+      <c r="U49">
+        <v>36</v>
+      </c>
+      <c r="V49">
+        <v>16</v>
+      </c>
+      <c r="W49">
+        <v>26</v>
+      </c>
+      <c r="X49">
+        <v>18</v>
+      </c>
+      <c r="Z49">
+        <v>1</v>
+      </c>
+      <c r="AA49">
+        <v>24</v>
+      </c>
+      <c r="AB49">
+        <v>38</v>
+      </c>
+      <c r="AC49">
+        <v>16</v>
+      </c>
+      <c r="AD49">
+        <v>26</v>
+      </c>
+      <c r="AE49">
+        <v>11</v>
+      </c>
+      <c r="AF49">
+        <v>1</v>
+      </c>
+      <c r="AG49">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>13</v>
+      </c>
+      <c r="E50">
+        <v>25</v>
+      </c>
+      <c r="F50">
+        <v>31</v>
+      </c>
+      <c r="G50">
+        <v>21</v>
+      </c>
+      <c r="H50">
+        <v>28</v>
+      </c>
+      <c r="I50">
+        <v>17</v>
+      </c>
+      <c r="J50">
+        <v>11</v>
+      </c>
+      <c r="L50">
+        <v>24</v>
+      </c>
+      <c r="M50">
+        <v>19</v>
+      </c>
+      <c r="N50">
+        <v>18</v>
+      </c>
+      <c r="O50">
+        <v>25</v>
+      </c>
+      <c r="P50">
+        <v>13</v>
+      </c>
+      <c r="Q50">
+        <v>8</v>
+      </c>
+      <c r="S50">
+        <v>20</v>
+      </c>
+      <c r="T50">
+        <v>24</v>
+      </c>
+      <c r="U50">
+        <v>22</v>
+      </c>
+      <c r="V50">
+        <v>22</v>
+      </c>
+      <c r="W50">
+        <v>15</v>
+      </c>
+      <c r="X50">
+        <v>7</v>
+      </c>
+      <c r="AA50">
+        <v>2</v>
+      </c>
+      <c r="AB50">
+        <v>23</v>
+      </c>
+      <c r="AC50">
+        <v>26</v>
+      </c>
+      <c r="AD50">
+        <v>20</v>
+      </c>
+      <c r="AE50">
+        <v>1</v>
+      </c>
+      <c r="AF50">
+        <v>2</v>
+      </c>
+      <c r="AG50">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>16</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>38</v>
+      </c>
+      <c r="F51">
+        <v>23</v>
+      </c>
+      <c r="G51">
+        <v>20</v>
+      </c>
+      <c r="H51">
+        <v>18</v>
+      </c>
+      <c r="I51">
+        <v>24</v>
+      </c>
+      <c r="J51">
+        <v>4</v>
+      </c>
+      <c r="K51">
+        <v>2</v>
+      </c>
+      <c r="L51">
+        <v>31</v>
+      </c>
+      <c r="M51">
+        <v>39</v>
+      </c>
+      <c r="N51">
+        <v>20</v>
+      </c>
+      <c r="O51">
+        <v>17</v>
+      </c>
+      <c r="P51">
+        <v>17</v>
+      </c>
+      <c r="Q51">
+        <v>3</v>
+      </c>
+      <c r="S51">
+        <v>20</v>
+      </c>
+      <c r="T51">
+        <v>11</v>
+      </c>
+      <c r="U51">
+        <v>20</v>
+      </c>
+      <c r="V51">
+        <v>34</v>
+      </c>
+      <c r="W51">
+        <v>14</v>
+      </c>
+      <c r="X51">
+        <v>4</v>
+      </c>
+      <c r="AB51">
+        <v>18</v>
+      </c>
+      <c r="AC51">
+        <v>53</v>
+      </c>
+      <c r="AD51">
+        <v>21</v>
+      </c>
+      <c r="AE51">
+        <v>4</v>
+      </c>
+      <c r="AF51">
+        <v>1</v>
+      </c>
+      <c r="AG51">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>35</v>
+      </c>
+      <c r="C52">
+        <v>30</v>
+      </c>
+      <c r="D52">
+        <v>18</v>
+      </c>
+      <c r="E52">
+        <v>47</v>
+      </c>
+      <c r="F52">
+        <v>47</v>
+      </c>
+      <c r="G52">
+        <v>51</v>
+      </c>
+      <c r="H52">
+        <v>45</v>
+      </c>
+      <c r="I52">
+        <v>37</v>
+      </c>
+      <c r="J52">
+        <v>37</v>
+      </c>
+      <c r="K52">
+        <v>13</v>
+      </c>
+      <c r="L52">
+        <v>45</v>
+      </c>
+      <c r="M52">
+        <v>37</v>
+      </c>
+      <c r="N52">
+        <v>41</v>
+      </c>
+      <c r="O52">
+        <v>46</v>
+      </c>
+      <c r="P52">
+        <v>46</v>
+      </c>
+      <c r="Q52">
+        <v>44</v>
+      </c>
+      <c r="R52">
+        <v>9</v>
+      </c>
+      <c r="S52">
+        <v>46</v>
+      </c>
+      <c r="T52">
+        <v>72</v>
+      </c>
+      <c r="U52">
+        <v>46</v>
+      </c>
+      <c r="V52">
+        <v>51</v>
+      </c>
+      <c r="W52">
+        <v>53</v>
+      </c>
+      <c r="X52">
+        <v>26</v>
+      </c>
+      <c r="Y52">
+        <v>4</v>
+      </c>
+      <c r="Z52">
+        <v>1</v>
+      </c>
+      <c r="AA52">
+        <v>38</v>
+      </c>
+      <c r="AB52">
+        <v>50</v>
+      </c>
+      <c r="AC52">
+        <v>50</v>
+      </c>
+      <c r="AD52">
+        <v>48</v>
+      </c>
+      <c r="AE52">
+        <v>39</v>
+      </c>
+      <c r="AF52">
+        <v>11</v>
+      </c>
+      <c r="AG52">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="E53">
+        <v>6</v>
+      </c>
+      <c r="F53">
+        <v>4</v>
+      </c>
+      <c r="G53">
+        <v>9</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
+      <c r="I53">
+        <v>13</v>
+      </c>
+      <c r="J53">
+        <v>4</v>
+      </c>
+      <c r="L53">
+        <v>5</v>
+      </c>
+      <c r="M53">
+        <v>7</v>
+      </c>
+      <c r="N53">
+        <v>6</v>
+      </c>
+      <c r="O53">
+        <v>4</v>
+      </c>
+      <c r="P53">
+        <v>14</v>
+      </c>
+      <c r="Q53">
+        <v>3</v>
+      </c>
+      <c r="R53">
+        <v>1</v>
+      </c>
+      <c r="S53">
+        <v>5</v>
+      </c>
+      <c r="T53">
+        <v>6</v>
+      </c>
+      <c r="U53">
+        <v>8</v>
+      </c>
+      <c r="V53">
+        <v>4</v>
+      </c>
+      <c r="W53">
+        <v>8</v>
+      </c>
+      <c r="X53">
+        <v>1</v>
+      </c>
+      <c r="Y53">
+        <v>1</v>
+      </c>
+      <c r="AA53">
+        <v>4</v>
+      </c>
+      <c r="AB53">
+        <v>13</v>
+      </c>
+      <c r="AC53">
+        <v>5</v>
+      </c>
+      <c r="AD53">
+        <v>8</v>
+      </c>
+      <c r="AE53">
+        <v>5</v>
+      </c>
+      <c r="AG53">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>21</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>21</v>
+      </c>
+      <c r="F54">
+        <v>13</v>
+      </c>
+      <c r="G54">
+        <v>10</v>
+      </c>
+      <c r="H54">
+        <v>16</v>
+      </c>
+      <c r="I54">
+        <v>27</v>
+      </c>
+      <c r="J54">
+        <v>4</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>20</v>
+      </c>
+      <c r="M54">
+        <v>17</v>
+      </c>
+      <c r="N54">
+        <v>7</v>
+      </c>
+      <c r="O54">
+        <v>17</v>
+      </c>
+      <c r="P54">
+        <v>9</v>
+      </c>
+      <c r="Q54">
+        <v>11</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <v>23</v>
+      </c>
+      <c r="T54">
+        <v>14</v>
+      </c>
+      <c r="U54">
+        <v>17</v>
+      </c>
+      <c r="V54">
+        <v>21</v>
+      </c>
+      <c r="W54">
+        <v>12</v>
+      </c>
+      <c r="AA54">
+        <v>4</v>
+      </c>
+      <c r="AB54">
+        <v>24</v>
+      </c>
+      <c r="AC54">
+        <v>10</v>
+      </c>
+      <c r="AD54">
+        <v>9</v>
+      </c>
+      <c r="AE54">
+        <v>4</v>
+      </c>
+      <c r="AG54">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>11</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+      <c r="I55">
+        <v>2</v>
+      </c>
+      <c r="J55">
+        <v>3</v>
+      </c>
+      <c r="L55">
+        <v>1</v>
+      </c>
+      <c r="M55">
+        <v>2</v>
+      </c>
+      <c r="N55">
+        <v>2</v>
+      </c>
+      <c r="P55">
+        <v>3</v>
+      </c>
+      <c r="Q55">
+        <v>3</v>
+      </c>
+      <c r="S55">
+        <v>6</v>
+      </c>
+      <c r="T55">
+        <v>2</v>
+      </c>
+      <c r="U55">
+        <v>4</v>
+      </c>
+      <c r="V55">
+        <v>6</v>
+      </c>
+      <c r="W55">
+        <v>3</v>
+      </c>
+      <c r="AA55">
+        <v>2</v>
+      </c>
+      <c r="AB55">
+        <v>3</v>
+      </c>
+      <c r="AC55">
+        <v>4</v>
+      </c>
+      <c r="AD55">
+        <v>5</v>
+      </c>
+      <c r="AG55">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>6</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>2</v>
+      </c>
+      <c r="M56">
+        <v>2</v>
+      </c>
+      <c r="N56">
+        <v>10</v>
+      </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
+      <c r="Q56">
+        <v>2</v>
+      </c>
+      <c r="S56">
+        <v>4</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+      <c r="U56">
+        <v>4</v>
+      </c>
+      <c r="V56">
+        <v>1</v>
+      </c>
+      <c r="AB56">
+        <v>8</v>
+      </c>
+      <c r="AC56">
+        <v>1</v>
+      </c>
+      <c r="AD56">
+        <v>1</v>
+      </c>
+      <c r="AG56">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>11</v>
+      </c>
+      <c r="F57">
+        <v>4</v>
+      </c>
+      <c r="G57">
+        <v>6</v>
+      </c>
+      <c r="H57">
+        <v>8</v>
+      </c>
+      <c r="I57">
+        <v>7</v>
+      </c>
+      <c r="J57">
+        <v>4</v>
+      </c>
+      <c r="L57">
+        <v>12</v>
+      </c>
+      <c r="M57">
+        <v>2</v>
+      </c>
+      <c r="N57">
+        <v>2</v>
+      </c>
+      <c r="O57">
+        <v>7</v>
+      </c>
+      <c r="P57">
+        <v>2</v>
+      </c>
+      <c r="Q57">
+        <v>2</v>
+      </c>
+      <c r="S57">
+        <v>8</v>
+      </c>
+      <c r="T57">
+        <v>7</v>
+      </c>
+      <c r="U57">
+        <v>7</v>
+      </c>
+      <c r="V57">
+        <v>7</v>
+      </c>
+      <c r="W57">
+        <v>13</v>
+      </c>
+      <c r="X57">
+        <v>1</v>
+      </c>
+      <c r="AB57">
+        <v>10</v>
+      </c>
+      <c r="AC57">
+        <v>8</v>
+      </c>
+      <c r="AD57">
+        <v>6</v>
+      </c>
+      <c r="AG57">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>